<commit_message>
chg: Added Range 14 freqs
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -573,7 +573,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="875">
   <si>
     <t>AWACS</t>
   </si>
@@ -3192,6 +3192,12 @@
   </si>
   <si>
     <t>ATRM FREQ ONEPAGER v1.0</t>
+  </si>
+  <si>
+    <t>YELLOW 3</t>
+  </si>
+  <si>
+    <t>YELLOW 5</t>
   </si>
 </sst>
 </file>
@@ -4144,7 +4150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="246">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4530,6 +4536,48 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4548,18 +4596,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4569,36 +4605,6 @@
     <xf numFmtId="0" fontId="14" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4705,6 +4711,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5359,8 +5368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AI70"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U60" sqref="U60:Y60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5409,16 +5418,16 @@
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="197" t="s">
+      <c r="R3" s="207" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="198"/>
-      <c r="T3" s="199"/>
-      <c r="V3" s="187" t="s">
+      <c r="S3" s="208"/>
+      <c r="T3" s="209"/>
+      <c r="V3" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="W3" s="188"/>
-      <c r="X3" s="189"/>
+      <c r="W3" s="202"/>
+      <c r="X3" s="203"/>
     </row>
     <row r="4" spans="2:32">
       <c r="B4" s="1" t="s">
@@ -5461,11 +5470,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="47"/>
-      <c r="R4" s="201" t="s">
+      <c r="R4" s="195" t="s">
         <v>707</v>
       </c>
-      <c r="S4" s="202"/>
-      <c r="T4" s="203"/>
+      <c r="S4" s="196"/>
+      <c r="T4" s="197"/>
       <c r="V4" s="9" t="s">
         <v>2</v>
       </c>
@@ -5475,16 +5484,16 @@
       <c r="X4" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="Z4" s="196" t="s">
+      <c r="Z4" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="196"/>
-      <c r="AB4" s="196"/>
-      <c r="AD4" s="196" t="s">
+      <c r="AA4" s="188"/>
+      <c r="AB4" s="188"/>
+      <c r="AD4" s="188" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="196"/>
-      <c r="AF4" s="196"/>
+      <c r="AE4" s="188"/>
+      <c r="AF4" s="188"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
@@ -5644,13 +5653,13 @@
       <c r="D7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="50" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="50" t="s">
         <v>63</v>
       </c>
       <c r="H7" s="50" t="s">
@@ -5959,11 +5968,11 @@
       <c r="X11" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="Z11" s="196" t="s">
+      <c r="Z11" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="196"/>
-      <c r="AB11" s="196"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="188"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
@@ -6342,11 +6351,11 @@
         <v>385</v>
       </c>
       <c r="Q17" s="5"/>
-      <c r="R17" s="193" t="s">
+      <c r="R17" s="198" t="s">
         <v>717</v>
       </c>
-      <c r="S17" s="194"/>
-      <c r="T17" s="195"/>
+      <c r="S17" s="199"/>
+      <c r="T17" s="200"/>
       <c r="V17" s="35" t="s">
         <v>759</v>
       </c>
@@ -6460,25 +6469,25 @@
         <v>314</v>
       </c>
       <c r="Q19" s="5"/>
-      <c r="R19" s="201" t="s">
+      <c r="R19" s="195" t="s">
         <v>708</v>
       </c>
-      <c r="S19" s="202"/>
-      <c r="T19" s="203"/>
-      <c r="V19" s="205" t="s">
+      <c r="S19" s="196"/>
+      <c r="T19" s="197"/>
+      <c r="V19" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="206"/>
-      <c r="X19" s="206"/>
-      <c r="Y19" s="206"/>
-      <c r="Z19" s="207"/>
-      <c r="AB19" s="196" t="s">
+      <c r="W19" s="190"/>
+      <c r="X19" s="190"/>
+      <c r="Y19" s="190"/>
+      <c r="Z19" s="191"/>
+      <c r="AB19" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="196"/>
-      <c r="AD19" s="196"/>
-      <c r="AE19" s="196"/>
-      <c r="AF19" s="196"/>
+      <c r="AC19" s="188"/>
+      <c r="AD19" s="188"/>
+      <c r="AE19" s="188"/>
+      <c r="AF19" s="188"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -7119,31 +7128,31 @@
       <c r="Z30" t="s">
         <v>754</v>
       </c>
-      <c r="AC30" s="196" t="s">
+      <c r="AC30" s="188" t="s">
         <v>592</v>
       </c>
-      <c r="AD30" s="196"/>
-      <c r="AE30" s="196"/>
+      <c r="AD30" s="188"/>
+      <c r="AE30" s="188"/>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="196" t="s">
+      <c r="B31" s="188" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="196"/>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="196"/>
-      <c r="J31" s="196" t="s">
+      <c r="C31" s="188"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="188"/>
+      <c r="F31" s="188"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="188"/>
+      <c r="J31" s="188" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="196"/>
-      <c r="L31" s="196"/>
-      <c r="M31" s="196"/>
-      <c r="N31" s="196"/>
-      <c r="O31" s="196"/>
-      <c r="P31" s="196"/>
+      <c r="K31" s="188"/>
+      <c r="L31" s="188"/>
+      <c r="M31" s="188"/>
+      <c r="N31" s="188"/>
+      <c r="O31" s="188"/>
+      <c r="P31" s="188"/>
       <c r="R31" s="97"/>
       <c r="S31" s="97"/>
       <c r="T31" s="97"/>
@@ -7203,15 +7212,15 @@
       <c r="R32" s="97"/>
       <c r="S32" s="97"/>
       <c r="T32" s="97"/>
-      <c r="U32" s="196" t="s">
+      <c r="U32" s="188" t="s">
         <v>688</v>
       </c>
-      <c r="V32" s="196"/>
-      <c r="W32" s="196"/>
-      <c r="X32" s="196"/>
-      <c r="Y32" s="196"/>
-      <c r="Z32" s="196"/>
-      <c r="AA32" s="196"/>
+      <c r="V32" s="188"/>
+      <c r="W32" s="188"/>
+      <c r="X32" s="188"/>
+      <c r="Y32" s="188"/>
+      <c r="Z32" s="188"/>
+      <c r="AA32" s="188"/>
       <c r="AC32" s="9"/>
       <c r="AD32" s="63" t="s">
         <v>113</v>
@@ -7320,9 +7329,9 @@
       <c r="P34" t="s">
         <v>407</v>
       </c>
-      <c r="R34" s="200"/>
-      <c r="S34" s="200"/>
-      <c r="T34" s="200"/>
+      <c r="R34" s="194"/>
+      <c r="S34" s="194"/>
+      <c r="T34" s="194"/>
       <c r="W34" t="s">
         <v>737</v>
       </c>
@@ -7593,15 +7602,15 @@
       <c r="H39" t="s">
         <v>393</v>
       </c>
-      <c r="J39" s="204" t="s">
+      <c r="J39" s="187" t="s">
         <v>404</v>
       </c>
-      <c r="K39" s="204"/>
-      <c r="L39" s="204"/>
-      <c r="M39" s="204"/>
-      <c r="N39" s="204"/>
-      <c r="O39" s="204"/>
-      <c r="P39" s="204"/>
+      <c r="K39" s="187"/>
+      <c r="L39" s="187"/>
+      <c r="M39" s="187"/>
+      <c r="N39" s="187"/>
+      <c r="O39" s="187"/>
+      <c r="P39" s="187"/>
       <c r="R39" s="97"/>
       <c r="S39" s="95"/>
       <c r="T39" s="97"/>
@@ -7674,13 +7683,13 @@
         <v>405</v>
       </c>
       <c r="Z41" s="18"/>
-      <c r="AC41" s="208" t="s">
+      <c r="AC41" s="192" t="s">
         <v>786</v>
       </c>
-      <c r="AD41" s="209"/>
-      <c r="AE41" s="209"/>
-      <c r="AF41" s="209"/>
-      <c r="AG41" s="209"/>
+      <c r="AD41" s="193"/>
+      <c r="AE41" s="193"/>
+      <c r="AF41" s="193"/>
+      <c r="AG41" s="193"/>
     </row>
     <row r="42" spans="2:33">
       <c r="E42" s="14" t="s">
@@ -7749,19 +7758,19 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="193" t="s">
+      <c r="Q45" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="R45" s="194"/>
-      <c r="S45" s="195"/>
+      <c r="R45" s="199"/>
+      <c r="S45" s="200"/>
       <c r="T45" s="39"/>
-      <c r="U45" s="196" t="s">
+      <c r="U45" s="188" t="s">
         <v>777</v>
       </c>
-      <c r="V45" s="196"/>
-      <c r="W45" s="196"/>
-      <c r="X45" s="196"/>
-      <c r="Y45" s="196"/>
+      <c r="V45" s="188"/>
+      <c r="W45" s="188"/>
+      <c r="X45" s="188"/>
+      <c r="Y45" s="188"/>
       <c r="AD45" s="65" t="s">
         <v>218</v>
       </c>
@@ -7776,7 +7785,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="190" t="s">
+      <c r="Q46" s="204" t="s">
         <v>707</v>
       </c>
       <c r="R46" s="99" t="s">
@@ -7814,7 +7823,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="191"/>
+      <c r="Q47" s="205"/>
       <c r="R47" s="9" t="s">
         <v>671</v>
       </c>
@@ -7838,7 +7847,7 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q48" s="192"/>
+      <c r="Q48" s="206"/>
       <c r="R48" s="85" t="s">
         <v>672</v>
       </c>
@@ -7863,7 +7872,7 @@
       </c>
     </row>
     <row r="49" spans="17:35">
-      <c r="Q49" s="190" t="s">
+      <c r="Q49" s="204" t="s">
         <v>708</v>
       </c>
       <c r="R49" s="99" t="s">
@@ -7889,7 +7898,7 @@
       </c>
     </row>
     <row r="50" spans="17:35">
-      <c r="Q50" s="191"/>
+      <c r="Q50" s="205"/>
       <c r="R50" s="9" t="s">
         <v>673</v>
       </c>
@@ -7913,7 +7922,7 @@
       </c>
     </row>
     <row r="51" spans="17:35" ht="15.75" thickBot="1">
-      <c r="Q51" s="192"/>
+      <c r="Q51" s="206"/>
       <c r="R51" s="85" t="s">
         <v>674</v>
       </c>
@@ -7935,15 +7944,15 @@
       <c r="Y51" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AC51" s="196" t="s">
+      <c r="AC51" s="188" t="s">
         <v>633</v>
       </c>
-      <c r="AD51" s="196"/>
-      <c r="AE51" s="196"/>
-      <c r="AF51" s="196"/>
-      <c r="AG51" s="196"/>
-      <c r="AH51" s="196"/>
-      <c r="AI51" s="196"/>
+      <c r="AD51" s="188"/>
+      <c r="AE51" s="188"/>
+      <c r="AF51" s="188"/>
+      <c r="AG51" s="188"/>
+      <c r="AH51" s="188"/>
+      <c r="AI51" s="188"/>
     </row>
     <row r="52" spans="17:35">
       <c r="U52" s="78">
@@ -8215,6 +8224,21 @@
       </c>
     </row>
     <row r="60" spans="17:35">
+      <c r="U60" s="246">
+        <v>14</v>
+      </c>
+      <c r="V60" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="W60" s="55" t="s">
+        <v>873</v>
+      </c>
+      <c r="X60" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>874</v>
+      </c>
       <c r="AC60" t="s">
         <v>663</v>
       </c>
@@ -8232,13 +8256,13 @@
       </c>
     </row>
     <row r="62" spans="17:35">
-      <c r="U62" s="196" t="s">
+      <c r="U62" s="188" t="s">
         <v>776</v>
       </c>
-      <c r="V62" s="196"/>
-      <c r="W62" s="196"/>
-      <c r="X62" s="196"/>
-      <c r="Y62" s="196"/>
+      <c r="V62" s="188"/>
+      <c r="W62" s="188"/>
+      <c r="X62" s="188"/>
+      <c r="Y62" s="188"/>
     </row>
     <row r="63" spans="17:35">
       <c r="U63" s="77" t="s">
@@ -8271,15 +8295,15 @@
         <v>783</v>
       </c>
       <c r="Y64" s="9"/>
-      <c r="AC64" s="196" t="s">
+      <c r="AC64" s="188" t="s">
         <v>686</v>
       </c>
-      <c r="AD64" s="196"/>
-      <c r="AE64" s="196"/>
-      <c r="AF64" s="196"/>
-      <c r="AG64" s="196"/>
-      <c r="AH64" s="196"/>
-      <c r="AI64" s="196"/>
+      <c r="AD64" s="188"/>
+      <c r="AE64" s="188"/>
+      <c r="AF64" s="188"/>
+      <c r="AG64" s="188"/>
+      <c r="AH64" s="188"/>
+      <c r="AI64" s="188"/>
     </row>
     <row r="65" spans="21:35">
       <c r="U65" s="78" t="s">
@@ -8426,6 +8450,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Q46:Q48"/>
+    <mergeCell ref="Q49:Q51"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="U62:Y62"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="J31:P31"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="AC64:AI64"/>
     <mergeCell ref="AC51:AI51"/>
@@ -8437,19 +8474,6 @@
     <mergeCell ref="AC30:AE30"/>
     <mergeCell ref="AC41:AG41"/>
     <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Q46:Q48"/>
-    <mergeCell ref="Q49:Q51"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="U62:Y62"/>
-    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9053,8 +9077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9588,6 +9612,15 @@
       <c r="C29" s="179" t="s">
         <v>93</v>
       </c>
+      <c r="D29" s="121" t="s">
+        <v>330</v>
+      </c>
+      <c r="E29" s="122" t="s">
+        <v>302</v>
+      </c>
+      <c r="F29" s="172" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="154">
@@ -9598,6 +9631,15 @@
       </c>
       <c r="C30" s="179" t="s">
         <v>79</v>
+      </c>
+      <c r="D30" s="154">
+        <v>14</v>
+      </c>
+      <c r="E30" s="148" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="148" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75">

</xml_diff>

<commit_message>
chg: Added Sas Al Nakheel Airport ATIS
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -573,7 +573,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="877">
   <si>
     <t>AWACS</t>
   </si>
@@ -3198,6 +3198,12 @@
   </si>
   <si>
     <t>YELLOW 5</t>
+  </si>
+  <si>
+    <t>128.4</t>
+  </si>
+  <si>
+    <t>RED ATC</t>
   </si>
 </sst>
 </file>
@@ -3568,7 +3574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -4146,11 +4152,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4450,21 +4493,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4473,9 +4505,6 @@
     <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4506,9 +4535,6 @@
     <xf numFmtId="0" fontId="26" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4536,12 +4562,63 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4557,54 +4634,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4713,8 +4742,38 @@
     <xf numFmtId="0" fontId="19" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5368,8 +5427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AI70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U60" sqref="U60:Y60"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5418,16 +5477,16 @@
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="207" t="s">
+      <c r="R3" s="191" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="208"/>
-      <c r="T3" s="209"/>
-      <c r="V3" s="201" t="s">
+      <c r="S3" s="192"/>
+      <c r="T3" s="193"/>
+      <c r="V3" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="W3" s="202"/>
-      <c r="X3" s="203"/>
+      <c r="W3" s="182"/>
+      <c r="X3" s="183"/>
     </row>
     <row r="4" spans="2:32">
       <c r="B4" s="1" t="s">
@@ -5484,16 +5543,16 @@
       <c r="X4" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="188"/>
-      <c r="AB4" s="188"/>
-      <c r="AD4" s="188" t="s">
+      <c r="AA4" s="190"/>
+      <c r="AB4" s="190"/>
+      <c r="AD4" s="190" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="188"/>
-      <c r="AF4" s="188"/>
+      <c r="AE4" s="190"/>
+      <c r="AF4" s="190"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
@@ -5968,11 +6027,11 @@
       <c r="X11" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="Z11" s="188" t="s">
+      <c r="Z11" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="188"/>
+      <c r="AA11" s="190"/>
+      <c r="AB11" s="190"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
@@ -6351,11 +6410,11 @@
         <v>385</v>
       </c>
       <c r="Q17" s="5"/>
-      <c r="R17" s="198" t="s">
+      <c r="R17" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="S17" s="199"/>
-      <c r="T17" s="200"/>
+      <c r="S17" s="188"/>
+      <c r="T17" s="189"/>
       <c r="V17" s="35" t="s">
         <v>759</v>
       </c>
@@ -6474,20 +6533,20 @@
       </c>
       <c r="S19" s="196"/>
       <c r="T19" s="197"/>
-      <c r="V19" s="189" t="s">
+      <c r="V19" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="190"/>
-      <c r="X19" s="190"/>
-      <c r="Y19" s="190"/>
-      <c r="Z19" s="191"/>
-      <c r="AB19" s="188" t="s">
+      <c r="W19" s="200"/>
+      <c r="X19" s="200"/>
+      <c r="Y19" s="200"/>
+      <c r="Z19" s="201"/>
+      <c r="AB19" s="190" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="188"/>
-      <c r="AD19" s="188"/>
-      <c r="AE19" s="188"/>
-      <c r="AF19" s="188"/>
+      <c r="AC19" s="190"/>
+      <c r="AD19" s="190"/>
+      <c r="AE19" s="190"/>
+      <c r="AF19" s="190"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -6732,7 +6791,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="23" spans="2:32">
+    <row r="23" spans="2:32" ht="15.75" thickBot="1">
       <c r="B23" s="1" t="s">
         <v>237</v>
       </c>
@@ -6775,6 +6834,15 @@
       <c r="O23" s="65"/>
       <c r="P23" s="5" t="s">
         <v>635</v>
+      </c>
+      <c r="R23" s="251" t="s">
+        <v>713</v>
+      </c>
+      <c r="S23" s="240" t="s">
+        <v>694</v>
+      </c>
+      <c r="T23" s="241" t="s">
+        <v>875</v>
       </c>
       <c r="V23" t="s">
         <v>741</v>
@@ -7128,31 +7196,31 @@
       <c r="Z30" t="s">
         <v>754</v>
       </c>
-      <c r="AC30" s="188" t="s">
+      <c r="AC30" s="190" t="s">
         <v>592</v>
       </c>
-      <c r="AD30" s="188"/>
-      <c r="AE30" s="188"/>
+      <c r="AD30" s="190"/>
+      <c r="AE30" s="190"/>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="188" t="s">
+      <c r="B31" s="190" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="188"/>
-      <c r="D31" s="188"/>
-      <c r="E31" s="188"/>
-      <c r="F31" s="188"/>
-      <c r="G31" s="188"/>
-      <c r="H31" s="188"/>
-      <c r="J31" s="188" t="s">
+      <c r="C31" s="190"/>
+      <c r="D31" s="190"/>
+      <c r="E31" s="190"/>
+      <c r="F31" s="190"/>
+      <c r="G31" s="190"/>
+      <c r="H31" s="190"/>
+      <c r="J31" s="190" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="188"/>
-      <c r="L31" s="188"/>
-      <c r="M31" s="188"/>
-      <c r="N31" s="188"/>
-      <c r="O31" s="188"/>
-      <c r="P31" s="188"/>
+      <c r="K31" s="190"/>
+      <c r="L31" s="190"/>
+      <c r="M31" s="190"/>
+      <c r="N31" s="190"/>
+      <c r="O31" s="190"/>
+      <c r="P31" s="190"/>
       <c r="R31" s="97"/>
       <c r="S31" s="97"/>
       <c r="T31" s="97"/>
@@ -7212,15 +7280,15 @@
       <c r="R32" s="97"/>
       <c r="S32" s="97"/>
       <c r="T32" s="97"/>
-      <c r="U32" s="188" t="s">
+      <c r="U32" s="190" t="s">
         <v>688</v>
       </c>
-      <c r="V32" s="188"/>
-      <c r="W32" s="188"/>
-      <c r="X32" s="188"/>
-      <c r="Y32" s="188"/>
-      <c r="Z32" s="188"/>
-      <c r="AA32" s="188"/>
+      <c r="V32" s="190"/>
+      <c r="W32" s="190"/>
+      <c r="X32" s="190"/>
+      <c r="Y32" s="190"/>
+      <c r="Z32" s="190"/>
+      <c r="AA32" s="190"/>
       <c r="AC32" s="9"/>
       <c r="AD32" s="63" t="s">
         <v>113</v>
@@ -7602,15 +7670,15 @@
       <c r="H39" t="s">
         <v>393</v>
       </c>
-      <c r="J39" s="187" t="s">
+      <c r="J39" s="198" t="s">
         <v>404</v>
       </c>
-      <c r="K39" s="187"/>
-      <c r="L39" s="187"/>
-      <c r="M39" s="187"/>
-      <c r="N39" s="187"/>
-      <c r="O39" s="187"/>
-      <c r="P39" s="187"/>
+      <c r="K39" s="198"/>
+      <c r="L39" s="198"/>
+      <c r="M39" s="198"/>
+      <c r="N39" s="198"/>
+      <c r="O39" s="198"/>
+      <c r="P39" s="198"/>
       <c r="R39" s="97"/>
       <c r="S39" s="95"/>
       <c r="T39" s="97"/>
@@ -7683,13 +7751,13 @@
         <v>405</v>
       </c>
       <c r="Z41" s="18"/>
-      <c r="AC41" s="192" t="s">
+      <c r="AC41" s="202" t="s">
         <v>786</v>
       </c>
-      <c r="AD41" s="193"/>
-      <c r="AE41" s="193"/>
-      <c r="AF41" s="193"/>
-      <c r="AG41" s="193"/>
+      <c r="AD41" s="203"/>
+      <c r="AE41" s="203"/>
+      <c r="AF41" s="203"/>
+      <c r="AG41" s="203"/>
     </row>
     <row r="42" spans="2:33">
       <c r="E42" s="14" t="s">
@@ -7758,19 +7826,19 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="198" t="s">
+      <c r="Q45" s="187" t="s">
         <v>657</v>
       </c>
-      <c r="R45" s="199"/>
-      <c r="S45" s="200"/>
+      <c r="R45" s="188"/>
+      <c r="S45" s="189"/>
       <c r="T45" s="39"/>
-      <c r="U45" s="188" t="s">
+      <c r="U45" s="190" t="s">
         <v>777</v>
       </c>
-      <c r="V45" s="188"/>
-      <c r="W45" s="188"/>
-      <c r="X45" s="188"/>
-      <c r="Y45" s="188"/>
+      <c r="V45" s="190"/>
+      <c r="W45" s="190"/>
+      <c r="X45" s="190"/>
+      <c r="Y45" s="190"/>
       <c r="AD45" s="65" t="s">
         <v>218</v>
       </c>
@@ -7785,7 +7853,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="204" t="s">
+      <c r="Q46" s="184" t="s">
         <v>707</v>
       </c>
       <c r="R46" s="99" t="s">
@@ -7823,7 +7891,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="205"/>
+      <c r="Q47" s="185"/>
       <c r="R47" s="9" t="s">
         <v>671</v>
       </c>
@@ -7847,7 +7915,7 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q48" s="206"/>
+      <c r="Q48" s="186"/>
       <c r="R48" s="85" t="s">
         <v>672</v>
       </c>
@@ -7872,7 +7940,7 @@
       </c>
     </row>
     <row r="49" spans="17:35">
-      <c r="Q49" s="204" t="s">
+      <c r="Q49" s="184" t="s">
         <v>708</v>
       </c>
       <c r="R49" s="99" t="s">
@@ -7898,7 +7966,7 @@
       </c>
     </row>
     <row r="50" spans="17:35">
-      <c r="Q50" s="205"/>
+      <c r="Q50" s="185"/>
       <c r="R50" s="9" t="s">
         <v>673</v>
       </c>
@@ -7922,7 +7990,7 @@
       </c>
     </row>
     <row r="51" spans="17:35" ht="15.75" thickBot="1">
-      <c r="Q51" s="206"/>
+      <c r="Q51" s="186"/>
       <c r="R51" s="85" t="s">
         <v>674</v>
       </c>
@@ -7944,15 +8012,15 @@
       <c r="Y51" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AC51" s="188" t="s">
+      <c r="AC51" s="190" t="s">
         <v>633</v>
       </c>
-      <c r="AD51" s="188"/>
-      <c r="AE51" s="188"/>
-      <c r="AF51" s="188"/>
-      <c r="AG51" s="188"/>
-      <c r="AH51" s="188"/>
-      <c r="AI51" s="188"/>
+      <c r="AD51" s="190"/>
+      <c r="AE51" s="190"/>
+      <c r="AF51" s="190"/>
+      <c r="AG51" s="190"/>
+      <c r="AH51" s="190"/>
+      <c r="AI51" s="190"/>
     </row>
     <row r="52" spans="17:35">
       <c r="U52" s="78">
@@ -8224,7 +8292,7 @@
       </c>
     </row>
     <row r="60" spans="17:35">
-      <c r="U60" s="246">
+      <c r="U60" s="180">
         <v>14</v>
       </c>
       <c r="V60" s="50" t="s">
@@ -8256,13 +8324,13 @@
       </c>
     </row>
     <row r="62" spans="17:35">
-      <c r="U62" s="188" t="s">
+      <c r="U62" s="190" t="s">
         <v>776</v>
       </c>
-      <c r="V62" s="188"/>
-      <c r="W62" s="188"/>
-      <c r="X62" s="188"/>
-      <c r="Y62" s="188"/>
+      <c r="V62" s="190"/>
+      <c r="W62" s="190"/>
+      <c r="X62" s="190"/>
+      <c r="Y62" s="190"/>
     </row>
     <row r="63" spans="17:35">
       <c r="U63" s="77" t="s">
@@ -8295,15 +8363,15 @@
         <v>783</v>
       </c>
       <c r="Y64" s="9"/>
-      <c r="AC64" s="188" t="s">
+      <c r="AC64" s="190" t="s">
         <v>686</v>
       </c>
-      <c r="AD64" s="188"/>
-      <c r="AE64" s="188"/>
-      <c r="AF64" s="188"/>
-      <c r="AG64" s="188"/>
-      <c r="AH64" s="188"/>
-      <c r="AI64" s="188"/>
+      <c r="AD64" s="190"/>
+      <c r="AE64" s="190"/>
+      <c r="AF64" s="190"/>
+      <c r="AG64" s="190"/>
+      <c r="AH64" s="190"/>
+      <c r="AI64" s="190"/>
     </row>
     <row r="65" spans="21:35">
       <c r="U65" s="78" t="s">
@@ -8450,19 +8518,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Q46:Q48"/>
-    <mergeCell ref="Q49:Q51"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="U62:Y62"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="AC64:AI64"/>
     <mergeCell ref="AC51:AI51"/>
@@ -8474,6 +8529,19 @@
     <mergeCell ref="AC30:AE30"/>
     <mergeCell ref="AC41:AG41"/>
     <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Q46:Q48"/>
+    <mergeCell ref="Q49:Q51"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="U62:Y62"/>
+    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8523,40 +8591,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="226" t="s">
         <v>788</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="232"/>
-      <c r="H1" s="232"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="233"/>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="227"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="222" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="229"/>
-      <c r="C3" s="230"/>
-      <c r="D3" s="231"/>
-      <c r="E3" s="228" t="s">
+      <c r="B3" s="223"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="222" t="s">
         <v>644</v>
       </c>
-      <c r="F3" s="229"/>
-      <c r="G3" s="230"/>
-      <c r="H3" s="231"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="225"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="115">
@@ -9077,8 +9145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9091,26 +9159,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="237" t="s">
         <v>872</v>
       </c>
-      <c r="B1" s="244"/>
-      <c r="C1" s="244"/>
-      <c r="D1" s="244"/>
-      <c r="E1" s="244"/>
-      <c r="F1" s="245"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="239"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" thickBot="1">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="231" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="239"/>
-      <c r="D2" s="240" t="s">
+      <c r="B2" s="232"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="234" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="241"/>
-      <c r="F2" s="242"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="236"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="123" t="s">
@@ -9121,7 +9189,7 @@
       <c r="D3" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="148" t="s">
+      <c r="E3" s="147" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="126" t="s">
@@ -9141,7 +9209,7 @@
       <c r="D4" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="175" t="s">
+      <c r="E4" s="168" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="126" t="s">
@@ -9161,7 +9229,7 @@
       <c r="D5" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="147" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="126" t="s">
@@ -9181,7 +9249,7 @@
       <c r="D6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="175" t="s">
+      <c r="E6" s="168" t="s">
         <v>80</v>
       </c>
       <c r="F6" s="126" t="s">
@@ -9201,7 +9269,7 @@
       <c r="D7" s="125" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="148" t="s">
+      <c r="E7" s="147" t="s">
         <v>108</v>
       </c>
       <c r="F7" s="126" t="s">
@@ -9221,7 +9289,7 @@
       <c r="D8" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="148" t="s">
+      <c r="E8" s="147" t="s">
         <v>343</v>
       </c>
       <c r="F8" s="126" t="s">
@@ -9241,7 +9309,7 @@
       <c r="D9" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="148" t="s">
+      <c r="E9" s="147" t="s">
         <v>139</v>
       </c>
       <c r="F9" s="126" t="s">
@@ -9261,7 +9329,7 @@
       <c r="D10" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="148" t="s">
+      <c r="E10" s="147" t="s">
         <v>270</v>
       </c>
       <c r="F10" s="126" t="s">
@@ -9281,7 +9349,7 @@
       <c r="D11" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="148" t="s">
+      <c r="E11" s="147" t="s">
         <v>275</v>
       </c>
       <c r="F11" s="126" t="s">
@@ -9301,7 +9369,7 @@
       <c r="D12" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="148" t="s">
+      <c r="E12" s="147" t="s">
         <v>238</v>
       </c>
       <c r="F12" s="126" t="s">
@@ -9321,7 +9389,7 @@
       <c r="D13" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="148" t="s">
+      <c r="E13" s="147" t="s">
         <v>219</v>
       </c>
       <c r="F13" s="126" t="s">
@@ -9341,7 +9409,7 @@
       <c r="D14" s="136" t="s">
         <v>482</v>
       </c>
-      <c r="E14" s="148" t="s">
+      <c r="E14" s="147" t="s">
         <v>151</v>
       </c>
       <c r="F14" s="126" t="s">
@@ -9387,7 +9455,7 @@
       <c r="B17" s="144" t="s">
         <v>717</v>
       </c>
-      <c r="C17" s="171" t="s">
+      <c r="C17" s="165" t="s">
         <v>420</v>
       </c>
       <c r="D17" s="137" t="s">
@@ -9399,163 +9467,167 @@
       <c r="F17" s="146"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A18" s="123" t="s">
-        <v>708</v>
-      </c>
-      <c r="B18" s="124"/>
-      <c r="C18" s="147"/>
-      <c r="D18" s="155" t="s">
+      <c r="A18" s="121" t="s">
+        <v>330</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" s="166" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="150" t="s">
         <v>657</v>
       </c>
-      <c r="E18" s="155"/>
-      <c r="F18" s="156"/>
+      <c r="E18" s="150"/>
+      <c r="F18" s="151"/>
     </row>
     <row r="19" spans="1:6" ht="15.75">
-      <c r="A19" s="173" t="s">
-        <v>709</v>
-      </c>
-      <c r="B19" s="148" t="s">
-        <v>692</v>
-      </c>
-      <c r="C19" s="149" t="s">
-        <v>712</v>
-      </c>
-      <c r="D19" s="176" t="s">
+      <c r="A19" s="149">
+        <v>1</v>
+      </c>
+      <c r="B19" s="147" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" s="172" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="169" t="s">
         <v>707</v>
       </c>
-      <c r="E19" s="157" t="s">
+      <c r="E19" s="152" t="s">
         <v>669</v>
       </c>
-      <c r="F19" s="184" t="s">
+      <c r="F19" s="177" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75">
-      <c r="A20" s="125" t="s">
-        <v>710</v>
-      </c>
-      <c r="B20" s="130" t="s">
-        <v>692</v>
-      </c>
-      <c r="C20" s="150" t="s">
-        <v>711</v>
-      </c>
-      <c r="D20" s="177"/>
+      <c r="A20" s="149">
+        <v>2</v>
+      </c>
+      <c r="B20" s="147" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" s="172" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="170"/>
       <c r="E20" s="130" t="s">
         <v>671</v>
       </c>
-      <c r="F20" s="185" t="s">
+      <c r="F20" s="178" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A21" s="151" t="s">
-        <v>713</v>
-      </c>
-      <c r="B21" s="152" t="s">
-        <v>692</v>
-      </c>
-      <c r="C21" s="153" t="s">
-        <v>714</v>
-      </c>
-      <c r="D21" s="178"/>
-      <c r="E21" s="174" t="s">
+      <c r="A21" s="149">
+        <v>3</v>
+      </c>
+      <c r="B21" s="147" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="172" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="171"/>
+      <c r="E21" s="167" t="s">
         <v>672</v>
       </c>
-      <c r="F21" s="186" t="s">
+      <c r="F21" s="179" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75">
-      <c r="A22" s="121" t="s">
-        <v>330</v>
-      </c>
-      <c r="B22" s="122" t="s">
-        <v>302</v>
+      <c r="A22" s="149">
+        <v>4</v>
+      </c>
+      <c r="B22" s="147" t="s">
+        <v>223</v>
       </c>
       <c r="C22" s="172" t="s">
-        <v>303</v>
-      </c>
-      <c r="D22" s="234" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="228" t="s">
         <v>708</v>
       </c>
-      <c r="E22" s="157" t="s">
+      <c r="E22" s="152" t="s">
         <v>670</v>
       </c>
-      <c r="F22" s="184" t="s">
+      <c r="F22" s="177" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75">
-      <c r="A23" s="154">
-        <v>1</v>
-      </c>
-      <c r="B23" s="148" t="s">
-        <v>265</v>
-      </c>
-      <c r="C23" s="179" t="s">
-        <v>169</v>
-      </c>
-      <c r="D23" s="235"/>
+      <c r="A23" s="149">
+        <v>5</v>
+      </c>
+      <c r="B23" s="147" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="172" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23" s="229"/>
       <c r="E23" s="130" t="s">
         <v>673</v>
       </c>
-      <c r="F23" s="179" t="s">
+      <c r="F23" s="172" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A24" s="154">
-        <v>2</v>
-      </c>
-      <c r="B24" s="148" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="179" t="s">
-        <v>204</v>
-      </c>
-      <c r="D24" s="236"/>
-      <c r="E24" s="174" t="s">
+      <c r="A24" s="149">
+        <v>6</v>
+      </c>
+      <c r="B24" s="147" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="172" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="230"/>
+      <c r="E24" s="167" t="s">
         <v>674</v>
       </c>
-      <c r="F24" s="186" t="s">
+      <c r="F24" s="179" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75">
-      <c r="A25" s="154">
-        <v>3</v>
-      </c>
-      <c r="B25" s="148" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="179" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="158" t="s">
+      <c r="A25" s="149">
+        <v>7</v>
+      </c>
+      <c r="B25" s="147" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="172" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="247" t="s">
         <v>775</v>
       </c>
-      <c r="E25" s="159" t="s">
+      <c r="E25" s="153" t="s">
         <v>302</v>
       </c>
-      <c r="F25" s="160" t="s">
+      <c r="F25" s="154" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75">
-      <c r="A26" s="154">
-        <v>4</v>
-      </c>
-      <c r="B26" s="148" t="s">
-        <v>223</v>
-      </c>
-      <c r="C26" s="179" t="s">
-        <v>266</v>
-      </c>
-      <c r="D26" s="154" t="s">
+      <c r="A26" s="149">
+        <v>8</v>
+      </c>
+      <c r="B26" s="147" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="172" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="248" t="s">
         <v>770</v>
       </c>
-      <c r="E26" s="148" t="s">
+      <c r="E26" s="147" t="s">
         <v>105</v>
       </c>
       <c r="F26" s="140" t="s">
@@ -9563,19 +9635,19 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75">
-      <c r="A27" s="154">
-        <v>5</v>
-      </c>
-      <c r="B27" s="148" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" s="179" t="s">
-        <v>269</v>
-      </c>
-      <c r="D27" s="154" t="s">
+      <c r="A27" s="149">
+        <v>9</v>
+      </c>
+      <c r="B27" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" s="172" t="s">
+        <v>779</v>
+      </c>
+      <c r="D27" s="248" t="s">
         <v>771</v>
       </c>
-      <c r="E27" s="148" t="s">
+      <c r="E27" s="147" t="s">
         <v>77</v>
       </c>
       <c r="F27" s="140" t="s">
@@ -9583,16 +9655,16 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A28" s="154">
-        <v>6</v>
-      </c>
-      <c r="B28" s="148" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="179" t="s">
-        <v>175</v>
-      </c>
-      <c r="D28" s="161" t="s">
+      <c r="A28" s="149">
+        <v>10</v>
+      </c>
+      <c r="B28" s="147" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="172" t="s">
+        <v>780</v>
+      </c>
+      <c r="D28" s="249" t="s">
         <v>772</v>
       </c>
       <c r="E28" s="145" t="s">
@@ -9602,305 +9674,310 @@
         <v>785</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75">
-      <c r="A29" s="154">
-        <v>7</v>
-      </c>
-      <c r="B29" s="148" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="179" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="121" t="s">
-        <v>330</v>
-      </c>
-      <c r="E29" s="122" t="s">
-        <v>302</v>
-      </c>
-      <c r="F29" s="172" t="s">
-        <v>303</v>
-      </c>
+    <row r="29" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A29" s="149">
+        <v>11</v>
+      </c>
+      <c r="B29" s="147" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="172" t="s">
+        <v>781</v>
+      </c>
+      <c r="D29" s="244" t="s">
+        <v>876</v>
+      </c>
+      <c r="E29" s="244"/>
+      <c r="F29" s="245"/>
     </row>
     <row r="30" spans="1:6" ht="15.75">
-      <c r="A30" s="154">
-        <v>8</v>
-      </c>
-      <c r="B30" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" s="179" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="154">
+      <c r="A30" s="149">
+        <v>12</v>
+      </c>
+      <c r="B30" s="147" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="172" t="s">
+        <v>782</v>
+      </c>
+      <c r="D30" s="250" t="s">
+        <v>709</v>
+      </c>
+      <c r="E30" s="242" t="s">
+        <v>692</v>
+      </c>
+      <c r="F30" s="243" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75">
+      <c r="A31" s="149">
+        <v>13</v>
+      </c>
+      <c r="B31" s="147" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="172" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="246" t="s">
+        <v>710</v>
+      </c>
+      <c r="E31" s="130" t="s">
+        <v>692</v>
+      </c>
+      <c r="F31" s="148" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="149">
         <v>14</v>
       </c>
-      <c r="E30" s="148" t="s">
+      <c r="B32" s="147" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="148" t="s">
+      <c r="C32" s="252" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75">
-      <c r="A31" s="154">
-        <v>9</v>
-      </c>
-      <c r="B31" s="148" t="s">
-        <v>232</v>
-      </c>
-      <c r="C31" s="179" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75">
-      <c r="A32" s="154">
-        <v>10</v>
-      </c>
-      <c r="B32" s="148" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="179" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75">
-      <c r="A33" s="154">
-        <v>11</v>
-      </c>
-      <c r="B33" s="148" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="179" t="s">
-        <v>781</v>
+      <c r="D32" s="246" t="s">
+        <v>713</v>
+      </c>
+      <c r="E32" s="130" t="s">
+        <v>692</v>
+      </c>
+      <c r="F32" s="148" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A33" s="149"/>
+      <c r="B33" s="147"/>
+      <c r="C33" s="172"/>
+      <c r="D33" s="251" t="s">
+        <v>713</v>
+      </c>
+      <c r="E33" s="240" t="s">
+        <v>694</v>
+      </c>
+      <c r="F33" s="241" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75">
-      <c r="A34" s="154">
-        <v>12</v>
-      </c>
-      <c r="B34" s="148" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="179" t="s">
-        <v>782</v>
-      </c>
+      <c r="A34" s="149"/>
+      <c r="B34" s="147"/>
+      <c r="C34" s="172"/>
     </row>
     <row r="35" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A35" s="161">
-        <v>13</v>
-      </c>
-      <c r="B35" s="145" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="180" t="s">
-        <v>103</v>
-      </c>
+      <c r="A35" s="155"/>
+      <c r="B35" s="145"/>
+      <c r="C35" s="173"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="240" t="s">
+      <c r="A36" s="234" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="241"/>
-      <c r="C36" s="241"/>
-      <c r="D36" s="241"/>
-      <c r="E36" s="242"/>
+      <c r="B36" s="235"/>
+      <c r="C36" s="235"/>
+      <c r="D36" s="235"/>
+      <c r="E36" s="236"/>
       <c r="F36" s="120"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="162" t="s">
+      <c r="A37" s="156" t="s">
         <v>842</v>
       </c>
-      <c r="B37" s="163" t="s">
+      <c r="B37" s="157" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="163" t="s">
+      <c r="C37" s="157" t="s">
         <v>320</v>
       </c>
-      <c r="D37" s="163" t="s">
+      <c r="D37" s="157" t="s">
         <v>755</v>
       </c>
-      <c r="E37" s="164" t="s">
+      <c r="E37" s="158" t="s">
         <v>316</v>
       </c>
       <c r="F37" s="120"/>
     </row>
     <row r="38" spans="1:6" ht="15.75">
-      <c r="A38" s="165" t="s">
+      <c r="A38" s="159" t="s">
         <v>739</v>
       </c>
-      <c r="B38" s="166" t="s">
+      <c r="B38" s="160" t="s">
         <v>430</v>
       </c>
-      <c r="C38" s="181" t="s">
+      <c r="C38" s="174" t="s">
         <v>793</v>
       </c>
-      <c r="D38" s="166" t="s">
+      <c r="D38" s="160" t="s">
         <v>757</v>
       </c>
-      <c r="E38" s="167" t="s">
+      <c r="E38" s="161" t="s">
         <v>868</v>
       </c>
       <c r="F38" s="120"/>
     </row>
     <row r="39" spans="1:6" ht="15.75">
-      <c r="A39" s="165" t="s">
+      <c r="A39" s="159" t="s">
         <v>740</v>
       </c>
-      <c r="B39" s="166" t="s">
+      <c r="B39" s="160" t="s">
         <v>490</v>
       </c>
-      <c r="C39" s="181" t="s">
+      <c r="C39" s="174" t="s">
         <v>794</v>
       </c>
-      <c r="D39" s="166" t="s">
+      <c r="D39" s="160" t="s">
         <v>757</v>
       </c>
-      <c r="E39" s="167" t="s">
+      <c r="E39" s="161" t="s">
         <v>866</v>
       </c>
       <c r="F39" s="120"/>
     </row>
     <row r="40" spans="1:6" ht="15.75">
-      <c r="A40" s="165" t="s">
+      <c r="A40" s="159" t="s">
         <v>741</v>
       </c>
-      <c r="B40" s="166" t="s">
+      <c r="B40" s="160" t="s">
         <v>431</v>
       </c>
-      <c r="C40" s="182" t="s">
+      <c r="C40" s="175" t="s">
         <v>580</v>
       </c>
-      <c r="D40" s="166" t="s">
+      <c r="D40" s="160" t="s">
         <v>756</v>
       </c>
-      <c r="E40" s="167" t="s">
+      <c r="E40" s="161" t="s">
         <v>749</v>
       </c>
       <c r="F40" s="120"/>
     </row>
     <row r="41" spans="1:6" ht="15.75">
-      <c r="A41" s="165" t="s">
+      <c r="A41" s="159" t="s">
         <v>742</v>
       </c>
-      <c r="B41" s="166" t="s">
+      <c r="B41" s="160" t="s">
         <v>431</v>
       </c>
-      <c r="C41" s="182" t="s">
+      <c r="C41" s="175" t="s">
         <v>835</v>
       </c>
-      <c r="D41" s="166" t="s">
+      <c r="D41" s="160" t="s">
         <v>756</v>
       </c>
-      <c r="E41" s="167" t="s">
+      <c r="E41" s="161" t="s">
         <v>750</v>
       </c>
       <c r="F41" s="120"/>
     </row>
     <row r="42" spans="1:6" ht="15.75">
-      <c r="A42" s="165" t="s">
+      <c r="A42" s="159" t="s">
         <v>743</v>
       </c>
-      <c r="B42" s="166" t="s">
+      <c r="B42" s="160" t="s">
         <v>431</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="175" t="s">
         <v>840</v>
       </c>
-      <c r="D42" s="166" t="s">
+      <c r="D42" s="160" t="s">
         <v>756</v>
       </c>
-      <c r="E42" s="167" t="s">
+      <c r="E42" s="161" t="s">
         <v>751</v>
       </c>
       <c r="F42" s="120"/>
     </row>
     <row r="43" spans="1:6" ht="15.75">
-      <c r="A43" s="165" t="s">
+      <c r="A43" s="159" t="s">
         <v>744</v>
       </c>
-      <c r="B43" s="166" t="s">
+      <c r="B43" s="160" t="s">
         <v>431</v>
       </c>
-      <c r="C43" s="182" t="s">
+      <c r="C43" s="175" t="s">
         <v>841</v>
       </c>
-      <c r="D43" s="166" t="s">
+      <c r="D43" s="160" t="s">
         <v>756</v>
       </c>
-      <c r="E43" s="167" t="s">
+      <c r="E43" s="161" t="s">
         <v>752</v>
       </c>
       <c r="F43" s="120"/>
     </row>
     <row r="44" spans="1:6" ht="15.75">
-      <c r="A44" s="165" t="s">
+      <c r="A44" s="159" t="s">
         <v>745</v>
       </c>
-      <c r="B44" s="166" t="s">
+      <c r="B44" s="160" t="s">
         <v>431</v>
       </c>
-      <c r="C44" s="182" t="s">
+      <c r="C44" s="175" t="s">
         <v>838</v>
       </c>
-      <c r="D44" s="166" t="s">
+      <c r="D44" s="160" t="s">
         <v>756</v>
       </c>
-      <c r="E44" s="167" t="s">
+      <c r="E44" s="161" t="s">
         <v>753</v>
       </c>
       <c r="F44" s="120"/>
     </row>
     <row r="45" spans="1:6" ht="15.75">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="159" t="s">
         <v>746</v>
       </c>
-      <c r="B45" s="166" t="s">
+      <c r="B45" s="160" t="s">
         <v>490</v>
       </c>
-      <c r="C45" s="182" t="s">
+      <c r="C45" s="175" t="s">
         <v>839</v>
       </c>
-      <c r="D45" s="166" t="s">
+      <c r="D45" s="160" t="s">
         <v>757</v>
       </c>
-      <c r="E45" s="167" t="s">
+      <c r="E45" s="161" t="s">
         <v>867</v>
       </c>
       <c r="F45" s="120"/>
     </row>
     <row r="46" spans="1:6" ht="15.75">
-      <c r="A46" s="165" t="s">
+      <c r="A46" s="159" t="s">
         <v>747</v>
       </c>
-      <c r="B46" s="166" t="s">
+      <c r="B46" s="160" t="s">
         <v>490</v>
       </c>
-      <c r="C46" s="182" t="s">
+      <c r="C46" s="175" t="s">
         <v>837</v>
       </c>
-      <c r="D46" s="166" t="s">
+      <c r="D46" s="160" t="s">
         <v>757</v>
       </c>
-      <c r="E46" s="167" t="s">
+      <c r="E46" s="161" t="s">
         <v>869</v>
       </c>
       <c r="F46" s="120"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A47" s="168" t="s">
+      <c r="A47" s="162" t="s">
         <v>748</v>
       </c>
-      <c r="B47" s="169" t="s">
+      <c r="B47" s="163" t="s">
         <v>431</v>
       </c>
-      <c r="C47" s="183" t="s">
+      <c r="C47" s="176" t="s">
         <v>836</v>
       </c>
-      <c r="D47" s="169" t="s">
+      <c r="D47" s="163" t="s">
         <v>758</v>
       </c>
-      <c r="E47" s="170" t="s">
+      <c r="E47" s="164" t="s">
         <v>754</v>
       </c>
       <c r="F47" s="120"/>
@@ -9914,12 +9991,13 @@
       <c r="F48" s="120"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A36:E36"/>
+    <mergeCell ref="D29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11122,28 +11200,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="207" t="s">
         <v>582</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="207"/>
     </row>
     <row r="2" spans="1:17" ht="15.75">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="204" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="211"/>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
-      <c r="H2" s="212"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="206"/>
     </row>
     <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="23"/>
@@ -11441,16 +11519,16 @@
       <c r="Q14" s="39"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="210" t="s">
+      <c r="A15" s="204" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="211"/>
-      <c r="C15" s="211"/>
-      <c r="D15" s="211"/>
-      <c r="E15" s="211"/>
-      <c r="F15" s="211"/>
-      <c r="G15" s="211"/>
-      <c r="H15" s="212"/>
+      <c r="B15" s="205"/>
+      <c r="C15" s="205"/>
+      <c r="D15" s="205"/>
+      <c r="E15" s="205"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="206"/>
       <c r="M15" s="39"/>
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
@@ -11810,16 +11888,16 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:17" ht="15.75">
-      <c r="A28" s="210" t="s">
+      <c r="A28" s="204" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="211"/>
-      <c r="C28" s="211"/>
-      <c r="D28" s="211"/>
-      <c r="E28" s="211"/>
-      <c r="F28" s="211"/>
-      <c r="G28" s="211"/>
-      <c r="H28" s="212"/>
+      <c r="B28" s="205"/>
+      <c r="C28" s="205"/>
+      <c r="D28" s="205"/>
+      <c r="E28" s="205"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
+      <c r="H28" s="206"/>
     </row>
     <row r="29" spans="1:17" ht="15.75">
       <c r="A29" s="23"/>
@@ -12133,12 +12211,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="207" t="s">
         <v>843</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="41"/>
@@ -12345,28 +12423,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="208" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="214"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="204" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="211"/>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
-      <c r="H2" s="212"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="206"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="29" t="s">
@@ -12653,12 +12731,12 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="210" t="s">
+      <c r="A15" s="204" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="211"/>
-      <c r="C15" s="211"/>
-      <c r="D15" s="212"/>
+      <c r="B15" s="205"/>
+      <c r="C15" s="205"/>
+      <c r="D15" s="206"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -12837,12 +12915,12 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="210" t="s">
+      <c r="A28" s="204" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="211"/>
-      <c r="C28" s="211"/>
-      <c r="D28" s="212"/>
+      <c r="B28" s="205"/>
+      <c r="C28" s="205"/>
+      <c r="D28" s="206"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -13040,36 +13118,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="209" t="s">
         <v>579</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
+      <c r="B1" s="209"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
       <c r="G1" s="59"/>
       <c r="H1" s="59"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="216"/>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
+      <c r="A2" s="210"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="211" t="s">
         <v>612</v>
       </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="219"/>
-      <c r="D3" s="217" t="s">
+      <c r="B3" s="212"/>
+      <c r="C3" s="213"/>
+      <c r="D3" s="211" t="s">
         <v>613</v>
       </c>
-      <c r="E3" s="218"/>
-      <c r="F3" s="219"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="213"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="53">
@@ -13614,22 +13692,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="221" t="s">
+      <c r="A1" s="215" t="s">
         <v>584</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="220" t="s">
+      <c r="B2" s="214" t="s">
         <v>605</v>
       </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
+      <c r="C2" s="214"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="41"/>
@@ -13734,12 +13812,12 @@
       <c r="E10" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="220" t="s">
+      <c r="B14" s="214" t="s">
         <v>600</v>
       </c>
-      <c r="C14" s="220"/>
-      <c r="D14" s="220"/>
-      <c r="E14" s="220"/>
+      <c r="C14" s="214"/>
+      <c r="D14" s="214"/>
+      <c r="E14" s="214"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="41"/>
@@ -13866,42 +13944,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="216" t="s">
         <v>871</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="224"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="218"/>
       <c r="I1" s="59"/>
       <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="225"/>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="227"/>
+      <c r="A2" s="219"/>
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
+      <c r="H2" s="221"/>
     </row>
     <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="222" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="229"/>
-      <c r="C3" s="230"/>
-      <c r="D3" s="231"/>
-      <c r="E3" s="228" t="s">
+      <c r="B3" s="223"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="222" t="s">
         <v>644</v>
       </c>
-      <c r="F3" s="229"/>
-      <c r="G3" s="230"/>
-      <c r="H3" s="231"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="225"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="119">

</xml_diff>

<commit_message>
chg: Updated freqs with recovery tankers
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -21,6 +21,7 @@
     <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -573,7 +574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="886">
   <si>
     <t>AWACS</t>
   </si>
@@ -3191,9 +3192,6 @@
     <t>F/A-18C presets Training mission (ATRM) V1.0</t>
   </si>
   <si>
-    <t>ATRM FREQ ONEPAGER v1.0</t>
-  </si>
-  <si>
     <t>YELLOW 3</t>
   </si>
   <si>
@@ -3204,6 +3202,36 @@
   </si>
   <si>
     <t>RED ATC</t>
+  </si>
+  <si>
+    <t>Recovery tanker Stennis</t>
+  </si>
+  <si>
+    <t>Recovery Tanker nimitz</t>
+  </si>
+  <si>
+    <t>142.5</t>
+  </si>
+  <si>
+    <t>143.5</t>
+  </si>
+  <si>
+    <t>48Y</t>
+  </si>
+  <si>
+    <t>49Y</t>
+  </si>
+  <si>
+    <t>Recovery tanker 48Y</t>
+  </si>
+  <si>
+    <t>Recovery tanker 49Y</t>
+  </si>
+  <si>
+    <t>ATRM FREQ ONEPAGER v1.1</t>
+  </si>
+  <si>
+    <t>Carriers</t>
   </si>
 </sst>
 </file>
@@ -3574,7 +3602,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -4189,11 +4217,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4502,15 +4593,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4535,17 +4618,7 @@
     <xf numFmtId="0" fontId="26" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4557,189 +4630,7 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4752,16 +4643,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4774,6 +4656,228 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5427,8 +5531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AI70"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q53" sqref="Q53:T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5477,16 +5581,16 @@
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="191" t="s">
+      <c r="R3" s="192" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="192"/>
-      <c r="T3" s="193"/>
-      <c r="V3" s="181" t="s">
+      <c r="S3" s="193"/>
+      <c r="T3" s="194"/>
+      <c r="V3" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="W3" s="182"/>
-      <c r="X3" s="183"/>
+      <c r="W3" s="183"/>
+      <c r="X3" s="184"/>
     </row>
     <row r="4" spans="2:32">
       <c r="B4" s="1" t="s">
@@ -5529,11 +5633,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="47"/>
-      <c r="R4" s="195" t="s">
+      <c r="R4" s="196" t="s">
         <v>707</v>
       </c>
-      <c r="S4" s="196"/>
-      <c r="T4" s="197"/>
+      <c r="S4" s="197"/>
+      <c r="T4" s="198"/>
       <c r="V4" s="9" t="s">
         <v>2</v>
       </c>
@@ -5543,16 +5647,16 @@
       <c r="X4" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="Z4" s="190" t="s">
+      <c r="Z4" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="190"/>
-      <c r="AB4" s="190"/>
-      <c r="AD4" s="190" t="s">
+      <c r="AA4" s="191"/>
+      <c r="AB4" s="191"/>
+      <c r="AD4" s="191" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="190"/>
-      <c r="AF4" s="190"/>
+      <c r="AE4" s="191"/>
+      <c r="AF4" s="191"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
@@ -6027,11 +6131,11 @@
       <c r="X11" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="Z11" s="190" t="s">
+      <c r="Z11" s="191" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="190"/>
-      <c r="AB11" s="190"/>
+      <c r="AA11" s="191"/>
+      <c r="AB11" s="191"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
@@ -6410,11 +6514,11 @@
         <v>385</v>
       </c>
       <c r="Q17" s="5"/>
-      <c r="R17" s="187" t="s">
+      <c r="R17" s="188" t="s">
         <v>717</v>
       </c>
-      <c r="S17" s="188"/>
-      <c r="T17" s="189"/>
+      <c r="S17" s="189"/>
+      <c r="T17" s="190"/>
       <c r="V17" s="35" t="s">
         <v>759</v>
       </c>
@@ -6528,25 +6632,25 @@
         <v>314</v>
       </c>
       <c r="Q19" s="5"/>
-      <c r="R19" s="195" t="s">
+      <c r="R19" s="196" t="s">
         <v>708</v>
       </c>
-      <c r="S19" s="196"/>
-      <c r="T19" s="197"/>
-      <c r="V19" s="199" t="s">
+      <c r="S19" s="197"/>
+      <c r="T19" s="198"/>
+      <c r="V19" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="200"/>
-      <c r="X19" s="200"/>
-      <c r="Y19" s="200"/>
-      <c r="Z19" s="201"/>
-      <c r="AB19" s="190" t="s">
+      <c r="W19" s="201"/>
+      <c r="X19" s="201"/>
+      <c r="Y19" s="201"/>
+      <c r="Z19" s="202"/>
+      <c r="AB19" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="190"/>
-      <c r="AD19" s="190"/>
-      <c r="AE19" s="190"/>
-      <c r="AF19" s="190"/>
+      <c r="AC19" s="191"/>
+      <c r="AD19" s="191"/>
+      <c r="AE19" s="191"/>
+      <c r="AF19" s="191"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -6835,14 +6939,14 @@
       <c r="P23" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="R23" s="251" t="s">
+      <c r="R23" s="178" t="s">
         <v>713</v>
       </c>
-      <c r="S23" s="240" t="s">
+      <c r="S23" s="170" t="s">
         <v>694</v>
       </c>
-      <c r="T23" s="241" t="s">
-        <v>875</v>
+      <c r="T23" s="171" t="s">
+        <v>874</v>
       </c>
       <c r="V23" t="s">
         <v>741</v>
@@ -7196,31 +7300,31 @@
       <c r="Z30" t="s">
         <v>754</v>
       </c>
-      <c r="AC30" s="190" t="s">
+      <c r="AC30" s="191" t="s">
         <v>592</v>
       </c>
-      <c r="AD30" s="190"/>
-      <c r="AE30" s="190"/>
+      <c r="AD30" s="191"/>
+      <c r="AE30" s="191"/>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="190" t="s">
+      <c r="B31" s="191" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="190"/>
-      <c r="D31" s="190"/>
-      <c r="E31" s="190"/>
-      <c r="F31" s="190"/>
-      <c r="G31" s="190"/>
-      <c r="H31" s="190"/>
-      <c r="J31" s="190" t="s">
+      <c r="C31" s="191"/>
+      <c r="D31" s="191"/>
+      <c r="E31" s="191"/>
+      <c r="F31" s="191"/>
+      <c r="G31" s="191"/>
+      <c r="H31" s="191"/>
+      <c r="J31" s="191" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="190"/>
-      <c r="L31" s="190"/>
-      <c r="M31" s="190"/>
-      <c r="N31" s="190"/>
-      <c r="O31" s="190"/>
-      <c r="P31" s="190"/>
+      <c r="K31" s="191"/>
+      <c r="L31" s="191"/>
+      <c r="M31" s="191"/>
+      <c r="N31" s="191"/>
+      <c r="O31" s="191"/>
+      <c r="P31" s="191"/>
       <c r="R31" s="97"/>
       <c r="S31" s="97"/>
       <c r="T31" s="97"/>
@@ -7280,15 +7384,15 @@
       <c r="R32" s="97"/>
       <c r="S32" s="97"/>
       <c r="T32" s="97"/>
-      <c r="U32" s="190" t="s">
+      <c r="U32" s="191" t="s">
         <v>688</v>
       </c>
-      <c r="V32" s="190"/>
-      <c r="W32" s="190"/>
-      <c r="X32" s="190"/>
-      <c r="Y32" s="190"/>
-      <c r="Z32" s="190"/>
-      <c r="AA32" s="190"/>
+      <c r="V32" s="191"/>
+      <c r="W32" s="191"/>
+      <c r="X32" s="191"/>
+      <c r="Y32" s="191"/>
+      <c r="Z32" s="191"/>
+      <c r="AA32" s="191"/>
       <c r="AC32" s="9"/>
       <c r="AD32" s="63" t="s">
         <v>113</v>
@@ -7397,9 +7501,9 @@
       <c r="P34" t="s">
         <v>407</v>
       </c>
-      <c r="R34" s="194"/>
-      <c r="S34" s="194"/>
-      <c r="T34" s="194"/>
+      <c r="R34" s="195"/>
+      <c r="S34" s="195"/>
+      <c r="T34" s="195"/>
       <c r="W34" t="s">
         <v>737</v>
       </c>
@@ -7670,15 +7774,15 @@
       <c r="H39" t="s">
         <v>393</v>
       </c>
-      <c r="J39" s="198" t="s">
+      <c r="J39" s="199" t="s">
         <v>404</v>
       </c>
-      <c r="K39" s="198"/>
-      <c r="L39" s="198"/>
-      <c r="M39" s="198"/>
-      <c r="N39" s="198"/>
-      <c r="O39" s="198"/>
-      <c r="P39" s="198"/>
+      <c r="K39" s="199"/>
+      <c r="L39" s="199"/>
+      <c r="M39" s="199"/>
+      <c r="N39" s="199"/>
+      <c r="O39" s="199"/>
+      <c r="P39" s="199"/>
       <c r="R39" s="97"/>
       <c r="S39" s="95"/>
       <c r="T39" s="97"/>
@@ -7751,13 +7855,13 @@
         <v>405</v>
       </c>
       <c r="Z41" s="18"/>
-      <c r="AC41" s="202" t="s">
+      <c r="AC41" s="203" t="s">
         <v>786</v>
       </c>
-      <c r="AD41" s="203"/>
-      <c r="AE41" s="203"/>
-      <c r="AF41" s="203"/>
-      <c r="AG41" s="203"/>
+      <c r="AD41" s="204"/>
+      <c r="AE41" s="204"/>
+      <c r="AF41" s="204"/>
+      <c r="AG41" s="204"/>
     </row>
     <row r="42" spans="2:33">
       <c r="E42" s="14" t="s">
@@ -7826,19 +7930,19 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="187" t="s">
+      <c r="Q45" s="188" t="s">
         <v>657</v>
       </c>
-      <c r="R45" s="188"/>
-      <c r="S45" s="189"/>
+      <c r="R45" s="189"/>
+      <c r="S45" s="190"/>
       <c r="T45" s="39"/>
-      <c r="U45" s="190" t="s">
+      <c r="U45" s="191" t="s">
         <v>777</v>
       </c>
-      <c r="V45" s="190"/>
-      <c r="W45" s="190"/>
-      <c r="X45" s="190"/>
-      <c r="Y45" s="190"/>
+      <c r="V45" s="191"/>
+      <c r="W45" s="191"/>
+      <c r="X45" s="191"/>
+      <c r="Y45" s="191"/>
       <c r="AD45" s="65" t="s">
         <v>218</v>
       </c>
@@ -7853,7 +7957,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="184" t="s">
+      <c r="Q46" s="185" t="s">
         <v>707</v>
       </c>
       <c r="R46" s="99" t="s">
@@ -7891,7 +7995,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="185"/>
+      <c r="Q47" s="186"/>
       <c r="R47" s="9" t="s">
         <v>671</v>
       </c>
@@ -7915,7 +8019,7 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q48" s="186"/>
+      <c r="Q48" s="187"/>
       <c r="R48" s="85" t="s">
         <v>672</v>
       </c>
@@ -7940,7 +8044,7 @@
       </c>
     </row>
     <row r="49" spans="17:35">
-      <c r="Q49" s="184" t="s">
+      <c r="Q49" s="185" t="s">
         <v>708</v>
       </c>
       <c r="R49" s="99" t="s">
@@ -7966,7 +8070,7 @@
       </c>
     </row>
     <row r="50" spans="17:35">
-      <c r="Q50" s="185"/>
+      <c r="Q50" s="186"/>
       <c r="R50" s="9" t="s">
         <v>673</v>
       </c>
@@ -7990,7 +8094,7 @@
       </c>
     </row>
     <row r="51" spans="17:35" ht="15.75" thickBot="1">
-      <c r="Q51" s="186"/>
+      <c r="Q51" s="187"/>
       <c r="R51" s="85" t="s">
         <v>674</v>
       </c>
@@ -8012,15 +8116,15 @@
       <c r="Y51" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AC51" s="190" t="s">
+      <c r="AC51" s="191" t="s">
         <v>633</v>
       </c>
-      <c r="AD51" s="190"/>
-      <c r="AE51" s="190"/>
-      <c r="AF51" s="190"/>
-      <c r="AG51" s="190"/>
-      <c r="AH51" s="190"/>
-      <c r="AI51" s="190"/>
+      <c r="AD51" s="191"/>
+      <c r="AE51" s="191"/>
+      <c r="AF51" s="191"/>
+      <c r="AG51" s="191"/>
+      <c r="AH51" s="191"/>
+      <c r="AI51" s="191"/>
     </row>
     <row r="52" spans="17:35">
       <c r="U52" s="78">
@@ -8061,9 +8165,16 @@
       </c>
     </row>
     <row r="53" spans="17:35">
+      <c r="Q53" t="s">
+        <v>876</v>
+      </c>
       <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="52"/>
+      <c r="S53" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="T53" s="52" t="s">
+        <v>880</v>
+      </c>
       <c r="U53" s="78">
         <v>7</v>
       </c>
@@ -8096,9 +8207,16 @@
       </c>
     </row>
     <row r="54" spans="17:35">
+      <c r="Q54" t="s">
+        <v>877</v>
+      </c>
       <c r="R54" s="52"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="52"/>
+      <c r="S54" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="T54" s="52" t="s">
+        <v>881</v>
+      </c>
       <c r="U54" s="78">
         <v>8</v>
       </c>
@@ -8292,20 +8410,20 @@
       </c>
     </row>
     <row r="60" spans="17:35">
-      <c r="U60" s="180">
+      <c r="U60" s="169">
         <v>14</v>
       </c>
       <c r="V60" s="50" t="s">
         <v>61</v>
       </c>
       <c r="W60" s="55" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="X60" s="50" t="s">
         <v>63</v>
       </c>
       <c r="Y60" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="AC60" t="s">
         <v>663</v>
@@ -8324,13 +8442,13 @@
       </c>
     </row>
     <row r="62" spans="17:35">
-      <c r="U62" s="190" t="s">
+      <c r="U62" s="191" t="s">
         <v>776</v>
       </c>
-      <c r="V62" s="190"/>
-      <c r="W62" s="190"/>
-      <c r="X62" s="190"/>
-      <c r="Y62" s="190"/>
+      <c r="V62" s="191"/>
+      <c r="W62" s="191"/>
+      <c r="X62" s="191"/>
+      <c r="Y62" s="191"/>
     </row>
     <row r="63" spans="17:35">
       <c r="U63" s="77" t="s">
@@ -8363,15 +8481,15 @@
         <v>783</v>
       </c>
       <c r="Y64" s="9"/>
-      <c r="AC64" s="190" t="s">
+      <c r="AC64" s="191" t="s">
         <v>686</v>
       </c>
-      <c r="AD64" s="190"/>
-      <c r="AE64" s="190"/>
-      <c r="AF64" s="190"/>
-      <c r="AG64" s="190"/>
-      <c r="AH64" s="190"/>
-      <c r="AI64" s="190"/>
+      <c r="AD64" s="191"/>
+      <c r="AE64" s="191"/>
+      <c r="AF64" s="191"/>
+      <c r="AG64" s="191"/>
+      <c r="AH64" s="191"/>
+      <c r="AI64" s="191"/>
     </row>
     <row r="65" spans="21:35">
       <c r="U65" s="78" t="s">
@@ -8591,40 +8709,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="227" t="s">
         <v>788</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="227"/>
-      <c r="B2" s="227"/>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
-      <c r="H2" s="227"/>
+      <c r="A2" s="228"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="222" t="s">
+      <c r="A3" s="223" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="223"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="225"/>
-      <c r="E3" s="222" t="s">
+      <c r="B3" s="224"/>
+      <c r="C3" s="225"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="223" t="s">
         <v>644</v>
       </c>
-      <c r="F3" s="223"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="225"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="226"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="115">
@@ -9143,10 +9261,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9159,26 +9277,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A1" s="237" t="s">
-        <v>872</v>
-      </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="239"/>
+      <c r="A1" s="235" t="s">
+        <v>884</v>
+      </c>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="237"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" thickBot="1">
-      <c r="A2" s="231" t="s">
+      <c r="A2" s="229" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="234" t="s">
+      <c r="B2" s="230"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="232" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="235"/>
-      <c r="F2" s="236"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="234"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="123" t="s">
@@ -9209,7 +9327,7 @@
       <c r="D4" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="168" t="s">
+      <c r="E4" s="163" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="126" t="s">
@@ -9249,7 +9367,7 @@
       <c r="D6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="168" t="s">
+      <c r="E6" s="163" t="s">
         <v>80</v>
       </c>
       <c r="F6" s="126" t="s">
@@ -9448,14 +9566,14 @@
       </c>
       <c r="F16" s="140"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="143" t="s">
         <v>787</v>
       </c>
       <c r="B17" s="144" t="s">
         <v>717</v>
       </c>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="161" t="s">
         <v>420</v>
       </c>
       <c r="D17" s="137" t="s">
@@ -9466,518 +9584,542 @@
       </c>
       <c r="F17" s="146"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1">
       <c r="A18" s="121" t="s">
         <v>330</v>
       </c>
       <c r="B18" s="122" t="s">
         <v>302</v>
       </c>
-      <c r="C18" s="166" t="s">
+      <c r="C18" s="162" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="150" t="s">
-        <v>657</v>
-      </c>
-      <c r="E18" s="150"/>
-      <c r="F18" s="151"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75">
+      <c r="D18" s="252" t="s">
+        <v>885</v>
+      </c>
+      <c r="E18" s="238"/>
+      <c r="F18" s="239"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75">
       <c r="A19" s="149">
         <v>1</v>
       </c>
       <c r="B19" s="147" t="s">
         <v>265</v>
       </c>
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="240" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="169" t="s">
+      <c r="D19" s="253" t="s">
         <v>707</v>
       </c>
-      <c r="E19" s="152" t="s">
+      <c r="E19" s="150" t="s">
         <v>669</v>
       </c>
-      <c r="F19" s="177" t="s">
+      <c r="F19" s="246" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75">
+    <row r="20" spans="1:18" ht="15.75">
       <c r="A20" s="149">
         <v>2</v>
       </c>
       <c r="B20" s="147" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="240" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="170"/>
+      <c r="D20" s="254"/>
       <c r="E20" s="130" t="s">
         <v>671</v>
       </c>
-      <c r="F20" s="178" t="s">
+      <c r="F20" s="247" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" thickBot="1">
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="52"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75">
       <c r="A21" s="149">
         <v>3</v>
       </c>
       <c r="B21" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="240" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="171"/>
-      <c r="E21" s="167" t="s">
+      <c r="D21" s="255"/>
+      <c r="E21" s="244" t="s">
         <v>672</v>
       </c>
-      <c r="F21" s="179" t="s">
+      <c r="F21" s="247" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75">
+      <c r="P21" s="52"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="52"/>
+    </row>
+    <row r="22" spans="1:18" ht="16.5" thickBot="1">
       <c r="A22" s="149">
         <v>4</v>
       </c>
       <c r="B22" s="147" t="s">
         <v>223</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="240" t="s">
         <v>266</v>
       </c>
-      <c r="D22" s="228" t="s">
-        <v>708</v>
-      </c>
-      <c r="E22" s="152" t="s">
-        <v>670</v>
-      </c>
-      <c r="F22" s="177" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75">
+      <c r="D22" s="248" t="s">
+        <v>882</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>431</v>
+      </c>
+      <c r="F22" s="250" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75">
       <c r="A23" s="149">
         <v>5</v>
       </c>
       <c r="B23" s="147" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="240" t="s">
         <v>269</v>
       </c>
-      <c r="D23" s="229"/>
-      <c r="E23" s="130" t="s">
-        <v>673</v>
-      </c>
-      <c r="F23" s="172" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" thickBot="1">
+      <c r="D23" s="253" t="s">
+        <v>708</v>
+      </c>
+      <c r="E23" s="150" t="s">
+        <v>670</v>
+      </c>
+      <c r="F23" s="246" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75">
       <c r="A24" s="149">
         <v>6</v>
       </c>
       <c r="B24" s="147" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="240" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="230"/>
-      <c r="E24" s="167" t="s">
-        <v>674</v>
-      </c>
-      <c r="F24" s="179" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75">
+      <c r="D24" s="254"/>
+      <c r="E24" s="130" t="s">
+        <v>673</v>
+      </c>
+      <c r="F24" s="251" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75">
       <c r="A25" s="149">
         <v>7</v>
       </c>
       <c r="B25" s="147" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="172" t="s">
+      <c r="C25" s="240" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="247" t="s">
-        <v>775</v>
-      </c>
-      <c r="E25" s="153" t="s">
-        <v>302</v>
-      </c>
-      <c r="F25" s="154" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75">
+      <c r="D25" s="255"/>
+      <c r="E25" s="244" t="s">
+        <v>674</v>
+      </c>
+      <c r="F25" s="247" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="16.5" thickBot="1">
       <c r="A26" s="149">
         <v>8</v>
       </c>
       <c r="B26" s="147" t="s">
         <v>224</v>
       </c>
-      <c r="C26" s="172" t="s">
+      <c r="C26" s="240" t="s">
         <v>79</v>
       </c>
       <c r="D26" s="248" t="s">
-        <v>770</v>
-      </c>
-      <c r="E26" s="147" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="140" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75">
+        <v>883</v>
+      </c>
+      <c r="E26" s="145" t="s">
+        <v>431</v>
+      </c>
+      <c r="F26" s="245" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75">
       <c r="A27" s="149">
         <v>9</v>
       </c>
       <c r="B27" s="147" t="s">
         <v>232</v>
       </c>
-      <c r="C27" s="172" t="s">
+      <c r="C27" s="164" t="s">
         <v>779</v>
       </c>
-      <c r="D27" s="248" t="s">
-        <v>771</v>
-      </c>
-      <c r="E27" s="147" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="140" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" thickBot="1">
+      <c r="D27" s="241" t="s">
+        <v>775</v>
+      </c>
+      <c r="E27" s="242" t="s">
+        <v>302</v>
+      </c>
+      <c r="F27" s="243" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75">
       <c r="A28" s="149">
         <v>10</v>
       </c>
       <c r="B28" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="172" t="s">
+      <c r="C28" s="164" t="s">
         <v>780</v>
       </c>
-      <c r="D28" s="249" t="s">
-        <v>772</v>
-      </c>
-      <c r="E28" s="145" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="146" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" thickBot="1">
+      <c r="D28" s="175" t="s">
+        <v>770</v>
+      </c>
+      <c r="E28" s="147" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="148" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="149">
         <v>11</v>
       </c>
       <c r="B29" s="147" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="172" t="s">
+      <c r="C29" s="164" t="s">
         <v>781</v>
       </c>
-      <c r="D29" s="244" t="s">
-        <v>876</v>
-      </c>
-      <c r="E29" s="244"/>
-      <c r="F29" s="245"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75">
+      <c r="D29" s="175" t="s">
+        <v>771</v>
+      </c>
+      <c r="E29" s="147" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="148" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="16.5" thickBot="1">
       <c r="A30" s="149">
         <v>12</v>
       </c>
       <c r="B30" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="172" t="s">
+      <c r="C30" s="164" t="s">
         <v>782</v>
       </c>
-      <c r="D30" s="250" t="s">
-        <v>709</v>
-      </c>
-      <c r="E30" s="242" t="s">
-        <v>692</v>
-      </c>
-      <c r="F30" s="243" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75">
+      <c r="D30" s="176" t="s">
+        <v>772</v>
+      </c>
+      <c r="E30" s="145" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="245" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="16.5" thickBot="1">
       <c r="A31" s="149">
         <v>13</v>
       </c>
       <c r="B31" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="164" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="246" t="s">
-        <v>710</v>
-      </c>
-      <c r="E31" s="130" t="s">
-        <v>692</v>
-      </c>
-      <c r="F31" s="148" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="D31" s="180" t="s">
+        <v>875</v>
+      </c>
+      <c r="E31" s="180"/>
+      <c r="F31" s="181"/>
+    </row>
+    <row r="32" spans="1:18" ht="15.75">
       <c r="A32" s="149">
         <v>14</v>
       </c>
       <c r="B32" s="147" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="252" t="s">
+      <c r="C32" s="179" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="246" t="s">
-        <v>713</v>
-      </c>
-      <c r="E32" s="130" t="s">
+      <c r="D32" s="177" t="s">
+        <v>709</v>
+      </c>
+      <c r="E32" s="172" t="s">
         <v>692</v>
       </c>
-      <c r="F32" s="148" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="16.5" thickBot="1">
+      <c r="F32" s="173" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="149"/>
       <c r="B33" s="147"/>
-      <c r="C33" s="172"/>
-      <c r="D33" s="251" t="s">
-        <v>713</v>
-      </c>
-      <c r="E33" s="240" t="s">
-        <v>694</v>
-      </c>
-      <c r="F33" s="241" t="s">
-        <v>875</v>
+      <c r="C33" s="164"/>
+      <c r="D33" s="174" t="s">
+        <v>710</v>
+      </c>
+      <c r="E33" s="130" t="s">
+        <v>692</v>
+      </c>
+      <c r="F33" s="148" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="149"/>
       <c r="B34" s="147"/>
-      <c r="C34" s="172"/>
+      <c r="C34" s="164"/>
+      <c r="D34" s="174" t="s">
+        <v>713</v>
+      </c>
+      <c r="E34" s="130" t="s">
+        <v>692</v>
+      </c>
+      <c r="F34" s="148" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A35" s="155"/>
+      <c r="A35" s="151"/>
       <c r="B35" s="145"/>
-      <c r="C35" s="173"/>
+      <c r="C35" s="165"/>
+      <c r="D35" s="178" t="s">
+        <v>713</v>
+      </c>
+      <c r="E35" s="170" t="s">
+        <v>694</v>
+      </c>
+      <c r="F35" s="171" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="234" t="s">
+      <c r="A36" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="235"/>
-      <c r="C36" s="235"/>
-      <c r="D36" s="235"/>
-      <c r="E36" s="236"/>
+      <c r="B36" s="233"/>
+      <c r="C36" s="233"/>
+      <c r="D36" s="233"/>
+      <c r="E36" s="234"/>
       <c r="F36" s="120"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="152" t="s">
         <v>842</v>
       </c>
-      <c r="B37" s="157" t="s">
+      <c r="B37" s="153" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="157" t="s">
+      <c r="C37" s="153" t="s">
         <v>320</v>
       </c>
-      <c r="D37" s="157" t="s">
+      <c r="D37" s="153" t="s">
         <v>755</v>
       </c>
-      <c r="E37" s="158" t="s">
+      <c r="E37" s="154" t="s">
         <v>316</v>
       </c>
       <c r="F37" s="120"/>
     </row>
     <row r="38" spans="1:6" ht="15.75">
-      <c r="A38" s="159" t="s">
+      <c r="A38" s="155" t="s">
         <v>739</v>
       </c>
-      <c r="B38" s="160" t="s">
+      <c r="B38" s="156" t="s">
         <v>430</v>
       </c>
-      <c r="C38" s="174" t="s">
+      <c r="C38" s="166" t="s">
         <v>793</v>
       </c>
-      <c r="D38" s="160" t="s">
+      <c r="D38" s="156" t="s">
         <v>757</v>
       </c>
-      <c r="E38" s="161" t="s">
+      <c r="E38" s="157" t="s">
         <v>868</v>
       </c>
       <c r="F38" s="120"/>
     </row>
     <row r="39" spans="1:6" ht="15.75">
-      <c r="A39" s="159" t="s">
+      <c r="A39" s="155" t="s">
         <v>740</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="156" t="s">
         <v>490</v>
       </c>
-      <c r="C39" s="174" t="s">
+      <c r="C39" s="166" t="s">
         <v>794</v>
       </c>
-      <c r="D39" s="160" t="s">
+      <c r="D39" s="156" t="s">
         <v>757</v>
       </c>
-      <c r="E39" s="161" t="s">
+      <c r="E39" s="157" t="s">
         <v>866</v>
       </c>
       <c r="F39" s="120"/>
     </row>
     <row r="40" spans="1:6" ht="15.75">
-      <c r="A40" s="159" t="s">
+      <c r="A40" s="155" t="s">
         <v>741</v>
       </c>
-      <c r="B40" s="160" t="s">
+      <c r="B40" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="C40" s="175" t="s">
+      <c r="C40" s="167" t="s">
         <v>580</v>
       </c>
-      <c r="D40" s="160" t="s">
+      <c r="D40" s="156" t="s">
         <v>756</v>
       </c>
-      <c r="E40" s="161" t="s">
+      <c r="E40" s="157" t="s">
         <v>749</v>
       </c>
       <c r="F40" s="120"/>
     </row>
     <row r="41" spans="1:6" ht="15.75">
-      <c r="A41" s="159" t="s">
+      <c r="A41" s="155" t="s">
         <v>742</v>
       </c>
-      <c r="B41" s="160" t="s">
+      <c r="B41" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="C41" s="175" t="s">
+      <c r="C41" s="167" t="s">
         <v>835</v>
       </c>
-      <c r="D41" s="160" t="s">
+      <c r="D41" s="156" t="s">
         <v>756</v>
       </c>
-      <c r="E41" s="161" t="s">
+      <c r="E41" s="157" t="s">
         <v>750</v>
       </c>
       <c r="F41" s="120"/>
     </row>
     <row r="42" spans="1:6" ht="15.75">
-      <c r="A42" s="159" t="s">
+      <c r="A42" s="155" t="s">
         <v>743</v>
       </c>
-      <c r="B42" s="160" t="s">
+      <c r="B42" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="C42" s="175" t="s">
+      <c r="C42" s="167" t="s">
         <v>840</v>
       </c>
-      <c r="D42" s="160" t="s">
+      <c r="D42" s="156" t="s">
         <v>756</v>
       </c>
-      <c r="E42" s="161" t="s">
+      <c r="E42" s="157" t="s">
         <v>751</v>
       </c>
       <c r="F42" s="120"/>
     </row>
     <row r="43" spans="1:6" ht="15.75">
-      <c r="A43" s="159" t="s">
+      <c r="A43" s="155" t="s">
         <v>744</v>
       </c>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="C43" s="175" t="s">
+      <c r="C43" s="167" t="s">
         <v>841</v>
       </c>
-      <c r="D43" s="160" t="s">
+      <c r="D43" s="156" t="s">
         <v>756</v>
       </c>
-      <c r="E43" s="161" t="s">
+      <c r="E43" s="157" t="s">
         <v>752</v>
       </c>
       <c r="F43" s="120"/>
     </row>
     <row r="44" spans="1:6" ht="15.75">
-      <c r="A44" s="159" t="s">
+      <c r="A44" s="155" t="s">
         <v>745</v>
       </c>
-      <c r="B44" s="160" t="s">
+      <c r="B44" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="C44" s="175" t="s">
+      <c r="C44" s="167" t="s">
         <v>838</v>
       </c>
-      <c r="D44" s="160" t="s">
+      <c r="D44" s="156" t="s">
         <v>756</v>
       </c>
-      <c r="E44" s="161" t="s">
+      <c r="E44" s="157" t="s">
         <v>753</v>
       </c>
       <c r="F44" s="120"/>
     </row>
     <row r="45" spans="1:6" ht="15.75">
-      <c r="A45" s="159" t="s">
+      <c r="A45" s="155" t="s">
         <v>746</v>
       </c>
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="156" t="s">
         <v>490</v>
       </c>
-      <c r="C45" s="175" t="s">
+      <c r="C45" s="167" t="s">
         <v>839</v>
       </c>
-      <c r="D45" s="160" t="s">
+      <c r="D45" s="156" t="s">
         <v>757</v>
       </c>
-      <c r="E45" s="161" t="s">
+      <c r="E45" s="157" t="s">
         <v>867</v>
       </c>
       <c r="F45" s="120"/>
     </row>
     <row r="46" spans="1:6" ht="15.75">
-      <c r="A46" s="159" t="s">
+      <c r="A46" s="155" t="s">
         <v>747</v>
       </c>
-      <c r="B46" s="160" t="s">
+      <c r="B46" s="156" t="s">
         <v>490</v>
       </c>
-      <c r="C46" s="175" t="s">
+      <c r="C46" s="167" t="s">
         <v>837</v>
       </c>
-      <c r="D46" s="160" t="s">
+      <c r="D46" s="156" t="s">
         <v>757</v>
       </c>
-      <c r="E46" s="161" t="s">
+      <c r="E46" s="157" t="s">
         <v>869</v>
       </c>
       <c r="F46" s="120"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A47" s="162" t="s">
+      <c r="A47" s="158" t="s">
         <v>748</v>
       </c>
-      <c r="B47" s="163" t="s">
+      <c r="B47" s="159" t="s">
         <v>431</v>
       </c>
-      <c r="C47" s="176" t="s">
+      <c r="C47" s="168" t="s">
         <v>836</v>
       </c>
-      <c r="D47" s="163" t="s">
+      <c r="D47" s="159" t="s">
         <v>758</v>
       </c>
-      <c r="E47" s="164" t="s">
+      <c r="E47" s="160" t="s">
         <v>754</v>
       </c>
       <c r="F47" s="120"/>
@@ -9991,13 +10133,14 @@
       <c r="F48" s="120"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="D22:D24"/>
+  <mergeCells count="7">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D23:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11200,28 +11343,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="208" t="s">
         <v>582</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
     </row>
     <row r="2" spans="1:17" ht="15.75">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="205" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="205"/>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="205"/>
-      <c r="H2" s="206"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="23"/>
@@ -11519,16 +11662,16 @@
       <c r="Q14" s="39"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="205" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="205"/>
-      <c r="C15" s="205"/>
-      <c r="D15" s="205"/>
-      <c r="E15" s="205"/>
-      <c r="F15" s="205"/>
-      <c r="G15" s="205"/>
-      <c r="H15" s="206"/>
+      <c r="B15" s="206"/>
+      <c r="C15" s="206"/>
+      <c r="D15" s="206"/>
+      <c r="E15" s="206"/>
+      <c r="F15" s="206"/>
+      <c r="G15" s="206"/>
+      <c r="H15" s="207"/>
       <c r="M15" s="39"/>
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
@@ -11888,16 +12031,16 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:17" ht="15.75">
-      <c r="A28" s="204" t="s">
+      <c r="A28" s="205" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="205"/>
-      <c r="C28" s="205"/>
-      <c r="D28" s="205"/>
-      <c r="E28" s="205"/>
-      <c r="F28" s="205"/>
-      <c r="G28" s="205"/>
-      <c r="H28" s="206"/>
+      <c r="B28" s="206"/>
+      <c r="C28" s="206"/>
+      <c r="D28" s="206"/>
+      <c r="E28" s="206"/>
+      <c r="F28" s="206"/>
+      <c r="G28" s="206"/>
+      <c r="H28" s="207"/>
     </row>
     <row r="29" spans="1:17" ht="15.75">
       <c r="A29" s="23"/>
@@ -12211,12 +12354,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="208" t="s">
         <v>843</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="41"/>
@@ -12423,28 +12566,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="209" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="208"/>
-      <c r="C1" s="208"/>
-      <c r="D1" s="208"/>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
+      <c r="B1" s="209"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="205" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="205"/>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="205"/>
-      <c r="H2" s="206"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="29" t="s">
@@ -12731,12 +12874,12 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="205" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="205"/>
-      <c r="C15" s="205"/>
-      <c r="D15" s="206"/>
+      <c r="B15" s="206"/>
+      <c r="C15" s="206"/>
+      <c r="D15" s="207"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -12915,12 +13058,12 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="204" t="s">
+      <c r="A28" s="205" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="205"/>
-      <c r="C28" s="205"/>
-      <c r="D28" s="206"/>
+      <c r="B28" s="206"/>
+      <c r="C28" s="206"/>
+      <c r="D28" s="207"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -13118,36 +13261,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>579</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
+      <c r="B1" s="210"/>
+      <c r="C1" s="210"/>
+      <c r="D1" s="210"/>
+      <c r="E1" s="210"/>
+      <c r="F1" s="210"/>
       <c r="G1" s="59"/>
       <c r="H1" s="59"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="210"/>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
+      <c r="A2" s="211"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="212" t="s">
         <v>612</v>
       </c>
-      <c r="B3" s="212"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="211" t="s">
+      <c r="B3" s="213"/>
+      <c r="C3" s="214"/>
+      <c r="D3" s="212" t="s">
         <v>613</v>
       </c>
-      <c r="E3" s="212"/>
-      <c r="F3" s="213"/>
+      <c r="E3" s="213"/>
+      <c r="F3" s="214"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="53">
@@ -13692,22 +13835,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="216" t="s">
         <v>584</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="214" t="s">
+      <c r="B2" s="215" t="s">
         <v>605</v>
       </c>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="41"/>
@@ -13812,12 +13955,12 @@
       <c r="E10" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="214" t="s">
+      <c r="B14" s="215" t="s">
         <v>600</v>
       </c>
-      <c r="C14" s="214"/>
-      <c r="D14" s="214"/>
-      <c r="E14" s="214"/>
+      <c r="C14" s="215"/>
+      <c r="D14" s="215"/>
+      <c r="E14" s="215"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="41"/>
@@ -13944,42 +14087,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="217" t="s">
         <v>871</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="218"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="219"/>
       <c r="I1" s="59"/>
       <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="219"/>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="221"/>
+      <c r="A2" s="220"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="222"/>
     </row>
     <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="222" t="s">
+      <c r="A3" s="223" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="223"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="225"/>
-      <c r="E3" s="222" t="s">
+      <c r="B3" s="224"/>
+      <c r="C3" s="225"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="223" t="s">
         <v>644</v>
       </c>
-      <c r="F3" s="223"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="225"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="226"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="119">

</xml_diff>

<commit_message>
chg: Updated freq: Added Fujairah TWR
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -520,30 +520,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Forfatter:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-On alert and can be launched as required</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A64" authorId="0">
       <text>
         <r>
@@ -616,12 +592,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+On alert and can be launched as required</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="923">
   <si>
     <t>AWACS</t>
   </si>
@@ -3335,9 +3335,6 @@
     <t>308.0</t>
   </si>
   <si>
-    <t>ATRM FREQ TWOPAGER v1.3</t>
-  </si>
-  <si>
     <t>BLUE Carrier</t>
   </si>
   <si>
@@ -3384,6 +3381,15 @@
   </si>
   <si>
     <t>80Y</t>
+  </si>
+  <si>
+    <t>Fujairah</t>
+  </si>
+  <si>
+    <t>ATRM FREQ TWOPAGER v1.4</t>
+  </si>
+  <si>
+    <t>124.8</t>
   </si>
 </sst>
 </file>
@@ -4402,7 +4408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4766,159 +4772,6 @@
     <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4937,25 +4790,7 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4983,47 +4818,8 @@
     <xf numFmtId="0" fontId="18" fillId="28" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5034,6 +4830,218 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5683,11 +5691,11 @@
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="181" t="s">
+      <c r="R3" s="223" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="182"/>
-      <c r="T3" s="183"/>
+      <c r="S3" s="224"/>
+      <c r="T3" s="225"/>
       <c r="V3" s="9" t="s">
         <v>3</v>
       </c>
@@ -5739,11 +5747,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="46"/>
-      <c r="R4" s="186" t="s">
+      <c r="R4" s="214" t="s">
         <v>690</v>
       </c>
-      <c r="S4" s="187"/>
-      <c r="T4" s="188"/>
+      <c r="S4" s="215"/>
+      <c r="T4" s="216"/>
       <c r="V4" s="9" t="s">
         <v>4</v>
       </c>
@@ -5753,16 +5761,16 @@
       <c r="X4" s="35" t="s">
         <v>338</v>
       </c>
-      <c r="Z4" s="184" t="s">
+      <c r="Z4" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="184"/>
-      <c r="AB4" s="184"/>
-      <c r="AD4" s="184" t="s">
+      <c r="AA4" s="206"/>
+      <c r="AB4" s="206"/>
+      <c r="AD4" s="206" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="184"/>
-      <c r="AF4" s="184"/>
+      <c r="AE4" s="206"/>
+      <c r="AF4" s="206"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
@@ -6237,11 +6245,11 @@
       <c r="X11" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="Z11" s="184" t="s">
+      <c r="Z11" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="184"/>
-      <c r="AB11" s="184"/>
+      <c r="AA11" s="206"/>
+      <c r="AB11" s="206"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
@@ -6616,11 +6624,11 @@
         <v>382</v>
       </c>
       <c r="Q17" s="5"/>
-      <c r="R17" s="178" t="s">
+      <c r="R17" s="217" t="s">
         <v>700</v>
       </c>
-      <c r="S17" s="179"/>
-      <c r="T17" s="180"/>
+      <c r="S17" s="218"/>
+      <c r="T17" s="219"/>
       <c r="V17" s="54" t="s">
         <v>902</v>
       </c>
@@ -6681,13 +6689,13 @@
         <v>417</v>
       </c>
       <c r="V18" s="54" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="W18" s="4" t="s">
         <v>195</v>
       </c>
       <c r="X18" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="19" spans="2:32">
@@ -6735,25 +6743,25 @@
         <v>314</v>
       </c>
       <c r="Q19" s="5"/>
-      <c r="R19" s="186" t="s">
+      <c r="R19" s="214" t="s">
         <v>691</v>
       </c>
-      <c r="S19" s="187"/>
-      <c r="T19" s="188"/>
-      <c r="V19" s="190" t="s">
+      <c r="S19" s="215"/>
+      <c r="T19" s="216"/>
+      <c r="V19" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="191"/>
-      <c r="X19" s="191"/>
-      <c r="Y19" s="191"/>
-      <c r="Z19" s="192"/>
-      <c r="AB19" s="184" t="s">
+      <c r="W19" s="208"/>
+      <c r="X19" s="208"/>
+      <c r="Y19" s="208"/>
+      <c r="Z19" s="209"/>
+      <c r="AB19" s="206" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="184"/>
-      <c r="AD19" s="184"/>
-      <c r="AE19" s="184"/>
-      <c r="AF19" s="184"/>
+      <c r="AC19" s="206"/>
+      <c r="AD19" s="206"/>
+      <c r="AE19" s="206"/>
+      <c r="AF19" s="206"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -7403,31 +7411,31 @@
       <c r="Z30" t="s">
         <v>852</v>
       </c>
-      <c r="AC30" s="184" t="s">
+      <c r="AC30" s="206" t="s">
         <v>575</v>
       </c>
-      <c r="AD30" s="184"/>
-      <c r="AE30" s="184"/>
+      <c r="AD30" s="206"/>
+      <c r="AE30" s="206"/>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="184" t="s">
+      <c r="B31" s="206" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="184"/>
-      <c r="D31" s="184"/>
-      <c r="E31" s="184"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="184"/>
-      <c r="H31" s="184"/>
-      <c r="J31" s="184" t="s">
+      <c r="C31" s="206"/>
+      <c r="D31" s="206"/>
+      <c r="E31" s="206"/>
+      <c r="F31" s="206"/>
+      <c r="G31" s="206"/>
+      <c r="H31" s="206"/>
+      <c r="J31" s="206" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="184"/>
-      <c r="L31" s="184"/>
-      <c r="M31" s="184"/>
-      <c r="N31" s="184"/>
-      <c r="O31" s="184"/>
-      <c r="P31" s="184"/>
+      <c r="K31" s="206"/>
+      <c r="L31" s="206"/>
+      <c r="M31" s="206"/>
+      <c r="N31" s="206"/>
+      <c r="O31" s="206"/>
+      <c r="P31" s="206"/>
       <c r="R31" s="95"/>
       <c r="S31" s="95"/>
       <c r="T31" s="95"/>
@@ -7504,19 +7512,19 @@
       <c r="T32" s="95"/>
       <c r="U32" s="163"/>
       <c r="V32" s="125" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="W32" s="126" t="s">
         <v>475</v>
       </c>
-      <c r="X32" s="269" t="s">
-        <v>915</v>
+      <c r="X32" s="199" t="s">
+        <v>914</v>
       </c>
       <c r="Y32" s="126" t="s">
         <v>740</v>
       </c>
-      <c r="Z32" s="270" t="s">
-        <v>916</v>
+      <c r="Z32" s="200" t="s">
+        <v>915</v>
       </c>
       <c r="AA32" s="163"/>
       <c r="AC32" s="9"/>
@@ -7565,19 +7573,19 @@
       <c r="S33" s="95"/>
       <c r="T33" s="95"/>
       <c r="V33" s="154" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="W33" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="X33" s="274" t="s">
+      <c r="X33" s="204" t="s">
+        <v>917</v>
+      </c>
+      <c r="Y33" s="155" t="s">
         <v>918</v>
       </c>
-      <c r="Y33" s="155" t="s">
+      <c r="Z33" s="134" t="s">
         <v>919</v>
-      </c>
-      <c r="Z33" s="134" t="s">
-        <v>920</v>
       </c>
       <c r="AC33" s="9"/>
       <c r="AD33" s="62" t="s">
@@ -7621,9 +7629,9 @@
       <c r="P34" t="s">
         <v>404</v>
       </c>
-      <c r="R34" s="185"/>
-      <c r="S34" s="185"/>
-      <c r="T34" s="185"/>
+      <c r="R34" s="213"/>
+      <c r="S34" s="213"/>
+      <c r="T34" s="213"/>
       <c r="AC34" s="9"/>
       <c r="AD34" s="62" t="s">
         <v>116</v>
@@ -7714,15 +7722,15 @@
       <c r="R36" s="93"/>
       <c r="S36" s="93"/>
       <c r="T36" s="95"/>
-      <c r="U36" s="195" t="s">
+      <c r="U36" s="212" t="s">
         <v>671</v>
       </c>
-      <c r="V36" s="195"/>
-      <c r="W36" s="195"/>
-      <c r="X36" s="195"/>
-      <c r="Y36" s="195"/>
-      <c r="Z36" s="195"/>
-      <c r="AA36" s="195"/>
+      <c r="V36" s="212"/>
+      <c r="W36" s="212"/>
+      <c r="X36" s="212"/>
+      <c r="Y36" s="212"/>
+      <c r="Z36" s="212"/>
+      <c r="AA36" s="212"/>
       <c r="AC36" s="9" t="s">
         <v>587</v>
       </c>
@@ -7867,15 +7875,15 @@
       <c r="H39" t="s">
         <v>390</v>
       </c>
-      <c r="J39" s="189" t="s">
+      <c r="J39" s="205" t="s">
         <v>401</v>
       </c>
-      <c r="K39" s="189"/>
-      <c r="L39" s="189"/>
-      <c r="M39" s="189"/>
-      <c r="N39" s="189"/>
-      <c r="O39" s="189"/>
-      <c r="P39" s="189"/>
+      <c r="K39" s="205"/>
+      <c r="L39" s="205"/>
+      <c r="M39" s="205"/>
+      <c r="N39" s="205"/>
+      <c r="O39" s="205"/>
+      <c r="P39" s="205"/>
       <c r="R39" s="95"/>
       <c r="S39" s="93"/>
       <c r="T39" s="95"/>
@@ -7964,13 +7972,13 @@
       <c r="AA41" t="s">
         <v>414</v>
       </c>
-      <c r="AC41" s="193" t="s">
+      <c r="AC41" s="210" t="s">
         <v>769</v>
       </c>
-      <c r="AD41" s="194"/>
-      <c r="AE41" s="194"/>
-      <c r="AF41" s="194"/>
-      <c r="AG41" s="194"/>
+      <c r="AD41" s="211"/>
+      <c r="AE41" s="211"/>
+      <c r="AF41" s="211"/>
+      <c r="AG41" s="211"/>
     </row>
     <row r="42" spans="2:33">
       <c r="E42" s="14" t="s">
@@ -8070,11 +8078,11 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="178" t="s">
+      <c r="Q45" s="217" t="s">
         <v>640</v>
       </c>
-      <c r="R45" s="179"/>
-      <c r="S45" s="180"/>
+      <c r="R45" s="218"/>
+      <c r="S45" s="219"/>
       <c r="T45" s="39"/>
       <c r="W45" t="s">
         <v>719</v>
@@ -8100,7 +8108,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="175" t="s">
+      <c r="Q46" s="220" t="s">
         <v>690</v>
       </c>
       <c r="R46" s="97" t="s">
@@ -8132,7 +8140,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="176"/>
+      <c r="Q47" s="221"/>
       <c r="R47" s="9" t="s">
         <v>654</v>
       </c>
@@ -8141,7 +8149,7 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q48" s="177"/>
+      <c r="Q48" s="222"/>
       <c r="R48" s="83" t="s">
         <v>655</v>
       </c>
@@ -8151,7 +8159,7 @@
       <c r="T48" s="39"/>
     </row>
     <row r="49" spans="17:35">
-      <c r="Q49" s="175" t="s">
+      <c r="Q49" s="220" t="s">
         <v>691</v>
       </c>
       <c r="R49" s="97" t="s">
@@ -8169,7 +8177,7 @@
       <c r="Y49" s="158"/>
     </row>
     <row r="50" spans="17:35">
-      <c r="Q50" s="176"/>
+      <c r="Q50" s="221"/>
       <c r="R50" s="9" t="s">
         <v>656</v>
       </c>
@@ -8193,7 +8201,7 @@
       </c>
     </row>
     <row r="51" spans="17:35" ht="15.75" thickBot="1">
-      <c r="Q51" s="177"/>
+      <c r="Q51" s="222"/>
       <c r="R51" s="83" t="s">
         <v>657</v>
       </c>
@@ -8215,15 +8223,15 @@
       <c r="Y51" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="AC51" s="184" t="s">
+      <c r="AC51" s="206" t="s">
         <v>616</v>
       </c>
-      <c r="AD51" s="184"/>
-      <c r="AE51" s="184"/>
-      <c r="AF51" s="184"/>
-      <c r="AG51" s="184"/>
-      <c r="AH51" s="184"/>
-      <c r="AI51" s="184"/>
+      <c r="AD51" s="206"/>
+      <c r="AE51" s="206"/>
+      <c r="AF51" s="206"/>
+      <c r="AG51" s="206"/>
+      <c r="AH51" s="206"/>
+      <c r="AI51" s="206"/>
     </row>
     <row r="52" spans="17:35">
       <c r="U52" s="76">
@@ -8607,15 +8615,15 @@
       <c r="Y64" t="s">
         <v>856</v>
       </c>
-      <c r="AC64" s="184" t="s">
+      <c r="AC64" s="206" t="s">
         <v>669</v>
       </c>
-      <c r="AD64" s="184"/>
-      <c r="AE64" s="184"/>
-      <c r="AF64" s="184"/>
-      <c r="AG64" s="184"/>
-      <c r="AH64" s="184"/>
-      <c r="AI64" s="184"/>
+      <c r="AD64" s="206"/>
+      <c r="AE64" s="206"/>
+      <c r="AF64" s="206"/>
+      <c r="AG64" s="206"/>
+      <c r="AH64" s="206"/>
+      <c r="AI64" s="206"/>
     </row>
     <row r="65" spans="21:35">
       <c r="AC65" s="16" t="s">
@@ -8817,6 +8825,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="J31:P31"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="AC64:AI64"/>
     <mergeCell ref="AC51:AI51"/>
@@ -8827,17 +8843,9 @@
     <mergeCell ref="AC41:AG41"/>
     <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="U36:AA36"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="Q46:Q48"/>
     <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8887,40 +8895,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="248" t="s">
         <v>771</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="219"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
+      <c r="A2" s="249"/>
+      <c r="B2" s="249"/>
+      <c r="C2" s="249"/>
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249"/>
+      <c r="H2" s="249"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="244" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="215"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="214" t="s">
+      <c r="B3" s="245"/>
+      <c r="C3" s="246"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="244" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="215"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="217"/>
+      <c r="F3" s="245"/>
+      <c r="G3" s="246"/>
+      <c r="H3" s="247"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="113">
@@ -9439,10 +9447,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R96"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9455,40 +9463,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A1" s="258" t="s">
-        <v>904</v>
-      </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="260"/>
+      <c r="A1" s="272" t="s">
+        <v>921</v>
+      </c>
+      <c r="B1" s="273"/>
+      <c r="C1" s="273"/>
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="274"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="253" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="263" t="s">
+      <c r="B2" s="254"/>
+      <c r="C2" s="254"/>
+      <c r="D2" s="269" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="264"/>
-      <c r="F2" s="265"/>
+      <c r="E2" s="270"/>
+      <c r="F2" s="271"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="266" t="s">
-        <v>913</v>
-      </c>
-      <c r="B3" s="267"/>
-      <c r="C3" s="268"/>
-      <c r="D3" s="261" t="s">
+      <c r="A3" s="256" t="s">
+        <v>912</v>
+      </c>
+      <c r="B3" s="257"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="227" t="s">
+      <c r="E3" s="176" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="262" t="s">
+      <c r="F3" s="198" t="s">
         <v>337</v>
       </c>
     </row>
@@ -9499,7 +9507,7 @@
       <c r="B4" s="123" t="s">
         <v>674</v>
       </c>
-      <c r="C4" s="241" t="s">
+      <c r="C4" s="184" t="s">
         <v>673</v>
       </c>
       <c r="D4" s="120" t="s">
@@ -9579,7 +9587,7 @@
       <c r="B8" s="123" t="s">
         <v>674</v>
       </c>
-      <c r="C8" s="241" t="s">
+      <c r="C8" s="184" t="s">
         <v>682</v>
       </c>
       <c r="D8" s="120" t="s">
@@ -9619,7 +9627,7 @@
       <c r="B10" s="124" t="s">
         <v>676</v>
       </c>
-      <c r="C10" s="242" t="s">
+      <c r="C10" s="185" t="s">
         <v>684</v>
       </c>
       <c r="D10" s="120" t="s">
@@ -9639,7 +9647,7 @@
       <c r="B11" s="124" t="s">
         <v>677</v>
       </c>
-      <c r="C11" s="242" t="s">
+      <c r="C11" s="185" t="s">
         <v>685</v>
       </c>
       <c r="D11" s="120" t="s">
@@ -9659,7 +9667,7 @@
       <c r="B12" s="124" t="s">
         <v>675</v>
       </c>
-      <c r="C12" s="242" t="s">
+      <c r="C12" s="185" t="s">
         <v>687</v>
       </c>
       <c r="D12" s="120" t="s">
@@ -9679,7 +9687,7 @@
       <c r="B13" s="126" t="s">
         <v>677</v>
       </c>
-      <c r="C13" s="243" t="s">
+      <c r="C13" s="186" t="s">
         <v>698</v>
       </c>
       <c r="D13" s="120" t="s">
@@ -9699,7 +9707,7 @@
       <c r="B14" s="124" t="s">
         <v>675</v>
       </c>
-      <c r="C14" s="242" t="s">
+      <c r="C14" s="185" t="s">
         <v>689</v>
       </c>
       <c r="D14" s="127" t="s">
@@ -9719,7 +9727,7 @@
       <c r="B15" s="129" t="s">
         <v>677</v>
       </c>
-      <c r="C15" s="244" t="s">
+      <c r="C15" s="187" t="s">
         <v>699</v>
       </c>
       <c r="D15" s="120" t="s">
@@ -9751,7 +9759,7 @@
       <c r="B17" s="132" t="s">
         <v>700</v>
       </c>
-      <c r="C17" s="240" t="s">
+      <c r="C17" s="183" t="s">
         <v>417</v>
       </c>
       <c r="D17" s="154" t="s">
@@ -9772,11 +9780,11 @@
       <c r="C18" s="140" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="223" t="s">
-        <v>905</v>
-      </c>
-      <c r="E18" s="224"/>
-      <c r="F18" s="225"/>
+      <c r="D18" s="253" t="s">
+        <v>904</v>
+      </c>
+      <c r="E18" s="254"/>
+      <c r="F18" s="255"/>
     </row>
     <row r="19" spans="1:18" ht="15.75">
       <c r="A19" s="137">
@@ -9788,7 +9796,7 @@
       <c r="C19" s="142" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="220" t="s">
+      <c r="D19" s="266" t="s">
         <v>690</v>
       </c>
       <c r="E19" s="138" t="s">
@@ -9808,7 +9816,7 @@
       <c r="C20" s="142" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="221"/>
+      <c r="D20" s="267"/>
       <c r="E20" s="124" t="s">
         <v>654</v>
       </c>
@@ -9829,7 +9837,7 @@
       <c r="C21" s="142" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="222"/>
+      <c r="D21" s="268"/>
       <c r="E21" s="150" t="s">
         <v>655</v>
       </c>
@@ -9870,13 +9878,13 @@
       <c r="C23" s="142" t="s">
         <v>269</v>
       </c>
-      <c r="D23" s="229" t="s">
+      <c r="D23" s="178" t="s">
         <v>758</v>
       </c>
-      <c r="E23" s="230" t="s">
+      <c r="E23" s="179" t="s">
         <v>302</v>
       </c>
-      <c r="F23" s="231" t="s">
+      <c r="F23" s="180" t="s">
         <v>303</v>
       </c>
     </row>
@@ -9890,13 +9898,13 @@
       <c r="C24" s="142" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="239" t="s">
+      <c r="D24" s="182" t="s">
         <v>753</v>
       </c>
-      <c r="E24" s="227" t="s">
+      <c r="E24" s="176" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="228" t="s">
+      <c r="F24" s="177" t="s">
         <v>766</v>
       </c>
     </row>
@@ -9950,9 +9958,9 @@
       <c r="C27" s="142" t="s">
         <v>762</v>
       </c>
-      <c r="D27" s="245"/>
-      <c r="E27" s="245"/>
-      <c r="F27" s="246"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="189"/>
     </row>
     <row r="28" spans="1:18" ht="15.75">
       <c r="A28" s="137">
@@ -9964,9 +9972,9 @@
       <c r="C28" s="142" t="s">
         <v>763</v>
       </c>
-      <c r="D28" s="245"/>
-      <c r="E28" s="245"/>
-      <c r="F28" s="246"/>
+      <c r="D28" s="188"/>
+      <c r="E28" s="188"/>
+      <c r="F28" s="189"/>
     </row>
     <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="137">
@@ -9978,9 +9986,9 @@
       <c r="C29" s="142" t="s">
         <v>764</v>
       </c>
-      <c r="D29" s="245"/>
-      <c r="E29" s="245"/>
-      <c r="F29" s="246"/>
+      <c r="D29" s="188"/>
+      <c r="E29" s="188"/>
+      <c r="F29" s="189"/>
     </row>
     <row r="30" spans="1:18" ht="15.75">
       <c r="A30" s="137">
@@ -9992,9 +10000,9 @@
       <c r="C30" s="142" t="s">
         <v>765</v>
       </c>
-      <c r="D30" s="245"/>
-      <c r="E30" s="245"/>
-      <c r="F30" s="246"/>
+      <c r="D30" s="188"/>
+      <c r="E30" s="188"/>
+      <c r="F30" s="189"/>
     </row>
     <row r="31" spans="1:18" ht="15.75">
       <c r="A31" s="137">
@@ -10006,9 +10014,9 @@
       <c r="C31" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="245"/>
-      <c r="E31" s="245"/>
-      <c r="F31" s="246"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="188"/>
+      <c r="F31" s="189"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="137">
@@ -10020,43 +10028,43 @@
       <c r="C32" s="148" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="245"/>
-      <c r="E32" s="245"/>
-      <c r="F32" s="246"/>
+      <c r="D32" s="188"/>
+      <c r="E32" s="188"/>
+      <c r="F32" s="189"/>
     </row>
     <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="137"/>
       <c r="B33" s="135"/>
       <c r="C33" s="142"/>
-      <c r="D33" s="245"/>
-      <c r="E33" s="245"/>
-      <c r="F33" s="246"/>
+      <c r="D33" s="188"/>
+      <c r="E33" s="188"/>
+      <c r="F33" s="189"/>
     </row>
     <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="137"/>
       <c r="B34" s="135"/>
       <c r="C34" s="142"/>
-      <c r="D34" s="245"/>
-      <c r="E34" s="245"/>
-      <c r="F34" s="246"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188"/>
+      <c r="F34" s="189"/>
     </row>
     <row r="35" spans="1:6" ht="16.5" thickBot="1">
       <c r="A35" s="139"/>
       <c r="B35" s="133"/>
       <c r="C35" s="143"/>
-      <c r="D35" s="245"/>
-      <c r="E35" s="245"/>
-      <c r="F35" s="246"/>
+      <c r="D35" s="188"/>
+      <c r="E35" s="188"/>
+      <c r="F35" s="189"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A36" s="236" t="s">
-        <v>906</v>
-      </c>
-      <c r="B36" s="237"/>
-      <c r="C36" s="237"/>
-      <c r="D36" s="237"/>
-      <c r="E36" s="238"/>
-      <c r="F36" s="247"/>
+      <c r="A36" s="250" t="s">
+        <v>905</v>
+      </c>
+      <c r="B36" s="251"/>
+      <c r="C36" s="251"/>
+      <c r="D36" s="251"/>
+      <c r="E36" s="252"/>
+      <c r="F36" s="190"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="166" t="s">
@@ -10074,7 +10082,7 @@
       <c r="E37" s="167" t="s">
         <v>316</v>
       </c>
-      <c r="F37" s="247"/>
+      <c r="F37" s="190"/>
     </row>
     <row r="38" spans="1:6" ht="15.75">
       <c r="A38" s="120" t="s">
@@ -10092,7 +10100,7 @@
       <c r="E38" s="130" t="s">
         <v>851</v>
       </c>
-      <c r="F38" s="247"/>
+      <c r="F38" s="190"/>
     </row>
     <row r="39" spans="1:6" ht="15.75">
       <c r="A39" s="120" t="s">
@@ -10110,7 +10118,7 @@
       <c r="E39" s="130" t="s">
         <v>849</v>
       </c>
-      <c r="F39" s="247"/>
+      <c r="F39" s="190"/>
     </row>
     <row r="40" spans="1:6" ht="15.75">
       <c r="A40" s="120" t="s">
@@ -10128,43 +10136,43 @@
       <c r="E40" s="130" t="s">
         <v>897</v>
       </c>
-      <c r="F40" s="247"/>
+      <c r="F40" s="190"/>
     </row>
     <row r="41" spans="1:6" ht="15.75">
       <c r="A41" s="125" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B41" s="126" t="s">
         <v>475</v>
       </c>
-      <c r="C41" s="269" t="s">
-        <v>915</v>
+      <c r="C41" s="199" t="s">
+        <v>914</v>
       </c>
       <c r="D41" s="126" t="s">
         <v>740</v>
       </c>
-      <c r="E41" s="270" t="s">
-        <v>916</v>
-      </c>
-      <c r="F41" s="247"/>
+      <c r="E41" s="200" t="s">
+        <v>915</v>
+      </c>
+      <c r="F41" s="190"/>
     </row>
     <row r="42" spans="1:6" ht="15.75">
-      <c r="A42" s="235" t="s">
+      <c r="A42" s="181" t="s">
         <v>898</v>
       </c>
-      <c r="B42" s="271" t="s">
+      <c r="B42" s="201" t="s">
         <v>425</v>
       </c>
-      <c r="C42" s="272" t="s">
+      <c r="C42" s="202" t="s">
         <v>565</v>
       </c>
-      <c r="D42" s="271" t="s">
+      <c r="D42" s="201" t="s">
         <v>739</v>
       </c>
-      <c r="E42" s="273" t="s">
+      <c r="E42" s="203" t="s">
         <v>732</v>
       </c>
-      <c r="F42" s="247"/>
+      <c r="F42" s="190"/>
     </row>
     <row r="43" spans="1:6" ht="15.75">
       <c r="A43" s="120" t="s">
@@ -10182,7 +10190,7 @@
       <c r="E43" s="130" t="s">
         <v>733</v>
       </c>
-      <c r="F43" s="247"/>
+      <c r="F43" s="190"/>
     </row>
     <row r="44" spans="1:6" ht="15.75">
       <c r="A44" s="120" t="s">
@@ -10200,7 +10208,7 @@
       <c r="E44" s="130" t="s">
         <v>734</v>
       </c>
-      <c r="F44" s="247"/>
+      <c r="F44" s="190"/>
     </row>
     <row r="45" spans="1:6" ht="15.75">
       <c r="A45" s="120" t="s">
@@ -10218,545 +10226,566 @@
       <c r="E45" s="130" t="s">
         <v>735</v>
       </c>
-      <c r="F45" s="247"/>
+      <c r="F45" s="190"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1">
       <c r="A46" s="154" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B46" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="C46" s="274" t="s">
+      <c r="C46" s="204" t="s">
+        <v>917</v>
+      </c>
+      <c r="D46" s="155" t="s">
         <v>918</v>
       </c>
-      <c r="D46" s="155" t="s">
+      <c r="E46" s="134" t="s">
         <v>919</v>
       </c>
-      <c r="E46" s="134" t="s">
-        <v>920</v>
-      </c>
-      <c r="F46" s="247"/>
+      <c r="F46" s="190"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A47" s="249"/>
-      <c r="B47" s="250"/>
-      <c r="C47" s="250"/>
-      <c r="D47" s="250"/>
-      <c r="E47" s="250"/>
-      <c r="F47" s="251"/>
+      <c r="A47" s="192"/>
+      <c r="B47" s="193"/>
+      <c r="C47" s="193"/>
+      <c r="D47" s="193"/>
+      <c r="E47" s="193"/>
+      <c r="F47" s="194"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A48" s="254" t="s">
-        <v>904</v>
-      </c>
-      <c r="B48" s="255"/>
-      <c r="C48" s="255"/>
-      <c r="D48" s="256"/>
-      <c r="E48" s="256"/>
-      <c r="F48" s="257"/>
+      <c r="A48" s="259" t="s">
+        <v>921</v>
+      </c>
+      <c r="B48" s="260"/>
+      <c r="C48" s="260"/>
+      <c r="D48" s="261"/>
+      <c r="E48" s="261"/>
+      <c r="F48" s="262"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="248"/>
-      <c r="B49" s="245"/>
-      <c r="C49" s="245"/>
-      <c r="D49" s="232" t="s">
+      <c r="A49" s="191"/>
+      <c r="B49" s="188"/>
+      <c r="C49" s="188"/>
+      <c r="D49" s="263" t="s">
+        <v>907</v>
+      </c>
+      <c r="E49" s="264"/>
+      <c r="F49" s="265"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="191"/>
+      <c r="B50" s="188"/>
+      <c r="C50" s="188"/>
+      <c r="D50" s="120" t="s">
         <v>908</v>
-      </c>
-      <c r="E49" s="233"/>
-      <c r="F49" s="234"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="248"/>
-      <c r="B50" s="245"/>
-      <c r="C50" s="245"/>
-      <c r="D50" s="120" t="s">
-        <v>909</v>
       </c>
       <c r="E50" s="120" t="s">
         <v>195</v>
       </c>
-      <c r="F50" s="252" t="s">
-        <v>911</v>
+      <c r="F50" s="195" t="s">
+        <v>910</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A51" s="248"/>
-      <c r="B51" s="245"/>
-      <c r="C51" s="245"/>
+      <c r="A51" s="191"/>
+      <c r="B51" s="188"/>
+      <c r="C51" s="188"/>
       <c r="D51" s="120" t="s">
         <v>743</v>
       </c>
       <c r="E51" s="120" t="s">
         <v>746</v>
       </c>
-      <c r="F51" s="252"/>
+      <c r="F51" s="195"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A52" s="248"/>
-      <c r="B52" s="245"/>
-      <c r="C52" s="245"/>
-      <c r="D52" s="223" t="s">
+      <c r="A52" s="191"/>
+      <c r="B52" s="188"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="253" t="s">
         <v>858</v>
       </c>
-      <c r="E52" s="224"/>
-      <c r="F52" s="225"/>
+      <c r="E52" s="254"/>
+      <c r="F52" s="255"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="248"/>
-      <c r="B53" s="245"/>
-      <c r="C53" s="245"/>
+      <c r="A53" s="191"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="188"/>
       <c r="D53" s="120" t="s">
         <v>692</v>
       </c>
       <c r="E53" s="120" t="s">
         <v>675</v>
       </c>
-      <c r="F53" s="252" t="s">
+      <c r="F53" s="195" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="248"/>
-      <c r="B54" s="245"/>
-      <c r="C54" s="245"/>
+      <c r="A54" s="191"/>
+      <c r="B54" s="188"/>
+      <c r="C54" s="188"/>
       <c r="D54" s="120" t="s">
         <v>693</v>
       </c>
       <c r="E54" s="120" t="s">
         <v>675</v>
       </c>
-      <c r="F54" s="252" t="s">
+      <c r="F54" s="195" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="248"/>
-      <c r="B55" s="245"/>
-      <c r="C55" s="245"/>
+      <c r="A55" s="191"/>
+      <c r="B55" s="188"/>
+      <c r="C55" s="188"/>
       <c r="D55" s="120" t="s">
-        <v>696</v>
+        <v>920</v>
       </c>
       <c r="E55" s="120" t="s">
         <v>675</v>
       </c>
-      <c r="F55" s="252" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A56" s="248"/>
-      <c r="B56" s="245"/>
-      <c r="C56" s="245"/>
+      <c r="F55" s="195" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="191"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="188"/>
       <c r="D56" s="120" t="s">
         <v>696</v>
       </c>
       <c r="E56" s="120" t="s">
+        <v>675</v>
+      </c>
+      <c r="F56" s="195" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A57" s="191"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="188"/>
+      <c r="D57" s="120" t="s">
+        <v>696</v>
+      </c>
+      <c r="E57" s="120" t="s">
         <v>677</v>
       </c>
-      <c r="F56" s="252" t="s">
+      <c r="F57" s="195" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A57" s="248"/>
-      <c r="B57" s="245"/>
-      <c r="C57" s="245"/>
-      <c r="D57" s="223" t="s">
-        <v>912</v>
-      </c>
-      <c r="E57" s="224"/>
-      <c r="F57" s="225"/>
-    </row>
-    <row r="58" spans="1:6" ht="15.75">
-      <c r="A58" s="248"/>
-      <c r="B58" s="245"/>
-      <c r="C58" s="245"/>
-      <c r="D58" s="220" t="s">
+    <row r="58" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A58" s="191"/>
+      <c r="B58" s="188"/>
+      <c r="C58" s="188"/>
+      <c r="D58" s="253" t="s">
+        <v>911</v>
+      </c>
+      <c r="E58" s="254"/>
+      <c r="F58" s="255"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75">
+      <c r="A59" s="191"/>
+      <c r="B59" s="188"/>
+      <c r="C59" s="188"/>
+      <c r="D59" s="266" t="s">
         <v>691</v>
       </c>
-      <c r="E58" s="138" t="s">
+      <c r="E59" s="138" t="s">
         <v>653</v>
       </c>
-      <c r="F58" s="152" t="s">
+      <c r="F59" s="152" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75">
-      <c r="A59" s="248"/>
-      <c r="B59" s="245"/>
-      <c r="C59" s="245"/>
-      <c r="D59" s="221"/>
-      <c r="E59" s="124" t="s">
+    <row r="60" spans="1:6" ht="15.75">
+      <c r="A60" s="191"/>
+      <c r="B60" s="188"/>
+      <c r="C60" s="188"/>
+      <c r="D60" s="267"/>
+      <c r="E60" s="124" t="s">
         <v>656</v>
       </c>
-      <c r="F59" s="157" t="s">
+      <c r="F60" s="157" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75">
-      <c r="A60" s="248"/>
-      <c r="B60" s="245"/>
-      <c r="C60" s="245"/>
-      <c r="D60" s="222"/>
-      <c r="E60" s="150" t="s">
+    <row r="61" spans="1:6" ht="15.75">
+      <c r="A61" s="191"/>
+      <c r="B61" s="188"/>
+      <c r="C61" s="188"/>
+      <c r="D61" s="268"/>
+      <c r="E61" s="150" t="s">
         <v>657</v>
       </c>
-      <c r="F60" s="153" t="s">
+      <c r="F61" s="153" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A61" s="248"/>
-      <c r="B61" s="245"/>
-      <c r="C61" s="245"/>
-      <c r="D61" s="235" t="s">
+    <row r="62" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A62" s="191"/>
+      <c r="B62" s="188"/>
+      <c r="C62" s="188"/>
+      <c r="D62" s="181" t="s">
         <v>866</v>
       </c>
-      <c r="E61" s="226" t="s">
+      <c r="E62" s="175" t="s">
         <v>425</v>
       </c>
-      <c r="F61" s="151" t="s">
+      <c r="F62" s="151" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A62" s="236" t="s">
-        <v>907</v>
-      </c>
-      <c r="B62" s="237"/>
-      <c r="C62" s="237"/>
-      <c r="D62" s="237"/>
-      <c r="E62" s="238"/>
-      <c r="F62" s="246"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75">
-      <c r="A63" s="120" t="s">
-        <v>728</v>
-      </c>
-      <c r="B63" s="124" t="s">
-        <v>425</v>
-      </c>
-      <c r="C63" s="165" t="s">
-        <v>821</v>
-      </c>
-      <c r="D63" s="124" t="s">
-        <v>739</v>
-      </c>
-      <c r="E63" s="130" t="s">
-        <v>736</v>
-      </c>
-      <c r="F63" s="246"/>
+    <row r="63" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A63" s="250" t="s">
+        <v>906</v>
+      </c>
+      <c r="B63" s="251"/>
+      <c r="C63" s="251"/>
+      <c r="D63" s="251"/>
+      <c r="E63" s="252"/>
+      <c r="F63" s="189"/>
     </row>
     <row r="64" spans="1:6" ht="15.75">
       <c r="A64" s="120" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B64" s="124" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="C64" s="165" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D64" s="124" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E64" s="130" t="s">
-        <v>850</v>
-      </c>
-      <c r="F64" s="246"/>
+        <v>736</v>
+      </c>
+      <c r="F64" s="189"/>
     </row>
     <row r="65" spans="1:6" ht="15.75">
       <c r="A65" s="120" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B65" s="124" t="s">
         <v>475</v>
       </c>
       <c r="C65" s="165" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D65" s="124" t="s">
         <v>740</v>
       </c>
       <c r="E65" s="130" t="s">
+        <v>850</v>
+      </c>
+      <c r="F65" s="189"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75">
+      <c r="A66" s="120" t="s">
+        <v>730</v>
+      </c>
+      <c r="B66" s="124" t="s">
+        <v>475</v>
+      </c>
+      <c r="C66" s="165" t="s">
+        <v>820</v>
+      </c>
+      <c r="D66" s="124" t="s">
+        <v>740</v>
+      </c>
+      <c r="E66" s="130" t="s">
         <v>852</v>
       </c>
-      <c r="F65" s="246"/>
-    </row>
-    <row r="66" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A66" s="154" t="s">
+      <c r="F66" s="189"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A67" s="154" t="s">
         <v>731</v>
       </c>
-      <c r="B66" s="155" t="s">
+      <c r="B67" s="155" t="s">
         <v>425</v>
       </c>
-      <c r="C66" s="168" t="s">
+      <c r="C67" s="168" t="s">
         <v>819</v>
       </c>
-      <c r="D66" s="155" t="s">
+      <c r="D67" s="155" t="s">
         <v>741</v>
       </c>
-      <c r="E66" s="134" t="s">
+      <c r="E67" s="134" t="s">
         <v>737</v>
       </c>
-      <c r="F66" s="246"/>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="248"/>
-      <c r="B67" s="245"/>
-      <c r="C67" s="245"/>
-      <c r="D67" s="245"/>
-      <c r="E67" s="245"/>
-      <c r="F67" s="246"/>
+      <c r="F67" s="189"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="248"/>
-      <c r="B68" s="245"/>
-      <c r="C68" s="245"/>
-      <c r="D68" s="245"/>
-      <c r="E68" s="245"/>
-      <c r="F68" s="246"/>
+      <c r="A68" s="191"/>
+      <c r="B68" s="188"/>
+      <c r="C68" s="188"/>
+      <c r="D68" s="188"/>
+      <c r="E68" s="188"/>
+      <c r="F68" s="189"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="248"/>
-      <c r="B69" s="245"/>
-      <c r="C69" s="245"/>
-      <c r="D69" s="245"/>
-      <c r="E69" s="245"/>
-      <c r="F69" s="246"/>
+      <c r="A69" s="191"/>
+      <c r="B69" s="188"/>
+      <c r="C69" s="188"/>
+      <c r="D69" s="188"/>
+      <c r="E69" s="188"/>
+      <c r="F69" s="189"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="248"/>
-      <c r="B70" s="245"/>
-      <c r="C70" s="245"/>
-      <c r="D70" s="245"/>
-      <c r="E70" s="245"/>
-      <c r="F70" s="246"/>
+      <c r="A70" s="191"/>
+      <c r="B70" s="188"/>
+      <c r="C70" s="188"/>
+      <c r="D70" s="188"/>
+      <c r="E70" s="188"/>
+      <c r="F70" s="189"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="248"/>
-      <c r="B71" s="245"/>
-      <c r="C71" s="245"/>
-      <c r="D71" s="245"/>
-      <c r="E71" s="245"/>
-      <c r="F71" s="246"/>
+      <c r="A71" s="191"/>
+      <c r="B71" s="188"/>
+      <c r="C71" s="188"/>
+      <c r="D71" s="188"/>
+      <c r="E71" s="188"/>
+      <c r="F71" s="189"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="248"/>
-      <c r="B72" s="245"/>
-      <c r="C72" s="245"/>
-      <c r="D72" s="245"/>
-      <c r="E72" s="245"/>
-      <c r="F72" s="246"/>
+      <c r="A72" s="191"/>
+      <c r="B72" s="188"/>
+      <c r="C72" s="188"/>
+      <c r="D72" s="188"/>
+      <c r="E72" s="188"/>
+      <c r="F72" s="189"/>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="248"/>
-      <c r="B73" s="245"/>
-      <c r="C73" s="245"/>
-      <c r="D73" s="245"/>
-      <c r="E73" s="245"/>
-      <c r="F73" s="246"/>
+      <c r="A73" s="191"/>
+      <c r="B73" s="188"/>
+      <c r="C73" s="188"/>
+      <c r="D73" s="188"/>
+      <c r="E73" s="188"/>
+      <c r="F73" s="189"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="248"/>
-      <c r="B74" s="245"/>
-      <c r="C74" s="245"/>
-      <c r="D74" s="245"/>
-      <c r="E74" s="245"/>
-      <c r="F74" s="246"/>
+      <c r="A74" s="191"/>
+      <c r="B74" s="188"/>
+      <c r="C74" s="188"/>
+      <c r="D74" s="188"/>
+      <c r="E74" s="188"/>
+      <c r="F74" s="189"/>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="248"/>
-      <c r="B75" s="245"/>
-      <c r="C75" s="245"/>
-      <c r="D75" s="245"/>
-      <c r="E75" s="245"/>
-      <c r="F75" s="246"/>
+      <c r="A75" s="191"/>
+      <c r="B75" s="188"/>
+      <c r="C75" s="188"/>
+      <c r="D75" s="188"/>
+      <c r="E75" s="188"/>
+      <c r="F75" s="189"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="248"/>
-      <c r="B76" s="245"/>
-      <c r="C76" s="245"/>
-      <c r="D76" s="245"/>
-      <c r="E76" s="245"/>
-      <c r="F76" s="246"/>
+      <c r="A76" s="191"/>
+      <c r="B76" s="188"/>
+      <c r="C76" s="188"/>
+      <c r="D76" s="188"/>
+      <c r="E76" s="188"/>
+      <c r="F76" s="189"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="248"/>
-      <c r="B77" s="245"/>
-      <c r="C77" s="245"/>
-      <c r="D77" s="245"/>
-      <c r="E77" s="245"/>
-      <c r="F77" s="246"/>
+      <c r="A77" s="191"/>
+      <c r="B77" s="188"/>
+      <c r="C77" s="188"/>
+      <c r="D77" s="188"/>
+      <c r="E77" s="188"/>
+      <c r="F77" s="189"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="248"/>
-      <c r="B78" s="245"/>
-      <c r="C78" s="245"/>
-      <c r="D78" s="245"/>
-      <c r="E78" s="245"/>
-      <c r="F78" s="246"/>
+      <c r="A78" s="191"/>
+      <c r="B78" s="188"/>
+      <c r="C78" s="188"/>
+      <c r="D78" s="188"/>
+      <c r="E78" s="188"/>
+      <c r="F78" s="189"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="248"/>
-      <c r="B79" s="245"/>
-      <c r="C79" s="245"/>
-      <c r="D79" s="245"/>
-      <c r="E79" s="245"/>
-      <c r="F79" s="246"/>
+      <c r="A79" s="191"/>
+      <c r="B79" s="188"/>
+      <c r="C79" s="188"/>
+      <c r="D79" s="188"/>
+      <c r="E79" s="188"/>
+      <c r="F79" s="189"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="248"/>
-      <c r="B80" s="245"/>
-      <c r="C80" s="245"/>
-      <c r="D80" s="245"/>
-      <c r="E80" s="245"/>
-      <c r="F80" s="246"/>
+      <c r="A80" s="191"/>
+      <c r="B80" s="188"/>
+      <c r="C80" s="188"/>
+      <c r="D80" s="188"/>
+      <c r="E80" s="188"/>
+      <c r="F80" s="189"/>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="248"/>
-      <c r="B81" s="245"/>
-      <c r="C81" s="245"/>
-      <c r="D81" s="245"/>
-      <c r="E81" s="245"/>
-      <c r="F81" s="246"/>
+      <c r="A81" s="191"/>
+      <c r="B81" s="188"/>
+      <c r="C81" s="188"/>
+      <c r="D81" s="188"/>
+      <c r="E81" s="188"/>
+      <c r="F81" s="189"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="248"/>
-      <c r="B82" s="245"/>
-      <c r="C82" s="245"/>
-      <c r="D82" s="245"/>
-      <c r="E82" s="245"/>
-      <c r="F82" s="246"/>
+      <c r="A82" s="191"/>
+      <c r="B82" s="188"/>
+      <c r="C82" s="188"/>
+      <c r="D82" s="188"/>
+      <c r="E82" s="188"/>
+      <c r="F82" s="189"/>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="248"/>
-      <c r="B83" s="245"/>
-      <c r="C83" s="245"/>
-      <c r="D83" s="245"/>
-      <c r="E83" s="245"/>
-      <c r="F83" s="246"/>
+      <c r="A83" s="191"/>
+      <c r="B83" s="188"/>
+      <c r="C83" s="188"/>
+      <c r="D83" s="188"/>
+      <c r="E83" s="188"/>
+      <c r="F83" s="189"/>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="248"/>
-      <c r="B84" s="245"/>
-      <c r="C84" s="245"/>
-      <c r="D84" s="245"/>
-      <c r="E84" s="245"/>
-      <c r="F84" s="246"/>
+      <c r="A84" s="191"/>
+      <c r="B84" s="188"/>
+      <c r="C84" s="188"/>
+      <c r="D84" s="188"/>
+      <c r="E84" s="188"/>
+      <c r="F84" s="189"/>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="248"/>
-      <c r="B85" s="245"/>
-      <c r="C85" s="245"/>
-      <c r="D85" s="245"/>
-      <c r="E85" s="245"/>
-      <c r="F85" s="246"/>
+      <c r="A85" s="191"/>
+      <c r="B85" s="188"/>
+      <c r="C85" s="188"/>
+      <c r="D85" s="188"/>
+      <c r="E85" s="188"/>
+      <c r="F85" s="189"/>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="248"/>
-      <c r="B86" s="245"/>
-      <c r="C86" s="245"/>
-      <c r="D86" s="245"/>
-      <c r="E86" s="245"/>
-      <c r="F86" s="246"/>
+      <c r="A86" s="191"/>
+      <c r="B86" s="188"/>
+      <c r="C86" s="188"/>
+      <c r="D86" s="188"/>
+      <c r="E86" s="188"/>
+      <c r="F86" s="189"/>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="248"/>
-      <c r="B87" s="245"/>
-      <c r="C87" s="245"/>
-      <c r="D87" s="245"/>
-      <c r="E87" s="245"/>
-      <c r="F87" s="246"/>
+      <c r="A87" s="191"/>
+      <c r="B87" s="188"/>
+      <c r="C87" s="188"/>
+      <c r="D87" s="188"/>
+      <c r="E87" s="188"/>
+      <c r="F87" s="189"/>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="248"/>
-      <c r="B88" s="245"/>
-      <c r="C88" s="245"/>
-      <c r="D88" s="245"/>
-      <c r="E88" s="245"/>
-      <c r="F88" s="246"/>
+      <c r="A88" s="191"/>
+      <c r="B88" s="188"/>
+      <c r="C88" s="188"/>
+      <c r="D88" s="188"/>
+      <c r="E88" s="188"/>
+      <c r="F88" s="189"/>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="248"/>
-      <c r="B89" s="245"/>
-      <c r="C89" s="245"/>
-      <c r="D89" s="245"/>
-      <c r="E89" s="245"/>
-      <c r="F89" s="246"/>
+      <c r="A89" s="191"/>
+      <c r="B89" s="188"/>
+      <c r="C89" s="188"/>
+      <c r="D89" s="188"/>
+      <c r="E89" s="188"/>
+      <c r="F89" s="189"/>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="248"/>
-      <c r="B90" s="245"/>
-      <c r="C90" s="245"/>
-      <c r="D90" s="245"/>
-      <c r="E90" s="245"/>
-      <c r="F90" s="246"/>
+      <c r="A90" s="191"/>
+      <c r="B90" s="188"/>
+      <c r="C90" s="188"/>
+      <c r="D90" s="188"/>
+      <c r="E90" s="188"/>
+      <c r="F90" s="189"/>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="248"/>
-      <c r="B91" s="245"/>
-      <c r="C91" s="245"/>
-      <c r="D91" s="245"/>
-      <c r="E91" s="245"/>
-      <c r="F91" s="246"/>
+      <c r="A91" s="191"/>
+      <c r="B91" s="188"/>
+      <c r="C91" s="188"/>
+      <c r="D91" s="188"/>
+      <c r="E91" s="188"/>
+      <c r="F91" s="189"/>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="248"/>
-      <c r="B92" s="245"/>
-      <c r="C92" s="245"/>
-      <c r="D92" s="245"/>
-      <c r="E92" s="245"/>
-      <c r="F92" s="246"/>
+      <c r="A92" s="191"/>
+      <c r="B92" s="188"/>
+      <c r="C92" s="188"/>
+      <c r="D92" s="188"/>
+      <c r="E92" s="188"/>
+      <c r="F92" s="189"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="248"/>
-      <c r="B93" s="245"/>
-      <c r="C93" s="245"/>
-      <c r="D93" s="245"/>
-      <c r="E93" s="245"/>
-      <c r="F93" s="246"/>
+      <c r="A93" s="191"/>
+      <c r="B93" s="188"/>
+      <c r="C93" s="188"/>
+      <c r="D93" s="188"/>
+      <c r="E93" s="188"/>
+      <c r="F93" s="189"/>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="248"/>
-      <c r="B94" s="245"/>
-      <c r="C94" s="245"/>
-      <c r="D94" s="245"/>
-      <c r="E94" s="245"/>
-      <c r="F94" s="246"/>
+      <c r="A94" s="191"/>
+      <c r="B94" s="188"/>
+      <c r="C94" s="188"/>
+      <c r="D94" s="188"/>
+      <c r="E94" s="188"/>
+      <c r="F94" s="189"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="248"/>
-      <c r="B95" s="245"/>
-      <c r="C95" s="245"/>
-      <c r="D95" s="245"/>
-      <c r="E95" s="245"/>
-      <c r="F95" s="246"/>
+      <c r="A95" s="191"/>
+      <c r="B95" s="188"/>
+      <c r="C95" s="188"/>
+      <c r="D95" s="188"/>
+      <c r="E95" s="188"/>
+      <c r="F95" s="189"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A96" s="249"/>
-      <c r="B96" s="250"/>
-      <c r="C96" s="250"/>
-      <c r="D96" s="250"/>
-      <c r="E96" s="250"/>
-      <c r="F96" s="253"/>
+      <c r="A96" s="192"/>
+      <c r="B96" s="193"/>
+      <c r="C96" s="193"/>
+      <c r="D96" s="193"/>
+      <c r="E96" s="193"/>
+      <c r="F96" s="196"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="275"/>
+      <c r="B99" s="276"/>
+      <c r="C99" s="276"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="276"/>
+      <c r="B100" s="276"/>
+      <c r="C100" s="276"/>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="276"/>
+      <c r="B101" s="276"/>
+      <c r="C101" s="276"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="D58:D60"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="D59:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11962,28 +11991,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="229" t="s">
         <v>893</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="226" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="198"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="23"/>
@@ -12234,16 +12263,16 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="226" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="197"/>
-      <c r="C15" s="197"/>
-      <c r="D15" s="197"/>
-      <c r="E15" s="197"/>
-      <c r="F15" s="197"/>
-      <c r="G15" s="197"/>
-      <c r="H15" s="198"/>
+      <c r="B15" s="227"/>
+      <c r="C15" s="227"/>
+      <c r="D15" s="227"/>
+      <c r="E15" s="227"/>
+      <c r="F15" s="227"/>
+      <c r="G15" s="227"/>
+      <c r="H15" s="228"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="28"/>
@@ -12526,16 +12555,16 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="196" t="s">
+      <c r="A28" s="226" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="197"/>
-      <c r="C28" s="197"/>
-      <c r="D28" s="197"/>
-      <c r="E28" s="197"/>
-      <c r="F28" s="197"/>
-      <c r="G28" s="197"/>
-      <c r="H28" s="198"/>
+      <c r="B28" s="227"/>
+      <c r="C28" s="227"/>
+      <c r="D28" s="227"/>
+      <c r="E28" s="227"/>
+      <c r="F28" s="227"/>
+      <c r="G28" s="227"/>
+      <c r="H28" s="228"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="23"/>
@@ -12808,12 +12837,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="229" t="s">
         <v>826</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="41"/>
@@ -13020,28 +13049,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="230" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="230"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="226" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="198"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="29" t="s">
@@ -13328,12 +13357,12 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="226" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="197"/>
-      <c r="C15" s="197"/>
-      <c r="D15" s="198"/>
+      <c r="B15" s="227"/>
+      <c r="C15" s="227"/>
+      <c r="D15" s="228"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -13512,12 +13541,12 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="196" t="s">
+      <c r="A28" s="226" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="197"/>
-      <c r="C28" s="197"/>
-      <c r="D28" s="198"/>
+      <c r="B28" s="227"/>
+      <c r="C28" s="227"/>
+      <c r="D28" s="228"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -13715,36 +13744,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="231" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="202"/>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
+      <c r="A2" s="232"/>
+      <c r="B2" s="232"/>
+      <c r="C2" s="232"/>
+      <c r="D2" s="232"/>
+      <c r="E2" s="232"/>
+      <c r="F2" s="232"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="233" t="s">
         <v>595</v>
       </c>
-      <c r="B3" s="204"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="203" t="s">
+      <c r="B3" s="234"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="233" t="s">
         <v>596</v>
       </c>
-      <c r="E3" s="204"/>
-      <c r="F3" s="205"/>
+      <c r="E3" s="234"/>
+      <c r="F3" s="235"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="52">
@@ -14289,22 +14318,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="237" t="s">
         <v>567</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
+      <c r="B1" s="237"/>
+      <c r="C1" s="237"/>
+      <c r="D1" s="237"/>
+      <c r="E1" s="237"/>
+      <c r="F1" s="237"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="206" t="s">
+      <c r="B2" s="236" t="s">
         <v>588</v>
       </c>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="206"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="41"/>
@@ -14409,12 +14438,12 @@
       <c r="E10" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="206" t="s">
+      <c r="B14" s="236" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="206"/>
-      <c r="D14" s="206"/>
-      <c r="E14" s="206"/>
+      <c r="C14" s="236"/>
+      <c r="D14" s="236"/>
+      <c r="E14" s="236"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="41"/>
@@ -14541,42 +14570,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="238" t="s">
         <v>854</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="210"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="240"/>
       <c r="I1" s="57"/>
       <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="211"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="213"/>
+      <c r="A2" s="241"/>
+      <c r="B2" s="242"/>
+      <c r="C2" s="242"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
+      <c r="G2" s="242"/>
+      <c r="H2" s="243"/>
     </row>
     <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="244" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="215"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="214" t="s">
+      <c r="B3" s="245"/>
+      <c r="C3" s="246"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="244" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="215"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="217"/>
+      <c r="F3" s="245"/>
+      <c r="G3" s="246"/>
+      <c r="H3" s="247"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="117">

</xml_diff>

<commit_message>
chg: Updated A-10 presets
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="930">
   <si>
     <t>AWACS</t>
   </si>
@@ -3302,9 +3302,6 @@
     <t>BACKUP</t>
   </si>
   <si>
-    <t>A-10C presets Advanced Training mission (ATRM) V1.0</t>
-  </si>
-  <si>
     <t>AR 202</t>
   </si>
   <si>
@@ -3390,6 +3387,30 @@
   </si>
   <si>
     <t>124.8</t>
+  </si>
+  <si>
+    <t>A-10C presets Advanced Training mission (ATRM) V1.1</t>
+  </si>
+  <si>
+    <t>SILVER 1</t>
+  </si>
+  <si>
+    <t>BRONCE 7</t>
+  </si>
+  <si>
+    <t>RANGE 12 SEC</t>
+  </si>
+  <si>
+    <t>COPPER 10</t>
+  </si>
+  <si>
+    <t>RANGE 14 SEC</t>
+  </si>
+  <si>
+    <t>RANGE 12 PRI</t>
+  </si>
+  <si>
+    <t>RANGE 14 PRI</t>
   </si>
 </sst>
 </file>
@@ -4830,12 +4851,44 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4854,27 +4907,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4884,15 +4916,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4965,6 +4988,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4974,15 +5033,6 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5013,35 +5063,6 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5691,11 +5712,11 @@
       </c>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="R3" s="223" t="s">
+      <c r="R3" s="207" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="224"/>
-      <c r="T3" s="225"/>
+      <c r="S3" s="208"/>
+      <c r="T3" s="209"/>
       <c r="V3" s="9" t="s">
         <v>3</v>
       </c>
@@ -5747,11 +5768,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="46"/>
-      <c r="R4" s="214" t="s">
+      <c r="R4" s="212" t="s">
         <v>690</v>
       </c>
-      <c r="S4" s="215"/>
-      <c r="T4" s="216"/>
+      <c r="S4" s="213"/>
+      <c r="T4" s="214"/>
       <c r="V4" s="9" t="s">
         <v>4</v>
       </c>
@@ -5761,16 +5782,16 @@
       <c r="X4" s="35" t="s">
         <v>338</v>
       </c>
-      <c r="Z4" s="206" t="s">
+      <c r="Z4" s="210" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="206"/>
-      <c r="AB4" s="206"/>
-      <c r="AD4" s="206" t="s">
+      <c r="AA4" s="210"/>
+      <c r="AB4" s="210"/>
+      <c r="AD4" s="210" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="206"/>
-      <c r="AF4" s="206"/>
+      <c r="AE4" s="210"/>
+      <c r="AF4" s="210"/>
     </row>
     <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
@@ -6245,11 +6266,11 @@
       <c r="X11" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="Z11" s="206" t="s">
+      <c r="Z11" s="210" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="206"/>
-      <c r="AB11" s="206"/>
+      <c r="AA11" s="210"/>
+      <c r="AB11" s="210"/>
     </row>
     <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
@@ -6624,16 +6645,16 @@
         <v>382</v>
       </c>
       <c r="Q17" s="5"/>
-      <c r="R17" s="217" t="s">
+      <c r="R17" s="215" t="s">
         <v>700</v>
       </c>
-      <c r="S17" s="218"/>
-      <c r="T17" s="219"/>
+      <c r="S17" s="216"/>
+      <c r="T17" s="217"/>
       <c r="V17" s="54" t="s">
+        <v>901</v>
+      </c>
+      <c r="W17" t="s">
         <v>902</v>
-      </c>
-      <c r="W17" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="18" spans="2:32" ht="15.75" thickBot="1">
@@ -6689,13 +6710,13 @@
         <v>417</v>
       </c>
       <c r="V18" s="54" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="W18" s="4" t="s">
         <v>195</v>
       </c>
       <c r="X18" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="19" spans="2:32">
@@ -6743,25 +6764,25 @@
         <v>314</v>
       </c>
       <c r="Q19" s="5"/>
-      <c r="R19" s="214" t="s">
+      <c r="R19" s="212" t="s">
         <v>691</v>
       </c>
-      <c r="S19" s="215"/>
-      <c r="T19" s="216"/>
-      <c r="V19" s="207" t="s">
+      <c r="S19" s="213"/>
+      <c r="T19" s="214"/>
+      <c r="V19" s="219" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="208"/>
-      <c r="X19" s="208"/>
-      <c r="Y19" s="208"/>
-      <c r="Z19" s="209"/>
-      <c r="AB19" s="206" t="s">
+      <c r="W19" s="220"/>
+      <c r="X19" s="220"/>
+      <c r="Y19" s="220"/>
+      <c r="Z19" s="221"/>
+      <c r="AB19" s="210" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="206"/>
-      <c r="AD19" s="206"/>
-      <c r="AE19" s="206"/>
-      <c r="AF19" s="206"/>
+      <c r="AC19" s="210"/>
+      <c r="AD19" s="210"/>
+      <c r="AE19" s="210"/>
+      <c r="AF19" s="210"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -7060,13 +7081,13 @@
         <v>857</v>
       </c>
       <c r="V23" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="W23" t="s">
         <v>475</v>
       </c>
       <c r="X23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="Y23" t="s">
         <v>739</v>
@@ -7411,31 +7432,31 @@
       <c r="Z30" t="s">
         <v>852</v>
       </c>
-      <c r="AC30" s="206" t="s">
+      <c r="AC30" s="210" t="s">
         <v>575</v>
       </c>
-      <c r="AD30" s="206"/>
-      <c r="AE30" s="206"/>
+      <c r="AD30" s="210"/>
+      <c r="AE30" s="210"/>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="206" t="s">
+      <c r="B31" s="210" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="206"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="J31" s="206" t="s">
+      <c r="C31" s="210"/>
+      <c r="D31" s="210"/>
+      <c r="E31" s="210"/>
+      <c r="F31" s="210"/>
+      <c r="G31" s="210"/>
+      <c r="H31" s="210"/>
+      <c r="J31" s="210" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="206"/>
-      <c r="L31" s="206"/>
-      <c r="M31" s="206"/>
-      <c r="N31" s="206"/>
-      <c r="O31" s="206"/>
-      <c r="P31" s="206"/>
+      <c r="K31" s="210"/>
+      <c r="L31" s="210"/>
+      <c r="M31" s="210"/>
+      <c r="N31" s="210"/>
+      <c r="O31" s="210"/>
+      <c r="P31" s="210"/>
       <c r="R31" s="95"/>
       <c r="S31" s="95"/>
       <c r="T31" s="95"/>
@@ -7512,19 +7533,19 @@
       <c r="T32" s="95"/>
       <c r="U32" s="163"/>
       <c r="V32" s="125" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="W32" s="126" t="s">
         <v>475</v>
       </c>
       <c r="X32" s="199" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Y32" s="126" t="s">
         <v>740</v>
       </c>
       <c r="Z32" s="200" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="AA32" s="163"/>
       <c r="AC32" s="9"/>
@@ -7573,19 +7594,19 @@
       <c r="S33" s="95"/>
       <c r="T33" s="95"/>
       <c r="V33" s="154" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="W33" s="155" t="s">
         <v>425</v>
       </c>
       <c r="X33" s="204" t="s">
+        <v>916</v>
+      </c>
+      <c r="Y33" s="155" t="s">
         <v>917</v>
       </c>
-      <c r="Y33" s="155" t="s">
+      <c r="Z33" s="134" t="s">
         <v>918</v>
-      </c>
-      <c r="Z33" s="134" t="s">
-        <v>919</v>
       </c>
       <c r="AC33" s="9"/>
       <c r="AD33" s="62" t="s">
@@ -7629,9 +7650,9 @@
       <c r="P34" t="s">
         <v>404</v>
       </c>
-      <c r="R34" s="213"/>
-      <c r="S34" s="213"/>
-      <c r="T34" s="213"/>
+      <c r="R34" s="211"/>
+      <c r="S34" s="211"/>
+      <c r="T34" s="211"/>
       <c r="AC34" s="9"/>
       <c r="AD34" s="62" t="s">
         <v>116</v>
@@ -7722,15 +7743,15 @@
       <c r="R36" s="93"/>
       <c r="S36" s="93"/>
       <c r="T36" s="95"/>
-      <c r="U36" s="212" t="s">
+      <c r="U36" s="224" t="s">
         <v>671</v>
       </c>
-      <c r="V36" s="212"/>
-      <c r="W36" s="212"/>
-      <c r="X36" s="212"/>
-      <c r="Y36" s="212"/>
-      <c r="Z36" s="212"/>
-      <c r="AA36" s="212"/>
+      <c r="V36" s="224"/>
+      <c r="W36" s="224"/>
+      <c r="X36" s="224"/>
+      <c r="Y36" s="224"/>
+      <c r="Z36" s="224"/>
+      <c r="AA36" s="224"/>
       <c r="AC36" s="9" t="s">
         <v>587</v>
       </c>
@@ -7875,20 +7896,20 @@
       <c r="H39" t="s">
         <v>390</v>
       </c>
-      <c r="J39" s="205" t="s">
+      <c r="J39" s="218" t="s">
         <v>401</v>
       </c>
-      <c r="K39" s="205"/>
-      <c r="L39" s="205"/>
-      <c r="M39" s="205"/>
-      <c r="N39" s="205"/>
-      <c r="O39" s="205"/>
-      <c r="P39" s="205"/>
+      <c r="K39" s="218"/>
+      <c r="L39" s="218"/>
+      <c r="M39" s="218"/>
+      <c r="N39" s="218"/>
+      <c r="O39" s="218"/>
+      <c r="P39" s="218"/>
       <c r="R39" s="95"/>
       <c r="S39" s="93"/>
       <c r="T39" s="95"/>
       <c r="V39" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="W39" t="s">
         <v>719</v>
@@ -7923,7 +7944,7 @@
       <c r="S40" s="93"/>
       <c r="T40" s="95"/>
       <c r="V40" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="W40" t="s">
         <v>720</v>
@@ -7972,13 +7993,13 @@
       <c r="AA41" t="s">
         <v>414</v>
       </c>
-      <c r="AC41" s="210" t="s">
+      <c r="AC41" s="222" t="s">
         <v>769</v>
       </c>
-      <c r="AD41" s="211"/>
-      <c r="AE41" s="211"/>
-      <c r="AF41" s="211"/>
-      <c r="AG41" s="211"/>
+      <c r="AD41" s="223"/>
+      <c r="AE41" s="223"/>
+      <c r="AF41" s="223"/>
+      <c r="AG41" s="223"/>
     </row>
     <row r="42" spans="2:33">
       <c r="E42" s="14" t="s">
@@ -8078,11 +8099,11 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="217" t="s">
+      <c r="Q45" s="215" t="s">
         <v>640</v>
       </c>
-      <c r="R45" s="218"/>
-      <c r="S45" s="219"/>
+      <c r="R45" s="216"/>
+      <c r="S45" s="217"/>
       <c r="T45" s="39"/>
       <c r="W45" t="s">
         <v>719</v>
@@ -8108,7 +8129,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="220" t="s">
+      <c r="Q46" s="225" t="s">
         <v>690</v>
       </c>
       <c r="R46" s="97" t="s">
@@ -8140,7 +8161,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="221"/>
+      <c r="Q47" s="226"/>
       <c r="R47" s="9" t="s">
         <v>654</v>
       </c>
@@ -8149,7 +8170,7 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q48" s="222"/>
+      <c r="Q48" s="227"/>
       <c r="R48" s="83" t="s">
         <v>655</v>
       </c>
@@ -8159,7 +8180,7 @@
       <c r="T48" s="39"/>
     </row>
     <row r="49" spans="17:35">
-      <c r="Q49" s="220" t="s">
+      <c r="Q49" s="225" t="s">
         <v>691</v>
       </c>
       <c r="R49" s="97" t="s">
@@ -8177,7 +8198,7 @@
       <c r="Y49" s="158"/>
     </row>
     <row r="50" spans="17:35">
-      <c r="Q50" s="221"/>
+      <c r="Q50" s="226"/>
       <c r="R50" s="9" t="s">
         <v>656</v>
       </c>
@@ -8201,7 +8222,7 @@
       </c>
     </row>
     <row r="51" spans="17:35" ht="15.75" thickBot="1">
-      <c r="Q51" s="222"/>
+      <c r="Q51" s="227"/>
       <c r="R51" s="83" t="s">
         <v>657</v>
       </c>
@@ -8223,15 +8244,15 @@
       <c r="Y51" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="AC51" s="206" t="s">
+      <c r="AC51" s="210" t="s">
         <v>616</v>
       </c>
-      <c r="AD51" s="206"/>
-      <c r="AE51" s="206"/>
-      <c r="AF51" s="206"/>
-      <c r="AG51" s="206"/>
-      <c r="AH51" s="206"/>
-      <c r="AI51" s="206"/>
+      <c r="AD51" s="210"/>
+      <c r="AE51" s="210"/>
+      <c r="AF51" s="210"/>
+      <c r="AG51" s="210"/>
+      <c r="AH51" s="210"/>
+      <c r="AI51" s="210"/>
     </row>
     <row r="52" spans="17:35">
       <c r="U52" s="76">
@@ -8615,15 +8636,15 @@
       <c r="Y64" t="s">
         <v>856</v>
       </c>
-      <c r="AC64" s="206" t="s">
+      <c r="AC64" s="210" t="s">
         <v>669</v>
       </c>
-      <c r="AD64" s="206"/>
-      <c r="AE64" s="206"/>
-      <c r="AF64" s="206"/>
-      <c r="AG64" s="206"/>
-      <c r="AH64" s="206"/>
-      <c r="AI64" s="206"/>
+      <c r="AD64" s="210"/>
+      <c r="AE64" s="210"/>
+      <c r="AF64" s="210"/>
+      <c r="AG64" s="210"/>
+      <c r="AH64" s="210"/>
+      <c r="AI64" s="210"/>
     </row>
     <row r="65" spans="21:35">
       <c r="AC65" s="16" t="s">
@@ -8805,7 +8826,7 @@
     </row>
     <row r="74" spans="21:35">
       <c r="U74" s="114" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="75" spans="21:35">
@@ -8825,14 +8846,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="AC64:AI64"/>
     <mergeCell ref="AC51:AI51"/>
@@ -8846,6 +8859,14 @@
     <mergeCell ref="Q46:Q48"/>
     <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="J31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8895,40 +8916,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="248" t="s">
+      <c r="A1" s="250" t="s">
         <v>771</v>
       </c>
-      <c r="B1" s="248"/>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="248"/>
-      <c r="G1" s="248"/>
-      <c r="H1" s="248"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="249"/>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249"/>
-      <c r="H2" s="249"/>
+      <c r="A2" s="251"/>
+      <c r="B2" s="251"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="246" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="247"/>
-      <c r="E3" s="244" t="s">
+      <c r="B3" s="247"/>
+      <c r="C3" s="248"/>
+      <c r="D3" s="249"/>
+      <c r="E3" s="246" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="245"/>
-      <c r="G3" s="246"/>
-      <c r="H3" s="247"/>
+      <c r="F3" s="247"/>
+      <c r="G3" s="248"/>
+      <c r="H3" s="249"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="113">
@@ -9449,7 +9470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A98" sqref="A98:A100"/>
     </sheetView>
   </sheetViews>
@@ -9463,33 +9484,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A1" s="272" t="s">
-        <v>921</v>
-      </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="274"/>
+      <c r="A1" s="257" t="s">
+        <v>920</v>
+      </c>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
+      <c r="F1" s="259"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="253" t="s">
+      <c r="A2" s="252" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="254"/>
-      <c r="C2" s="254"/>
-      <c r="D2" s="269" t="s">
+      <c r="B2" s="253"/>
+      <c r="C2" s="253"/>
+      <c r="D2" s="254" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="270"/>
-      <c r="F2" s="271"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="256"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="256" t="s">
-        <v>912</v>
-      </c>
-      <c r="B3" s="257"/>
-      <c r="C3" s="258"/>
+      <c r="A3" s="267" t="s">
+        <v>911</v>
+      </c>
+      <c r="B3" s="268"/>
+      <c r="C3" s="269"/>
       <c r="D3" s="197" t="s">
         <v>2</v>
       </c>
@@ -9763,10 +9784,10 @@
         <v>417</v>
       </c>
       <c r="D17" s="154" t="s">
+        <v>901</v>
+      </c>
+      <c r="E17" s="155" t="s">
         <v>902</v>
-      </c>
-      <c r="E17" s="155" t="s">
-        <v>903</v>
       </c>
       <c r="F17" s="134"/>
     </row>
@@ -9780,11 +9801,11 @@
       <c r="C18" s="140" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="253" t="s">
-        <v>904</v>
-      </c>
-      <c r="E18" s="254"/>
-      <c r="F18" s="255"/>
+      <c r="D18" s="252" t="s">
+        <v>903</v>
+      </c>
+      <c r="E18" s="253"/>
+      <c r="F18" s="260"/>
     </row>
     <row r="19" spans="1:18" ht="15.75">
       <c r="A19" s="137">
@@ -9796,7 +9817,7 @@
       <c r="C19" s="142" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="266" t="s">
+      <c r="D19" s="261" t="s">
         <v>690</v>
       </c>
       <c r="E19" s="138" t="s">
@@ -9816,7 +9837,7 @@
       <c r="C20" s="142" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="267"/>
+      <c r="D20" s="262"/>
       <c r="E20" s="124" t="s">
         <v>654</v>
       </c>
@@ -9837,7 +9858,7 @@
       <c r="C21" s="142" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="268"/>
+      <c r="D21" s="263"/>
       <c r="E21" s="150" t="s">
         <v>655</v>
       </c>
@@ -10057,13 +10078,13 @@
       <c r="F35" s="189"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A36" s="250" t="s">
-        <v>905</v>
-      </c>
-      <c r="B36" s="251"/>
-      <c r="C36" s="251"/>
-      <c r="D36" s="251"/>
-      <c r="E36" s="252"/>
+      <c r="A36" s="264" t="s">
+        <v>904</v>
+      </c>
+      <c r="B36" s="265"/>
+      <c r="C36" s="265"/>
+      <c r="D36" s="265"/>
+      <c r="E36" s="266"/>
       <c r="F36" s="190"/>
     </row>
     <row r="37" spans="1:6">
@@ -10122,43 +10143,43 @@
     </row>
     <row r="40" spans="1:6" ht="15.75">
       <c r="A40" s="120" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B40" s="124" t="s">
         <v>475</v>
       </c>
       <c r="C40" s="164" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D40" s="124" t="s">
         <v>740</v>
       </c>
       <c r="E40" s="130" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F40" s="190"/>
     </row>
     <row r="41" spans="1:6" ht="15.75">
       <c r="A41" s="125" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B41" s="126" t="s">
         <v>475</v>
       </c>
       <c r="C41" s="199" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D41" s="126" t="s">
         <v>740</v>
       </c>
       <c r="E41" s="200" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F41" s="190"/>
     </row>
     <row r="42" spans="1:6" ht="15.75">
       <c r="A42" s="181" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B42" s="201" t="s">
         <v>425</v>
@@ -10230,19 +10251,19 @@
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1">
       <c r="A46" s="154" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B46" s="155" t="s">
         <v>425</v>
       </c>
       <c r="C46" s="204" t="s">
+        <v>916</v>
+      </c>
+      <c r="D46" s="155" t="s">
         <v>917</v>
       </c>
-      <c r="D46" s="155" t="s">
+      <c r="E46" s="134" t="s">
         <v>918</v>
-      </c>
-      <c r="E46" s="134" t="s">
-        <v>919</v>
       </c>
       <c r="F46" s="190"/>
     </row>
@@ -10255,37 +10276,37 @@
       <c r="F47" s="194"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A48" s="259" t="s">
-        <v>921</v>
-      </c>
-      <c r="B48" s="260"/>
-      <c r="C48" s="260"/>
-      <c r="D48" s="261"/>
-      <c r="E48" s="261"/>
-      <c r="F48" s="262"/>
+      <c r="A48" s="270" t="s">
+        <v>920</v>
+      </c>
+      <c r="B48" s="271"/>
+      <c r="C48" s="271"/>
+      <c r="D48" s="272"/>
+      <c r="E48" s="272"/>
+      <c r="F48" s="273"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="191"/>
       <c r="B49" s="188"/>
       <c r="C49" s="188"/>
-      <c r="D49" s="263" t="s">
-        <v>907</v>
-      </c>
-      <c r="E49" s="264"/>
-      <c r="F49" s="265"/>
+      <c r="D49" s="274" t="s">
+        <v>906</v>
+      </c>
+      <c r="E49" s="275"/>
+      <c r="F49" s="276"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="191"/>
       <c r="B50" s="188"/>
       <c r="C50" s="188"/>
       <c r="D50" s="120" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E50" s="120" t="s">
         <v>195</v>
       </c>
       <c r="F50" s="195" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1">
@@ -10304,11 +10325,11 @@
       <c r="A52" s="191"/>
       <c r="B52" s="188"/>
       <c r="C52" s="188"/>
-      <c r="D52" s="253" t="s">
+      <c r="D52" s="252" t="s">
         <v>858</v>
       </c>
-      <c r="E52" s="254"/>
-      <c r="F52" s="255"/>
+      <c r="E52" s="253"/>
+      <c r="F52" s="260"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="191"/>
@@ -10343,13 +10364,13 @@
       <c r="B55" s="188"/>
       <c r="C55" s="188"/>
       <c r="D55" s="120" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E55" s="120" t="s">
         <v>675</v>
       </c>
       <c r="F55" s="195" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -10384,17 +10405,17 @@
       <c r="A58" s="191"/>
       <c r="B58" s="188"/>
       <c r="C58" s="188"/>
-      <c r="D58" s="253" t="s">
-        <v>911</v>
-      </c>
-      <c r="E58" s="254"/>
-      <c r="F58" s="255"/>
+      <c r="D58" s="252" t="s">
+        <v>910</v>
+      </c>
+      <c r="E58" s="253"/>
+      <c r="F58" s="260"/>
     </row>
     <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="191"/>
       <c r="B59" s="188"/>
       <c r="C59" s="188"/>
-      <c r="D59" s="266" t="s">
+      <c r="D59" s="261" t="s">
         <v>691</v>
       </c>
       <c r="E59" s="138" t="s">
@@ -10408,7 +10429,7 @@
       <c r="A60" s="191"/>
       <c r="B60" s="188"/>
       <c r="C60" s="188"/>
-      <c r="D60" s="267"/>
+      <c r="D60" s="262"/>
       <c r="E60" s="124" t="s">
         <v>656</v>
       </c>
@@ -10420,7 +10441,7 @@
       <c r="A61" s="191"/>
       <c r="B61" s="188"/>
       <c r="C61" s="188"/>
-      <c r="D61" s="268"/>
+      <c r="D61" s="263"/>
       <c r="E61" s="150" t="s">
         <v>657</v>
       </c>
@@ -10443,13 +10464,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A63" s="250" t="s">
-        <v>906</v>
-      </c>
-      <c r="B63" s="251"/>
-      <c r="C63" s="251"/>
-      <c r="D63" s="251"/>
-      <c r="E63" s="252"/>
+      <c r="A63" s="264" t="s">
+        <v>905</v>
+      </c>
+      <c r="B63" s="265"/>
+      <c r="C63" s="265"/>
+      <c r="D63" s="265"/>
+      <c r="E63" s="266"/>
       <c r="F63" s="189"/>
     </row>
     <row r="64" spans="1:6" ht="15.75">
@@ -10757,27 +10778,22 @@
       <c r="F96" s="196"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="275"/>
-      <c r="B99" s="276"/>
-      <c r="C99" s="276"/>
+      <c r="A99" s="205"/>
+      <c r="B99" s="206"/>
+      <c r="C99" s="206"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="276"/>
-      <c r="B100" s="276"/>
-      <c r="C100" s="276"/>
+      <c r="A100" s="206"/>
+      <c r="B100" s="206"/>
+      <c r="C100" s="206"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="276"/>
-      <c r="B101" s="276"/>
-      <c r="C101" s="276"/>
+      <c r="A101" s="206"/>
+      <c r="B101" s="206"/>
+      <c r="C101" s="206"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:D21"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="A3:C3"/>
@@ -10786,6 +10802,11 @@
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="D59:D61"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10930,7 +10951,7 @@
         <v>635</v>
       </c>
       <c r="I6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="J6" t="s">
         <v>367</v>
@@ -11978,8 +11999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11991,28 +12012,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="229" t="s">
-        <v>893</v>
-      </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
+      <c r="A1" s="231" t="s">
+        <v>922</v>
+      </c>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="231"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="226" t="s">
+      <c r="A2" s="228" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="227"/>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
-      <c r="H2" s="228"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="23"/>
@@ -12091,8 +12112,8 @@
       <c r="B6" s="27" t="s">
         <v>871</v>
       </c>
-      <c r="C6" s="159" t="s">
-        <v>417</v>
+      <c r="C6" s="159">
+        <v>127.1</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="24">
@@ -12125,8 +12146,12 @@
       <c r="F7" s="27" t="s">
         <v>874</v>
       </c>
-      <c r="G7" s="159"/>
-      <c r="H7" s="26"/>
+      <c r="G7" s="159">
+        <v>127.75</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="24">
@@ -12145,8 +12170,12 @@
       <c r="F8" s="27" t="s">
         <v>876</v>
       </c>
-      <c r="G8" s="159"/>
-      <c r="H8" s="26"/>
+      <c r="G8" s="159">
+        <v>131.69999999999999</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="24">
@@ -12165,8 +12194,12 @@
       <c r="F9" s="27" t="s">
         <v>878</v>
       </c>
-      <c r="G9" s="159"/>
-      <c r="H9" s="26"/>
+      <c r="G9" s="159">
+        <v>132.69999999999999</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>924</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="24">
@@ -12183,10 +12216,14 @@
         <v>17</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="G10" s="159"/>
-      <c r="H10" s="26"/>
+        <v>925</v>
+      </c>
+      <c r="G10" s="159">
+        <v>133.69999999999999</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="24">
@@ -12203,10 +12240,14 @@
         <v>18</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="G11" s="159"/>
-      <c r="H11" s="26"/>
+        <v>927</v>
+      </c>
+      <c r="G11" s="159">
+        <v>121.25</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="24">
@@ -12263,16 +12304,16 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="226" t="s">
+      <c r="A15" s="228" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="227"/>
-      <c r="C15" s="227"/>
-      <c r="D15" s="227"/>
-      <c r="E15" s="227"/>
-      <c r="F15" s="227"/>
-      <c r="G15" s="227"/>
-      <c r="H15" s="228"/>
+      <c r="B15" s="229"/>
+      <c r="C15" s="229"/>
+      <c r="D15" s="229"/>
+      <c r="E15" s="229"/>
+      <c r="F15" s="229"/>
+      <c r="G15" s="229"/>
+      <c r="H15" s="230"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="28"/>
@@ -12303,8 +12344,8 @@
       <c r="B17" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="160" t="s">
-        <v>25</v>
+      <c r="C17" s="159">
+        <v>237</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>337</v>
@@ -12315,7 +12356,7 @@
       <c r="F17" s="27" t="s">
         <v>882</v>
       </c>
-      <c r="G17" s="160">
+      <c r="G17" s="159">
         <v>228.75</v>
       </c>
       <c r="H17" s="26" t="s">
@@ -12329,8 +12370,8 @@
       <c r="B18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="160" t="s">
-        <v>38</v>
+      <c r="C18" s="159">
+        <v>229</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>336</v>
@@ -12339,10 +12380,14 @@
         <v>12</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="G18" s="160"/>
-      <c r="H18" s="26"/>
+        <v>928</v>
+      </c>
+      <c r="G18" s="159">
+        <v>242.25</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="24">
@@ -12351,8 +12396,8 @@
       <c r="B19" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="160" t="s">
-        <v>80</v>
+      <c r="C19" s="159">
+        <v>228</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>339</v>
@@ -12361,10 +12406,14 @@
         <v>13</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="G19" s="160"/>
-      <c r="H19" s="26"/>
+        <v>929</v>
+      </c>
+      <c r="G19" s="159">
+        <v>237.75</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15.75">
       <c r="A20" s="24">
@@ -12373,8 +12422,8 @@
       <c r="B20" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="160" t="s">
-        <v>270</v>
+      <c r="C20" s="159">
+        <v>234</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>345</v>
@@ -12385,7 +12434,7 @@
       <c r="F20" s="27" t="s">
         <v>754</v>
       </c>
-      <c r="G20" s="160">
+      <c r="G20" s="159">
         <v>246.25</v>
       </c>
       <c r="H20" s="26" t="s">
@@ -12399,8 +12448,8 @@
       <c r="B21" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="160" t="s">
-        <v>139</v>
+      <c r="C21" s="159">
+        <v>228.5</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>342</v>
@@ -12411,8 +12460,8 @@
       <c r="F21" s="27" t="s">
         <v>755</v>
       </c>
-      <c r="G21" s="160" t="s">
-        <v>64</v>
+      <c r="G21" s="159">
+        <v>230</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>473</v>
@@ -12425,7 +12474,7 @@
       <c r="B22" s="27" t="s">
         <v>883</v>
       </c>
-      <c r="C22" s="160">
+      <c r="C22" s="159">
         <v>225.75</v>
       </c>
       <c r="D22" s="26" t="s">
@@ -12437,7 +12486,7 @@
       <c r="F22" s="27" t="s">
         <v>614</v>
       </c>
-      <c r="G22" s="160"/>
+      <c r="G22" s="159"/>
       <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" ht="15.75">
@@ -12447,7 +12496,7 @@
       <c r="B23" s="27" t="s">
         <v>884</v>
       </c>
-      <c r="C23" s="160">
+      <c r="C23" s="159">
         <v>235.75</v>
       </c>
       <c r="D23" s="26" t="s">
@@ -12459,8 +12508,8 @@
       <c r="F23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="160" t="s">
-        <v>238</v>
+      <c r="G23" s="159">
+        <v>247.25</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>347</v>
@@ -12473,7 +12522,7 @@
       <c r="B24" s="27" t="s">
         <v>885</v>
       </c>
-      <c r="C24" s="160">
+      <c r="C24" s="159">
         <v>233.25</v>
       </c>
       <c r="D24" s="26" t="s">
@@ -12485,8 +12534,8 @@
       <c r="F24" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="G24" s="160" t="s">
-        <v>151</v>
+      <c r="G24" s="159">
+        <v>228.25</v>
       </c>
       <c r="H24" s="26" t="s">
         <v>468</v>
@@ -12499,7 +12548,7 @@
       <c r="B25" s="27" t="s">
         <v>886</v>
       </c>
-      <c r="C25" s="160">
+      <c r="C25" s="159">
         <v>234.75</v>
       </c>
       <c r="D25" s="26" t="s">
@@ -12511,8 +12560,8 @@
       <c r="F25" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="160" t="s">
-        <v>59</v>
+      <c r="G25" s="159">
+        <v>227.5</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>338</v>
@@ -12525,7 +12574,7 @@
       <c r="B26" s="27" t="s">
         <v>887</v>
       </c>
-      <c r="C26" s="160">
+      <c r="C26" s="159">
         <v>245</v>
       </c>
       <c r="D26" s="26" t="s">
@@ -12537,8 +12586,8 @@
       <c r="F26" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="160" t="s">
-        <v>108</v>
+      <c r="G26" s="159">
+        <v>248</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>340</v>
@@ -12555,16 +12604,16 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="226" t="s">
+      <c r="A28" s="228" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="227"/>
-      <c r="C28" s="227"/>
-      <c r="D28" s="227"/>
-      <c r="E28" s="227"/>
-      <c r="F28" s="227"/>
-      <c r="G28" s="227"/>
-      <c r="H28" s="228"/>
+      <c r="B28" s="229"/>
+      <c r="C28" s="229"/>
+      <c r="D28" s="229"/>
+      <c r="E28" s="229"/>
+      <c r="F28" s="229"/>
+      <c r="G28" s="229"/>
+      <c r="H28" s="230"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="23"/>
@@ -12595,7 +12644,7 @@
       <c r="B30" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="C30" s="160" t="s">
+      <c r="C30" s="159" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="26" t="s">
@@ -12621,7 +12670,7 @@
       <c r="B31" s="27" t="s">
         <v>437</v>
       </c>
-      <c r="C31" s="160" t="s">
+      <c r="C31" s="159" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="26" t="s">
@@ -12647,7 +12696,7 @@
       <c r="B32" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="C32" s="160" t="s">
+      <c r="C32" s="159" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="26" t="s">
@@ -12673,7 +12722,7 @@
       <c r="B33" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="C33" s="160" t="s">
+      <c r="C33" s="159" t="s">
         <v>78</v>
       </c>
       <c r="D33" s="26" t="s">
@@ -12695,7 +12744,7 @@
       <c r="B34" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C34" s="160" t="s">
+      <c r="C34" s="159" t="s">
         <v>126</v>
       </c>
       <c r="D34" s="26" t="s">
@@ -12717,7 +12766,7 @@
       <c r="B35" s="27" t="s">
         <v>441</v>
       </c>
-      <c r="C35" s="160" t="s">
+      <c r="C35" s="159" t="s">
         <v>203</v>
       </c>
       <c r="D35" s="26" t="s">
@@ -12837,12 +12886,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="231" t="s">
         <v>826</v>
       </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="41"/>
@@ -13049,28 +13098,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="232" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
-      <c r="F1" s="230"/>
-      <c r="G1" s="230"/>
-      <c r="H1" s="230"/>
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="226" t="s">
+      <c r="A2" s="228" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="227"/>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
-      <c r="H2" s="228"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="29" t="s">
@@ -13357,12 +13406,12 @@
       <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="226" t="s">
+      <c r="A15" s="228" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="227"/>
-      <c r="C15" s="227"/>
-      <c r="D15" s="228"/>
+      <c r="B15" s="229"/>
+      <c r="C15" s="229"/>
+      <c r="D15" s="230"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -13541,12 +13590,12 @@
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="226" t="s">
+      <c r="A28" s="228" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="227"/>
-      <c r="C28" s="227"/>
-      <c r="D28" s="228"/>
+      <c r="B28" s="229"/>
+      <c r="C28" s="229"/>
+      <c r="D28" s="230"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -13744,36 +13793,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="233" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
       <c r="G1" s="57"/>
       <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="232"/>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
+      <c r="A2" s="234"/>
+      <c r="B2" s="234"/>
+      <c r="C2" s="234"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="235" t="s">
         <v>595</v>
       </c>
-      <c r="B3" s="234"/>
-      <c r="C3" s="235"/>
-      <c r="D3" s="233" t="s">
+      <c r="B3" s="236"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="235" t="s">
         <v>596</v>
       </c>
-      <c r="E3" s="234"/>
-      <c r="F3" s="235"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="237"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="52">
@@ -14318,22 +14367,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="239" t="s">
         <v>567</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="236" t="s">
+      <c r="B2" s="238" t="s">
         <v>588</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="41"/>
@@ -14438,12 +14487,12 @@
       <c r="E10" s="41"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="236" t="s">
+      <c r="B14" s="238" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
+      <c r="C14" s="238"/>
+      <c r="D14" s="238"/>
+      <c r="E14" s="238"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="41"/>
@@ -14570,42 +14619,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="240" t="s">
         <v>854</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="242"/>
       <c r="I1" s="57"/>
       <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="241"/>
-      <c r="B2" s="242"/>
-      <c r="C2" s="242"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242"/>
-      <c r="H2" s="243"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
+      <c r="F2" s="244"/>
+      <c r="G2" s="244"/>
+      <c r="H2" s="245"/>
     </row>
     <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="246" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="247"/>
-      <c r="E3" s="244" t="s">
+      <c r="B3" s="247"/>
+      <c r="C3" s="248"/>
+      <c r="D3" s="249"/>
+      <c r="E3" s="246" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="245"/>
-      <c r="G3" s="246"/>
-      <c r="H3" s="247"/>
+      <c r="F3" s="247"/>
+      <c r="G3" s="248"/>
+      <c r="H3" s="249"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="117">

</xml_diff>

<commit_message>
chg: Added T12.10 , T12.11 and T12.12 to Combatflite
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
-    <sheet name="Callsigns" sheetId="2" r:id="rId2"/>
-    <sheet name="132nd Freqs" sheetId="3" r:id="rId3"/>
-    <sheet name="A10 presets" sheetId="5" r:id="rId4"/>
-    <sheet name="Ka-50 presets" sheetId="6" r:id="rId5"/>
-    <sheet name="MI-8 presets" sheetId="7" r:id="rId6"/>
-    <sheet name="AV-8B Presets" sheetId="8" r:id="rId7"/>
-    <sheet name="AJS-37 Presets" sheetId="10" r:id="rId8"/>
-    <sheet name="FA-18C Presets" sheetId="11" r:id="rId9"/>
-    <sheet name="F-14 Presets" sheetId="12" r:id="rId10"/>
-    <sheet name="F-16 Presets" sheetId="13" r:id="rId11"/>
-    <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId12"/>
-    <sheet name="TACAN and Lasercode" sheetId="15" r:id="rId13"/>
+    <sheet name="TACAN and Lasercode" sheetId="15" r:id="rId2"/>
+    <sheet name="Callsigns" sheetId="2" r:id="rId3"/>
+    <sheet name="132nd Freqs" sheetId="3" r:id="rId4"/>
+    <sheet name="A10 presets" sheetId="5" r:id="rId5"/>
+    <sheet name="Ka-50 presets" sheetId="6" r:id="rId6"/>
+    <sheet name="MI-8 presets" sheetId="7" r:id="rId7"/>
+    <sheet name="AV-8B Presets" sheetId="8" r:id="rId8"/>
+    <sheet name="AJS-37 Presets" sheetId="10" r:id="rId9"/>
+    <sheet name="FA-18C Presets" sheetId="11" r:id="rId10"/>
+    <sheet name="F-14 Presets" sheetId="12" r:id="rId11"/>
+    <sheet name="F-16 Presets" sheetId="13" r:id="rId12"/>
+    <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -5028,18 +5029,68 @@
       <color rgb="FF6600FF"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4097" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000001100000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8991600" y="2682240"/>
+          <a:ext cx="4594860" cy="1363980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5115,7 +5166,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5191,7 +5242,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5267,7 +5318,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5338,64 +5389,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4097" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000001100000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8991600" y="2682240"/>
-          <a:ext cx="4594860" cy="1363980"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5688,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AI77"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9263,6 +9256,605 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" customHeight="1">
+      <c r="A1" s="271" t="s">
+        <v>854</v>
+      </c>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="273"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="274"/>
+      <c r="B2" s="275"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="276"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75">
+      <c r="A3" s="277" t="s">
+        <v>626</v>
+      </c>
+      <c r="B3" s="278"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="277" t="s">
+        <v>627</v>
+      </c>
+      <c r="F3" s="278"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A4" s="115">
+        <v>1</v>
+      </c>
+      <c r="B4" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>620</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>829</v>
+      </c>
+      <c r="E4" s="70">
+        <v>1</v>
+      </c>
+      <c r="F4" s="113" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H4" s="70" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A5" s="115">
+        <v>2</v>
+      </c>
+      <c r="B5" s="113" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>621</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>831</v>
+      </c>
+      <c r="E5" s="70">
+        <v>2</v>
+      </c>
+      <c r="F5" s="113" t="s">
+        <v>853</v>
+      </c>
+      <c r="G5" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A6" s="115">
+        <v>3</v>
+      </c>
+      <c r="B6" s="113" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>832</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>833</v>
+      </c>
+      <c r="E6" s="70">
+        <v>3</v>
+      </c>
+      <c r="F6" s="113" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A7" s="115">
+        <v>4</v>
+      </c>
+      <c r="B7" s="113" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>623</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>835</v>
+      </c>
+      <c r="E7" s="70">
+        <v>4</v>
+      </c>
+      <c r="F7" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>337</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A8" s="115">
+        <v>5</v>
+      </c>
+      <c r="B8" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>624</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>836</v>
+      </c>
+      <c r="E8" s="70">
+        <v>5</v>
+      </c>
+      <c r="F8" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>339</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A9" s="115">
+        <v>6</v>
+      </c>
+      <c r="B9" s="113" t="s">
+        <v>565</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70" t="s">
+        <v>837</v>
+      </c>
+      <c r="E9" s="70">
+        <v>6</v>
+      </c>
+      <c r="F9" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A10" s="115">
+        <v>7</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>818</v>
+      </c>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70" t="s">
+        <v>839</v>
+      </c>
+      <c r="E10" s="70">
+        <v>7</v>
+      </c>
+      <c r="F10" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>756</v>
+      </c>
+      <c r="H10" s="70" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A11" s="115">
+        <v>8</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>841</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>704</v>
+      </c>
+      <c r="E11" s="70">
+        <v>8</v>
+      </c>
+      <c r="F11" s="113" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>757</v>
+      </c>
+      <c r="H11" s="70" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A12" s="115">
+        <v>9</v>
+      </c>
+      <c r="B12" s="113" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>426</v>
+      </c>
+      <c r="E12" s="70">
+        <v>9</v>
+      </c>
+      <c r="F12" s="113" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>473</v>
+      </c>
+      <c r="H12" s="70" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A13" s="115">
+        <v>10</v>
+      </c>
+      <c r="B13" s="113" t="s">
+        <v>217</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>349</v>
+      </c>
+      <c r="D13" s="70" t="s">
+        <v>706</v>
+      </c>
+      <c r="E13" s="70">
+        <v>10</v>
+      </c>
+      <c r="F13" s="113" t="s">
+        <v>747</v>
+      </c>
+      <c r="G13" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H13" s="70" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A14" s="115">
+        <v>11</v>
+      </c>
+      <c r="B14" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>707</v>
+      </c>
+      <c r="E14" s="70">
+        <v>11</v>
+      </c>
+      <c r="F14" s="113" t="s">
+        <v>748</v>
+      </c>
+      <c r="G14" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H14" s="70" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A15" s="115">
+        <v>12</v>
+      </c>
+      <c r="B15" s="113" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>708</v>
+      </c>
+      <c r="E15" s="70">
+        <v>12</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>749</v>
+      </c>
+      <c r="G15" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H15" s="70" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A16" s="115">
+        <v>13</v>
+      </c>
+      <c r="B16" s="113" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>352</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>709</v>
+      </c>
+      <c r="E16" s="70">
+        <v>13</v>
+      </c>
+      <c r="F16" s="113" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="70" t="s">
+        <v>620</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A17" s="115">
+        <v>14</v>
+      </c>
+      <c r="B17" s="113" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>353</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>710</v>
+      </c>
+      <c r="E17" s="70">
+        <v>14</v>
+      </c>
+      <c r="F17" s="113" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>621</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A18" s="115">
+        <v>15</v>
+      </c>
+      <c r="B18" s="113" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>354</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>711</v>
+      </c>
+      <c r="E18" s="70">
+        <v>15</v>
+      </c>
+      <c r="F18" s="113" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>832</v>
+      </c>
+      <c r="H18" s="70" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A19" s="115">
+        <v>16</v>
+      </c>
+      <c r="B19" s="113" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>712</v>
+      </c>
+      <c r="E19" s="70">
+        <v>16</v>
+      </c>
+      <c r="F19" s="113" t="s">
+        <v>210</v>
+      </c>
+      <c r="G19" s="70" t="s">
+        <v>623</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A20" s="115">
+        <v>17</v>
+      </c>
+      <c r="B20" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="70" t="s">
+        <v>649</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>713</v>
+      </c>
+      <c r="E20" s="70">
+        <v>17</v>
+      </c>
+      <c r="F20" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>624</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A21" s="115">
+        <v>18</v>
+      </c>
+      <c r="B21" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>658</v>
+      </c>
+      <c r="D21" s="70" t="s">
+        <v>433</v>
+      </c>
+      <c r="E21" s="70">
+        <v>18</v>
+      </c>
+      <c r="F21" s="113" t="s">
+        <v>270</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>345</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A22" s="115">
+        <v>19</v>
+      </c>
+      <c r="B22" s="113" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>470</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>714</v>
+      </c>
+      <c r="E22" s="70">
+        <v>19</v>
+      </c>
+      <c r="F22" s="113" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="70" t="s">
+        <v>468</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A23" s="115">
+        <v>20</v>
+      </c>
+      <c r="B23" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="D23" s="70" t="s">
+        <v>300</v>
+      </c>
+      <c r="E23" s="70">
+        <v>20</v>
+      </c>
+      <c r="F23" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" s="110" t="s">
+        <v>830</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.75">
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+    </row>
+    <row r="25" spans="1:8" ht="18.75">
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9282,11 +9874,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
@@ -9853,7 +10445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R101"/>
   <sheetViews>
@@ -11192,11 +11784,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -12200,7 +12792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K14"/>
   <sheetViews>
@@ -12425,7 +13017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:O32"/>
   <sheetViews>
@@ -13586,7 +14178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -14460,7 +15052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -14670,7 +15262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -15367,7 +15959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H29"/>
   <sheetViews>
@@ -15941,7 +16533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -16191,603 +16783,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="271" t="s">
-        <v>854</v>
-      </c>
-      <c r="B1" s="272"/>
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="273"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="274"/>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="276"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="277" t="s">
-        <v>626</v>
-      </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="279"/>
-      <c r="D3" s="280"/>
-      <c r="E3" s="277" t="s">
-        <v>627</v>
-      </c>
-      <c r="F3" s="278"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="280"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A4" s="115">
-        <v>1</v>
-      </c>
-      <c r="B4" s="113" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>620</v>
-      </c>
-      <c r="D4" s="70" t="s">
-        <v>829</v>
-      </c>
-      <c r="E4" s="70">
-        <v>1</v>
-      </c>
-      <c r="F4" s="113" t="s">
-        <v>239</v>
-      </c>
-      <c r="G4" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H4" s="70" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A5" s="115">
-        <v>2</v>
-      </c>
-      <c r="B5" s="113" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>621</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>831</v>
-      </c>
-      <c r="E5" s="70">
-        <v>2</v>
-      </c>
-      <c r="F5" s="113" t="s">
-        <v>853</v>
-      </c>
-      <c r="G5" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H5" s="70" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="115">
-        <v>3</v>
-      </c>
-      <c r="B6" s="113" t="s">
-        <v>245</v>
-      </c>
-      <c r="C6" s="70" t="s">
-        <v>832</v>
-      </c>
-      <c r="D6" s="70" t="s">
-        <v>833</v>
-      </c>
-      <c r="E6" s="70">
-        <v>3</v>
-      </c>
-      <c r="F6" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H6" s="70" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A7" s="115">
-        <v>4</v>
-      </c>
-      <c r="B7" s="113" t="s">
-        <v>210</v>
-      </c>
-      <c r="C7" s="70" t="s">
-        <v>623</v>
-      </c>
-      <c r="D7" s="70" t="s">
-        <v>835</v>
-      </c>
-      <c r="E7" s="70">
-        <v>4</v>
-      </c>
-      <c r="F7" s="113" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="70" t="s">
-        <v>337</v>
-      </c>
-      <c r="H7" s="70" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A8" s="115">
-        <v>5</v>
-      </c>
-      <c r="B8" s="113" t="s">
-        <v>262</v>
-      </c>
-      <c r="C8" s="70" t="s">
-        <v>624</v>
-      </c>
-      <c r="D8" s="70" t="s">
-        <v>836</v>
-      </c>
-      <c r="E8" s="70">
-        <v>5</v>
-      </c>
-      <c r="F8" s="113" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>339</v>
-      </c>
-      <c r="H8" s="70" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A9" s="115">
-        <v>6</v>
-      </c>
-      <c r="B9" s="113" t="s">
-        <v>565</v>
-      </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70" t="s">
-        <v>837</v>
-      </c>
-      <c r="E9" s="70">
-        <v>6</v>
-      </c>
-      <c r="F9" s="113" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A10" s="115">
-        <v>7</v>
-      </c>
-      <c r="B10" s="113" t="s">
-        <v>818</v>
-      </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70" t="s">
-        <v>839</v>
-      </c>
-      <c r="E10" s="70">
-        <v>7</v>
-      </c>
-      <c r="F10" s="113" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="70" t="s">
-        <v>756</v>
-      </c>
-      <c r="H10" s="70" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A11" s="115">
-        <v>8</v>
-      </c>
-      <c r="B11" s="113" t="s">
-        <v>841</v>
-      </c>
-      <c r="C11" s="70" t="s">
-        <v>336</v>
-      </c>
-      <c r="D11" s="70" t="s">
-        <v>704</v>
-      </c>
-      <c r="E11" s="70">
-        <v>8</v>
-      </c>
-      <c r="F11" s="113" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="70" t="s">
-        <v>757</v>
-      </c>
-      <c r="H11" s="70" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A12" s="115">
-        <v>9</v>
-      </c>
-      <c r="B12" s="113" t="s">
-        <v>265</v>
-      </c>
-      <c r="C12" s="70" t="s">
-        <v>349</v>
-      </c>
-      <c r="D12" s="70" t="s">
-        <v>426</v>
-      </c>
-      <c r="E12" s="70">
-        <v>9</v>
-      </c>
-      <c r="F12" s="113" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>473</v>
-      </c>
-      <c r="H12" s="70" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="115">
-        <v>10</v>
-      </c>
-      <c r="B13" s="113" t="s">
-        <v>217</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>349</v>
-      </c>
-      <c r="D13" s="70" t="s">
-        <v>706</v>
-      </c>
-      <c r="E13" s="70">
-        <v>10</v>
-      </c>
-      <c r="F13" s="113" t="s">
-        <v>747</v>
-      </c>
-      <c r="G13" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H13" s="70" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A14" s="115">
-        <v>11</v>
-      </c>
-      <c r="B14" s="113" t="s">
-        <v>185</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>350</v>
-      </c>
-      <c r="D14" s="70" t="s">
-        <v>707</v>
-      </c>
-      <c r="E14" s="70">
-        <v>11</v>
-      </c>
-      <c r="F14" s="113" t="s">
-        <v>748</v>
-      </c>
-      <c r="G14" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H14" s="70" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A15" s="115">
-        <v>12</v>
-      </c>
-      <c r="B15" s="113" t="s">
-        <v>223</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>351</v>
-      </c>
-      <c r="D15" s="70" t="s">
-        <v>708</v>
-      </c>
-      <c r="E15" s="70">
-        <v>12</v>
-      </c>
-      <c r="F15" s="114" t="s">
-        <v>749</v>
-      </c>
-      <c r="G15" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H15" s="70" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="115">
-        <v>13</v>
-      </c>
-      <c r="B16" s="113" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" s="70" t="s">
-        <v>352</v>
-      </c>
-      <c r="D16" s="70" t="s">
-        <v>709</v>
-      </c>
-      <c r="E16" s="70">
-        <v>13</v>
-      </c>
-      <c r="F16" s="113" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="70" t="s">
-        <v>620</v>
-      </c>
-      <c r="H16" s="70" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A17" s="115">
-        <v>14</v>
-      </c>
-      <c r="B17" s="113" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="70" t="s">
-        <v>353</v>
-      </c>
-      <c r="D17" s="70" t="s">
-        <v>710</v>
-      </c>
-      <c r="E17" s="70">
-        <v>14</v>
-      </c>
-      <c r="F17" s="113" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="70" t="s">
-        <v>621</v>
-      </c>
-      <c r="H17" s="70" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A18" s="115">
-        <v>15</v>
-      </c>
-      <c r="B18" s="113" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="70" t="s">
-        <v>354</v>
-      </c>
-      <c r="D18" s="70" t="s">
-        <v>711</v>
-      </c>
-      <c r="E18" s="70">
-        <v>15</v>
-      </c>
-      <c r="F18" s="113" t="s">
-        <v>245</v>
-      </c>
-      <c r="G18" s="70" t="s">
-        <v>832</v>
-      </c>
-      <c r="H18" s="70" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A19" s="115">
-        <v>16</v>
-      </c>
-      <c r="B19" s="113" t="s">
-        <v>224</v>
-      </c>
-      <c r="C19" s="70" t="s">
-        <v>355</v>
-      </c>
-      <c r="D19" s="70" t="s">
-        <v>712</v>
-      </c>
-      <c r="E19" s="70">
-        <v>16</v>
-      </c>
-      <c r="F19" s="113" t="s">
-        <v>210</v>
-      </c>
-      <c r="G19" s="70" t="s">
-        <v>623</v>
-      </c>
-      <c r="H19" s="70" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A20" s="115">
-        <v>17</v>
-      </c>
-      <c r="B20" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="C20" s="70" t="s">
-        <v>649</v>
-      </c>
-      <c r="D20" s="70" t="s">
-        <v>713</v>
-      </c>
-      <c r="E20" s="70">
-        <v>17</v>
-      </c>
-      <c r="F20" s="113" t="s">
-        <v>262</v>
-      </c>
-      <c r="G20" s="70" t="s">
-        <v>624</v>
-      </c>
-      <c r="H20" s="70" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A21" s="115">
-        <v>18</v>
-      </c>
-      <c r="B21" s="113" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="70" t="s">
-        <v>658</v>
-      </c>
-      <c r="D21" s="70" t="s">
-        <v>433</v>
-      </c>
-      <c r="E21" s="70">
-        <v>18</v>
-      </c>
-      <c r="F21" s="113" t="s">
-        <v>270</v>
-      </c>
-      <c r="G21" s="70" t="s">
-        <v>345</v>
-      </c>
-      <c r="H21" s="70" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A22" s="115">
-        <v>19</v>
-      </c>
-      <c r="B22" s="113" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="70" t="s">
-        <v>470</v>
-      </c>
-      <c r="D22" s="70" t="s">
-        <v>714</v>
-      </c>
-      <c r="E22" s="70">
-        <v>19</v>
-      </c>
-      <c r="F22" s="113" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="70" t="s">
-        <v>468</v>
-      </c>
-      <c r="H22" s="70" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A23" s="115">
-        <v>20</v>
-      </c>
-      <c r="B23" s="113" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="D23" s="70" t="s">
-        <v>300</v>
-      </c>
-      <c r="E23" s="70">
-        <v>20</v>
-      </c>
-      <c r="F23" s="113" t="s">
-        <v>182</v>
-      </c>
-      <c r="G23" s="110" t="s">
-        <v>830</v>
-      </c>
-      <c r="H23" s="70" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="18.75">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-    </row>
-    <row r="25" spans="1:8" ht="18.75">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chg: Added Range 15 freq to freq overview
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="417" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="F-16 Presets" sheetId="13" r:id="rId12"/>
     <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="1063">
   <si>
     <t>AWACS</t>
   </si>
@@ -3208,7 +3208,13 @@
     <t>137.700</t>
   </si>
   <si>
-    <t>ATRM FREQ TWOPAGER v1.6</t>
+    <t>PURPLE 1</t>
+  </si>
+  <si>
+    <t>OLIVE 8</t>
+  </si>
+  <si>
+    <t>ATRM FREQ TWOPAGER v1.7</t>
   </si>
 </sst>
 </file>
@@ -4317,7 +4323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="308">
+  <cellXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4809,9 +4815,48 @@
     <xf numFmtId="0" fontId="20" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4836,42 +4881,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4944,12 +4953,63 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4968,58 +5028,7 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5057,7 +5066,7 @@
         <xdr:cNvPr id="4097" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000001100000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000001100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5115,7 +5124,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5191,7 +5200,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5267,7 +5276,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5343,7 +5352,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5684,19 +5693,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AI77"/>
+  <dimension ref="B1:AI78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U65" sqref="U65:Y65"/>
+    <sheetView topLeftCell="R43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC68" sqref="AC68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="17" max="17" width="6.44140625" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32">
@@ -5706,7 +5715,7 @@
       <c r="W1" s="137"/>
       <c r="X1" s="138"/>
     </row>
-    <row r="2" spans="2:32" ht="15.75" thickBot="1">
+    <row r="2" spans="2:32" ht="15" thickBot="1">
       <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
@@ -5717,7 +5726,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="19.5" thickBot="1">
+    <row r="3" spans="2:32" ht="18.600000000000001" thickBot="1">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -5753,11 +5762,11 @@
       </c>
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
-      <c r="R3" s="239" t="s">
+      <c r="R3" s="252" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="240"/>
-      <c r="T3" s="241"/>
+      <c r="S3" s="253"/>
+      <c r="T3" s="254"/>
       <c r="V3" s="8" t="s">
         <v>3</v>
       </c>
@@ -5809,11 +5818,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="45"/>
-      <c r="R4" s="246" t="s">
+      <c r="R4" s="239" t="s">
         <v>690</v>
       </c>
-      <c r="S4" s="247"/>
-      <c r="T4" s="248"/>
+      <c r="S4" s="240"/>
+      <c r="T4" s="241"/>
       <c r="V4" s="8" t="s">
         <v>4</v>
       </c>
@@ -5823,18 +5832,18 @@
       <c r="X4" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="Z4" s="237" t="s">
+      <c r="Z4" s="238" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="237"/>
-      <c r="AB4" s="237"/>
-      <c r="AD4" s="237" t="s">
+      <c r="AA4" s="238"/>
+      <c r="AB4" s="238"/>
+      <c r="AD4" s="238" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="237"/>
-      <c r="AF4" s="237"/>
-    </row>
-    <row r="5" spans="2:32" ht="15.75">
+      <c r="AE4" s="238"/>
+      <c r="AF4" s="238"/>
+    </row>
+    <row r="5" spans="2:32" ht="15.6">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -5915,7 +5924,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="15.75">
+    <row r="6" spans="2:32" ht="15.6">
       <c r="B6" s="1" t="s">
         <v>46</v>
       </c>
@@ -5982,7 +5991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="15.75">
+    <row r="7" spans="2:32" ht="15.6">
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
@@ -6049,7 +6058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="15.75">
+    <row r="8" spans="2:32" ht="15.6">
       <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
@@ -6116,11 +6125,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="15.75">
+    <row r="9" spans="2:32" ht="15.6">
       <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="48" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -6180,7 +6189,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="15.75">
+    <row r="10" spans="2:32" ht="15.6">
       <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
@@ -6244,7 +6253,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="15.75">
+    <row r="11" spans="2:32" ht="15.6">
       <c r="B11" s="1" t="s">
         <v>106</v>
       </c>
@@ -6307,13 +6316,13 @@
       <c r="X11" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="Z11" s="237" t="s">
+      <c r="Z11" s="238" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="237"/>
-      <c r="AB11" s="237"/>
-    </row>
-    <row r="12" spans="2:32" ht="15.75">
+      <c r="AA11" s="238"/>
+      <c r="AB11" s="238"/>
+    </row>
+    <row r="12" spans="2:32" ht="15.6">
       <c r="B12" s="1" t="s">
         <v>118</v>
       </c>
@@ -6386,7 +6395,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="15.75">
+    <row r="13" spans="2:32" ht="15.6">
       <c r="B13" s="1" t="s">
         <v>130</v>
       </c>
@@ -6453,7 +6462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="15.75">
+    <row r="14" spans="2:32" ht="15.6">
       <c r="B14" s="1" t="s">
         <v>141</v>
       </c>
@@ -6520,7 +6529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="15.75">
+    <row r="15" spans="2:32" ht="15.6">
       <c r="B15" s="1" t="s">
         <v>153</v>
       </c>
@@ -6587,7 +6596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="16.5" thickBot="1">
+    <row r="16" spans="2:32" ht="16.2" thickBot="1">
       <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>1</v>
@@ -6647,7 +6656,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="15.75" thickBot="1">
+    <row r="17" spans="2:32" ht="15" thickBot="1">
       <c r="B17" s="1" t="s">
         <v>165</v>
       </c>
@@ -6692,11 +6701,11 @@
         <v>382</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="249" t="s">
+      <c r="R17" s="242" t="s">
         <v>700</v>
       </c>
-      <c r="S17" s="250"/>
-      <c r="T17" s="251"/>
+      <c r="S17" s="243"/>
+      <c r="T17" s="244"/>
       <c r="V17" s="53" t="s">
         <v>898</v>
       </c>
@@ -6707,7 +6716,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="18" spans="2:32" ht="15.75" thickBot="1">
+    <row r="18" spans="2:32" ht="15" thickBot="1">
       <c r="B18" s="1" t="s">
         <v>177</v>
       </c>
@@ -6814,27 +6823,27 @@
         <v>314</v>
       </c>
       <c r="Q19" s="4"/>
-      <c r="R19" s="246" t="s">
+      <c r="R19" s="239" t="s">
         <v>691</v>
       </c>
-      <c r="S19" s="247"/>
-      <c r="T19" s="248"/>
-      <c r="V19" s="252" t="s">
+      <c r="S19" s="240"/>
+      <c r="T19" s="241"/>
+      <c r="V19" s="245" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="253"/>
-      <c r="X19" s="253"/>
-      <c r="Y19" s="253"/>
-      <c r="Z19" s="254"/>
-      <c r="AB19" s="237" t="s">
+      <c r="W19" s="246"/>
+      <c r="X19" s="246"/>
+      <c r="Y19" s="246"/>
+      <c r="Z19" s="247"/>
+      <c r="AB19" s="238" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="237"/>
-      <c r="AD19" s="237"/>
-      <c r="AE19" s="237"/>
-      <c r="AF19" s="237"/>
-    </row>
-    <row r="20" spans="2:32" ht="15.75">
+      <c r="AC19" s="238"/>
+      <c r="AD19" s="238"/>
+      <c r="AE19" s="238"/>
+      <c r="AF19" s="238"/>
+    </row>
+    <row r="20" spans="2:32" ht="15.6">
       <c r="B20" s="1" t="s">
         <v>201</v>
       </c>
@@ -6996,7 +7005,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="22" spans="2:32" ht="15.75" thickBot="1">
+    <row r="22" spans="2:32" ht="15" thickBot="1">
       <c r="B22" s="1" t="s">
         <v>225</v>
       </c>
@@ -7077,7 +7086,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="15.75" thickBot="1">
+    <row r="23" spans="2:32" ht="15" thickBot="1">
       <c r="B23" s="1" t="s">
         <v>237</v>
       </c>
@@ -7301,7 +7310,7 @@
         <v>279</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="48" t="s">
         <v>566</v>
       </c>
       <c r="K26" s="17" t="s">
@@ -7550,11 +7559,11 @@
       <c r="Z30" t="s">
         <v>852</v>
       </c>
-      <c r="AC30" s="237" t="s">
+      <c r="AC30" s="238" t="s">
         <v>575</v>
       </c>
-      <c r="AD30" s="237"/>
-      <c r="AE30" s="237"/>
+      <c r="AD30" s="238"/>
+      <c r="AE30" s="238"/>
     </row>
     <row r="31" spans="2:32">
       <c r="B31" s="158" t="s">
@@ -7618,7 +7627,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="2:32" ht="15.75">
+    <row r="32" spans="2:32" ht="15.6">
       <c r="B32" s="158"/>
       <c r="C32" s="163">
         <v>1</v>
@@ -7684,7 +7693,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="33" spans="2:33" ht="15.75" thickBot="1">
+    <row r="33" spans="2:33" ht="15" thickBot="1">
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
@@ -7742,9 +7751,9 @@
       <c r="N34" s="38"/>
       <c r="O34" s="38"/>
       <c r="P34" s="38"/>
-      <c r="R34" s="242"/>
-      <c r="S34" s="242"/>
-      <c r="T34" s="242"/>
+      <c r="R34" s="255"/>
+      <c r="S34" s="255"/>
+      <c r="T34" s="255"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="61" t="s">
         <v>116</v>
@@ -7801,15 +7810,15 @@
       <c r="R36" s="92"/>
       <c r="S36" s="92"/>
       <c r="T36" s="94"/>
-      <c r="U36" s="257" t="s">
+      <c r="U36" s="250" t="s">
         <v>671</v>
       </c>
-      <c r="V36" s="257"/>
-      <c r="W36" s="257"/>
-      <c r="X36" s="257"/>
-      <c r="Y36" s="257"/>
-      <c r="Z36" s="257"/>
-      <c r="AA36" s="257"/>
+      <c r="V36" s="250"/>
+      <c r="W36" s="250"/>
+      <c r="X36" s="250"/>
+      <c r="Y36" s="250"/>
+      <c r="Z36" s="250"/>
+      <c r="AA36" s="250"/>
       <c r="AC36" s="8" t="s">
         <v>587</v>
       </c>
@@ -8019,13 +8028,13 @@
       <c r="AA41" t="s">
         <v>414</v>
       </c>
-      <c r="AC41" s="255" t="s">
+      <c r="AC41" s="248" t="s">
         <v>769</v>
       </c>
-      <c r="AD41" s="256"/>
-      <c r="AE41" s="256"/>
-      <c r="AF41" s="256"/>
-      <c r="AG41" s="256"/>
+      <c r="AD41" s="249"/>
+      <c r="AE41" s="249"/>
+      <c r="AF41" s="249"/>
+      <c r="AG41" s="249"/>
     </row>
     <row r="42" spans="2:33">
       <c r="B42" s="38"/>
@@ -8118,7 +8127,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="2:33" ht="15.75" thickBot="1">
+    <row r="44" spans="2:33" ht="15" thickBot="1">
       <c r="B44" s="38"/>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
@@ -8157,12 +8166,12 @@
         <v>611</v>
       </c>
     </row>
-    <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="249" t="s">
+    <row r="45" spans="2:33" ht="15" thickBot="1">
+      <c r="Q45" s="242" t="s">
         <v>640</v>
       </c>
-      <c r="R45" s="250"/>
-      <c r="S45" s="251"/>
+      <c r="R45" s="243"/>
+      <c r="S45" s="244"/>
       <c r="T45" s="38"/>
       <c r="W45" t="s">
         <v>719</v>
@@ -8188,7 +8197,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="243" t="s">
+      <c r="Q46" s="256" t="s">
         <v>690</v>
       </c>
       <c r="R46" s="96" t="s">
@@ -8220,7 +8229,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="244"/>
+      <c r="Q47" s="257"/>
       <c r="R47" s="8" t="s">
         <v>654</v>
       </c>
@@ -8228,26 +8237,26 @@
         <v>748</v>
       </c>
     </row>
-    <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="B48" s="237" t="s">
+    <row r="48" spans="2:33" ht="15" thickBot="1">
+      <c r="B48" s="238" t="s">
         <v>312</v>
       </c>
-      <c r="C48" s="237"/>
-      <c r="D48" s="237"/>
-      <c r="E48" s="237"/>
-      <c r="F48" s="237"/>
-      <c r="G48" s="237"/>
-      <c r="H48" s="237"/>
-      <c r="J48" s="237" t="s">
+      <c r="C48" s="238"/>
+      <c r="D48" s="238"/>
+      <c r="E48" s="238"/>
+      <c r="F48" s="238"/>
+      <c r="G48" s="238"/>
+      <c r="H48" s="238"/>
+      <c r="J48" s="238" t="s">
         <v>313</v>
       </c>
-      <c r="K48" s="237"/>
-      <c r="L48" s="237"/>
-      <c r="M48" s="237"/>
-      <c r="N48" s="237"/>
-      <c r="O48" s="237"/>
-      <c r="P48" s="237"/>
-      <c r="Q48" s="245"/>
+      <c r="K48" s="238"/>
+      <c r="L48" s="238"/>
+      <c r="M48" s="238"/>
+      <c r="N48" s="238"/>
+      <c r="O48" s="238"/>
+      <c r="P48" s="238"/>
+      <c r="Q48" s="258"/>
       <c r="R48" s="82" t="s">
         <v>655</v>
       </c>
@@ -8299,7 +8308,7 @@
       <c r="P49" s="157" t="s">
         <v>304</v>
       </c>
-      <c r="Q49" s="243" t="s">
+      <c r="Q49" s="256" t="s">
         <v>691</v>
       </c>
       <c r="R49" s="96" t="s">
@@ -8350,7 +8359,7 @@
       <c r="P50" t="s">
         <v>403</v>
       </c>
-      <c r="Q50" s="244"/>
+      <c r="Q50" s="257"/>
       <c r="R50" s="8" t="s">
         <v>656</v>
       </c>
@@ -8373,7 +8382,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="51" spans="2:35" ht="15.75" thickBot="1">
+    <row r="51" spans="2:35" ht="15" thickBot="1">
       <c r="B51" t="s">
         <v>365</v>
       </c>
@@ -8407,7 +8416,7 @@
       <c r="P51" t="s">
         <v>404</v>
       </c>
-      <c r="Q51" s="245"/>
+      <c r="Q51" s="258"/>
       <c r="R51" s="82" t="s">
         <v>657</v>
       </c>
@@ -8429,15 +8438,15 @@
       <c r="Y51" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="AC51" s="237" t="s">
+      <c r="AC51" s="238" t="s">
         <v>616</v>
       </c>
-      <c r="AD51" s="237"/>
-      <c r="AE51" s="237"/>
-      <c r="AF51" s="237"/>
-      <c r="AG51" s="237"/>
-      <c r="AH51" s="237"/>
-      <c r="AI51" s="237"/>
+      <c r="AD51" s="238"/>
+      <c r="AE51" s="238"/>
+      <c r="AF51" s="238"/>
+      <c r="AG51" s="238"/>
+      <c r="AH51" s="238"/>
+      <c r="AI51" s="238"/>
     </row>
     <row r="52" spans="2:35">
       <c r="B52" t="s">
@@ -8738,15 +8747,15 @@
       <c r="H56" t="s">
         <v>390</v>
       </c>
-      <c r="J56" s="238" t="s">
+      <c r="J56" s="251" t="s">
         <v>401</v>
       </c>
-      <c r="K56" s="238"/>
-      <c r="L56" s="238"/>
-      <c r="M56" s="238"/>
-      <c r="N56" s="238"/>
-      <c r="O56" s="238"/>
-      <c r="P56" s="238"/>
+      <c r="K56" s="251"/>
+      <c r="L56" s="251"/>
+      <c r="M56" s="251"/>
+      <c r="N56" s="251"/>
+      <c r="O56" s="251"/>
+      <c r="P56" s="251"/>
       <c r="R56" s="101"/>
       <c r="S56" s="101"/>
       <c r="T56" s="101"/>
@@ -9003,7 +9012,7 @@
       </c>
     </row>
     <row r="64" spans="2:35">
-      <c r="U64" s="307">
+      <c r="U64" s="237">
         <v>14</v>
       </c>
       <c r="V64" s="169" t="s">
@@ -9018,31 +9027,31 @@
       <c r="Y64" s="8" t="s">
         <v>856</v>
       </c>
-      <c r="AC64" s="237" t="s">
+      <c r="AC64" s="238" t="s">
         <v>669</v>
       </c>
-      <c r="AD64" s="237"/>
-      <c r="AE64" s="237"/>
-      <c r="AF64" s="237"/>
-      <c r="AG64" s="237"/>
-      <c r="AH64" s="237"/>
-      <c r="AI64" s="237"/>
+      <c r="AD64" s="238"/>
+      <c r="AE64" s="238"/>
+      <c r="AF64" s="238"/>
+      <c r="AG64" s="238"/>
+      <c r="AH64" s="238"/>
+      <c r="AI64" s="238"/>
     </row>
     <row r="65" spans="21:35">
-      <c r="U65" s="307">
-        <v>16</v>
+      <c r="U65" s="308">
+        <v>15</v>
       </c>
       <c r="V65" s="169" t="s">
-        <v>180</v>
-      </c>
-      <c r="W65" s="34" t="s">
-        <v>1058</v>
+        <v>83</v>
+      </c>
+      <c r="W65" s="53" t="s">
+        <v>1060</v>
       </c>
       <c r="X65" s="169" t="s">
-        <v>1059</v>
-      </c>
-      <c r="Y65" s="8" t="s">
-        <v>922</v>
+        <v>566</v>
+      </c>
+      <c r="Y65" s="53" t="s">
+        <v>1061</v>
       </c>
       <c r="AC65" s="15" t="s">
         <v>311</v>
@@ -9067,6 +9076,21 @@
       </c>
     </row>
     <row r="66" spans="21:35">
+      <c r="U66" s="237">
+        <v>16</v>
+      </c>
+      <c r="V66" s="169" t="s">
+        <v>180</v>
+      </c>
+      <c r="W66" s="34" t="s">
+        <v>1058</v>
+      </c>
+      <c r="X66" s="169" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Y66" s="8" t="s">
+        <v>922</v>
+      </c>
       <c r="AC66" t="s">
         <v>659</v>
       </c>
@@ -9087,13 +9111,6 @@
       </c>
     </row>
     <row r="67" spans="21:35">
-      <c r="U67" s="128" t="s">
-        <v>759</v>
-      </c>
-      <c r="V67" s="128"/>
-      <c r="W67" s="128"/>
-      <c r="X67" s="128"/>
-      <c r="Y67" s="128"/>
       <c r="AC67" t="s">
         <v>670</v>
       </c>
@@ -9115,20 +9132,12 @@
     </row>
     <row r="68" spans="21:35">
       <c r="U68" s="128" t="s">
-        <v>758</v>
-      </c>
-      <c r="V68" s="128" t="s">
-        <v>302</v>
-      </c>
-      <c r="W68" s="128" t="s">
-        <v>304</v>
-      </c>
-      <c r="X68" s="128" t="s">
-        <v>303</v>
-      </c>
-      <c r="Y68" s="128" t="s">
-        <v>304</v>
-      </c>
+        <v>759</v>
+      </c>
+      <c r="V68" s="128"/>
+      <c r="W68" s="128"/>
+      <c r="X68" s="128"/>
+      <c r="Y68" s="128"/>
       <c r="AC68" t="s">
         <v>721</v>
       </c>
@@ -9149,20 +9158,20 @@
       </c>
     </row>
     <row r="69" spans="21:35">
-      <c r="U69" s="75" t="s">
-        <v>753</v>
-      </c>
-      <c r="V69" s="169" t="s">
-        <v>105</v>
-      </c>
-      <c r="W69" s="8" t="s">
-        <v>756</v>
-      </c>
-      <c r="X69" s="169" t="s">
-        <v>766</v>
-      </c>
-      <c r="Y69" s="8" t="s">
-        <v>948</v>
+      <c r="U69" s="128" t="s">
+        <v>758</v>
+      </c>
+      <c r="V69" s="128" t="s">
+        <v>302</v>
+      </c>
+      <c r="W69" s="128" t="s">
+        <v>304</v>
+      </c>
+      <c r="X69" s="128" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y69" s="128" t="s">
+        <v>304</v>
       </c>
       <c r="AE69" t="s">
         <v>660</v>
@@ -9182,19 +9191,19 @@
     </row>
     <row r="70" spans="21:35">
       <c r="U70" s="75" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="V70" s="169" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="W70" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="X70" s="169" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Y70" s="8" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AE70" t="s">
         <v>660</v>
@@ -9214,43 +9223,67 @@
     </row>
     <row r="71" spans="21:35">
       <c r="U71" s="75" t="s">
+        <v>754</v>
+      </c>
+      <c r="V71" s="169" t="s">
+        <v>77</v>
+      </c>
+      <c r="W71" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="X71" s="169" t="s">
+        <v>767</v>
+      </c>
+      <c r="Y71" s="8" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="72" spans="21:35">
+      <c r="U72" s="75" t="s">
         <v>755</v>
       </c>
-      <c r="V71" s="169" t="s">
+      <c r="V72" s="169" t="s">
         <v>64</v>
       </c>
-      <c r="W71" s="8" t="s">
+      <c r="W72" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="X71" s="169" t="s">
+      <c r="X72" s="169" t="s">
         <v>768</v>
       </c>
-      <c r="Y71" s="8" t="s">
+      <c r="Y72" s="8" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="74" spans="21:35">
-      <c r="U74" s="112" t="s">
+    <row r="75" spans="21:35">
+      <c r="U75" s="112" t="s">
         <v>897</v>
-      </c>
-    </row>
-    <row r="75" spans="21:35">
-      <c r="U75" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="76" spans="21:35">
       <c r="U76" t="s">
-        <v>367</v>
+        <v>529</v>
       </c>
     </row>
     <row r="77" spans="21:35">
       <c r="U77" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="78" spans="21:35">
+      <c r="U78" t="s">
         <v>530</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="J48:P48"/>
+    <mergeCell ref="J56:P56"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="Q46:Q48"/>
+    <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="AB19:AF19"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="R19:T19"/>
@@ -9265,13 +9298,6 @@
     <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="U36:AA36"/>
     <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="J48:P48"/>
-    <mergeCell ref="J56:P56"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="Q46:Q48"/>
-    <mergeCell ref="Q49:Q51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9286,53 +9312,53 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="270" t="s">
+      <c r="A1" s="271" t="s">
         <v>854</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="272"/>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="273"/>
       <c r="I1" s="56"/>
       <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="273"/>
-      <c r="B2" s="274"/>
-      <c r="C2" s="274"/>
-      <c r="D2" s="274"/>
-      <c r="E2" s="274"/>
-      <c r="F2" s="274"/>
-      <c r="G2" s="274"/>
-      <c r="H2" s="275"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="276" t="s">
+      <c r="A2" s="274"/>
+      <c r="B2" s="275"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="276"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="277" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="277"/>
-      <c r="C3" s="278"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="276" t="s">
+      <c r="B3" s="278"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="277" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="277"/>
-      <c r="G3" s="278"/>
-      <c r="H3" s="279"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+      <c r="F3" s="278"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="115">
         <v>1</v>
       </c>
@@ -9358,7 +9384,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+    <row r="5" spans="1:10" ht="15" thickBot="1">
       <c r="A5" s="115">
         <v>2</v>
       </c>
@@ -9384,7 +9410,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="15" thickBot="1">
       <c r="A6" s="115">
         <v>3</v>
       </c>
@@ -9410,7 +9436,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="7" spans="1:10" ht="15" thickBot="1">
       <c r="A7" s="115">
         <v>4</v>
       </c>
@@ -9436,7 +9462,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="15" thickBot="1">
       <c r="A8" s="115">
         <v>5</v>
       </c>
@@ -9462,7 +9488,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="15" thickBot="1">
       <c r="A9" s="115">
         <v>6</v>
       </c>
@@ -9484,7 +9510,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:10" ht="15" thickBot="1">
       <c r="A10" s="115">
         <v>7</v>
       </c>
@@ -9508,7 +9534,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1">
       <c r="A11" s="115">
         <v>8</v>
       </c>
@@ -9534,7 +9560,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="15" thickBot="1">
       <c r="A12" s="115">
         <v>9</v>
       </c>
@@ -9560,7 +9586,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="A13" s="115">
         <v>10</v>
       </c>
@@ -9586,7 +9612,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="15" thickBot="1">
       <c r="A14" s="115">
         <v>11</v>
       </c>
@@ -9612,7 +9638,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="15" thickBot="1">
       <c r="A15" s="115">
         <v>12</v>
       </c>
@@ -9638,7 +9664,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="15" thickBot="1">
       <c r="A16" s="115">
         <v>13</v>
       </c>
@@ -9664,7 +9690,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" s="115">
         <v>14</v>
       </c>
@@ -9690,7 +9716,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" s="115">
         <v>15</v>
       </c>
@@ -9716,7 +9742,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" s="115">
         <v>16</v>
       </c>
@@ -9742,7 +9768,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="115">
         <v>17</v>
       </c>
@@ -9768,7 +9794,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="115">
         <v>18</v>
       </c>
@@ -9794,7 +9820,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" s="115">
         <v>19</v>
       </c>
@@ -9820,7 +9846,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1">
+    <row r="23" spans="1:8" ht="15" thickBot="1">
       <c r="A23" s="115">
         <v>20</v>
       </c>
@@ -9846,7 +9872,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75">
+    <row r="24" spans="1:8" ht="18">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -9856,7 +9882,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75">
+    <row r="25" spans="1:8" ht="18">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -9885,7 +9911,7 @@
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -9906,55 +9932,55 @@
       <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="280" t="s">
+      <c r="A1" s="281" t="s">
         <v>771</v>
       </c>
-      <c r="B1" s="280"/>
-      <c r="C1" s="280"/>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="281"/>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281"/>
-      <c r="D2" s="281"/>
-      <c r="E2" s="281"/>
-      <c r="F2" s="281"/>
-      <c r="G2" s="281"/>
-      <c r="H2" s="281"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="276" t="s">
+      <c r="B1" s="281"/>
+      <c r="C1" s="281"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="281"/>
+      <c r="F1" s="281"/>
+      <c r="G1" s="281"/>
+      <c r="H1" s="281"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1">
+      <c r="A2" s="282"/>
+      <c r="B2" s="282"/>
+      <c r="C2" s="282"/>
+      <c r="D2" s="282"/>
+      <c r="E2" s="282"/>
+      <c r="F2" s="282"/>
+      <c r="G2" s="282"/>
+      <c r="H2" s="282"/>
+    </row>
+    <row r="3" spans="1:8" ht="18">
+      <c r="A3" s="277" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="277"/>
-      <c r="C3" s="278"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="276" t="s">
+      <c r="B3" s="278"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="277" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="277"/>
-      <c r="G3" s="278"/>
-      <c r="H3" s="279"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+      <c r="F3" s="278"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="111">
         <v>1</v>
       </c>
@@ -9972,7 +9998,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="111">
         <v>2</v>
       </c>
@@ -9996,7 +10022,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+    <row r="6" spans="1:8" ht="15" thickBot="1">
       <c r="A6" s="111">
         <v>3</v>
       </c>
@@ -10020,7 +10046,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+    <row r="7" spans="1:8" ht="15" thickBot="1">
       <c r="A7" s="111">
         <v>4</v>
       </c>
@@ -10044,7 +10070,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" s="111">
         <v>5</v>
       </c>
@@ -10070,7 +10096,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+    <row r="9" spans="1:8" ht="15" thickBot="1">
       <c r="A9" s="111">
         <v>6</v>
       </c>
@@ -10096,7 +10122,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+    <row r="10" spans="1:8" ht="15" thickBot="1">
       <c r="A10" s="111">
         <v>7</v>
       </c>
@@ -10122,7 +10148,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+    <row r="11" spans="1:8" ht="15" thickBot="1">
       <c r="A11" s="111">
         <v>8</v>
       </c>
@@ -10148,7 +10174,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+    <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="111">
         <v>9</v>
       </c>
@@ -10174,7 +10200,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+    <row r="13" spans="1:8" ht="15" thickBot="1">
       <c r="A13" s="111">
         <v>10</v>
       </c>
@@ -10198,7 +10224,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+    <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="111">
         <v>11</v>
       </c>
@@ -10224,7 +10250,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="111">
         <v>12</v>
       </c>
@@ -10250,7 +10276,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+    <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="111">
         <v>13</v>
       </c>
@@ -10276,7 +10302,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" s="111">
         <v>14</v>
       </c>
@@ -10302,7 +10328,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1">
       <c r="A18" s="111">
         <v>15</v>
       </c>
@@ -10328,7 +10354,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1">
       <c r="A19" s="111">
         <v>16</v>
       </c>
@@ -10354,7 +10380,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1">
       <c r="A20" s="111">
         <v>17</v>
       </c>
@@ -10380,7 +10406,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="111">
         <v>18</v>
       </c>
@@ -10406,7 +10432,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1">
       <c r="A22" s="111">
         <v>19</v>
       </c>
@@ -10432,7 +10458,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1">
+    <row r="23" spans="1:8" ht="15" thickBot="1">
       <c r="A23" s="111">
         <v>20</v>
       </c>
@@ -10473,47 +10499,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A1" s="287" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="289"/>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1">
+      <c r="A1" s="305" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1" s="306"/>
+      <c r="C1" s="306"/>
+      <c r="D1" s="306"/>
+      <c r="E1" s="306"/>
+      <c r="F1" s="307"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="282" t="s">
+      <c r="A2" s="286" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="283"/>
-      <c r="C2" s="283"/>
-      <c r="D2" s="284" t="s">
+      <c r="B2" s="287"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="302" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="285"/>
-      <c r="F2" s="286"/>
+      <c r="E2" s="303"/>
+      <c r="F2" s="304"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="297" t="s">
+      <c r="A3" s="289" t="s">
         <v>908</v>
       </c>
-      <c r="B3" s="298"/>
-      <c r="C3" s="299"/>
+      <c r="B3" s="290"/>
+      <c r="C3" s="291"/>
       <c r="D3" s="230" t="s">
         <v>2</v>
       </c>
@@ -10524,7 +10550,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="232" t="s">
         <v>672</v>
       </c>
@@ -10544,7 +10570,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75">
+    <row r="5" spans="1:6" ht="15.6">
       <c r="A5" s="189" t="s">
         <v>672</v>
       </c>
@@ -10564,7 +10590,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75">
+    <row r="6" spans="1:6" ht="15.6">
       <c r="A6" s="189" t="s">
         <v>672</v>
       </c>
@@ -10584,7 +10610,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
+    <row r="7" spans="1:6" ht="15.6">
       <c r="A7" s="189" t="s">
         <v>672</v>
       </c>
@@ -10604,7 +10630,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6" ht="15.6">
       <c r="A8" s="232" t="s">
         <v>681</v>
       </c>
@@ -10624,7 +10650,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
+    <row r="9" spans="1:6" ht="15.6">
       <c r="A9" s="189" t="s">
         <v>681</v>
       </c>
@@ -10644,7 +10670,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75">
+    <row r="10" spans="1:6" ht="15.6">
       <c r="A10" s="189" t="s">
         <v>681</v>
       </c>
@@ -10664,7 +10690,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75">
+    <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="189" t="s">
         <v>681</v>
       </c>
@@ -10684,7 +10710,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75">
+    <row r="12" spans="1:6" ht="15.6">
       <c r="A12" s="189" t="s">
         <v>686</v>
       </c>
@@ -10704,7 +10730,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75">
+    <row r="13" spans="1:6" ht="15.6">
       <c r="A13" s="193" t="s">
         <v>686</v>
       </c>
@@ -10724,7 +10750,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75">
+    <row r="14" spans="1:6" ht="15.6">
       <c r="A14" s="189" t="s">
         <v>688</v>
       </c>
@@ -10744,7 +10770,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1">
+    <row r="15" spans="1:6" ht="16.2" thickBot="1">
       <c r="A15" s="202" t="s">
         <v>688</v>
       </c>
@@ -10762,7 +10788,7 @@
       </c>
       <c r="F15" s="192"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+    <row r="16" spans="1:6" ht="15" thickBot="1">
       <c r="A16" s="139" t="s">
         <v>700</v>
       </c>
@@ -10776,7 +10802,7 @@
       </c>
       <c r="F16" s="192"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1">
+    <row r="17" spans="1:18" ht="15" thickBot="1">
       <c r="A17" s="222" t="s">
         <v>770</v>
       </c>
@@ -10794,7 +10820,7 @@
       </c>
       <c r="F17" s="205"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1">
+    <row r="18" spans="1:18" ht="15" thickBot="1">
       <c r="A18" s="116" t="s">
         <v>330</v>
       </c>
@@ -10804,13 +10830,13 @@
       <c r="C18" s="121" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="282" t="s">
+      <c r="D18" s="286" t="s">
         <v>900</v>
       </c>
-      <c r="E18" s="283"/>
-      <c r="F18" s="290"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.75">
+      <c r="E18" s="287"/>
+      <c r="F18" s="288"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.6">
       <c r="A19" s="215">
         <v>1</v>
       </c>
@@ -10820,7 +10846,7 @@
       <c r="C19" s="217" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="291" t="s">
+      <c r="D19" s="299" t="s">
         <v>690</v>
       </c>
       <c r="E19" s="207" t="s">
@@ -10830,7 +10856,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75">
+    <row r="20" spans="1:18" ht="15.6">
       <c r="A20" s="215">
         <v>2</v>
       </c>
@@ -10840,7 +10866,7 @@
       <c r="C20" s="217" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="292"/>
+      <c r="D20" s="300"/>
       <c r="E20" s="190" t="s">
         <v>654</v>
       </c>
@@ -10851,7 +10877,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="50"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75">
+    <row r="21" spans="1:18" ht="15.6">
       <c r="A21" s="215">
         <v>3</v>
       </c>
@@ -10861,7 +10887,7 @@
       <c r="C21" s="217" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="293"/>
+      <c r="D21" s="301"/>
       <c r="E21" s="210" t="s">
         <v>655</v>
       </c>
@@ -10872,7 +10898,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="50"/>
     </row>
-    <row r="22" spans="1:18" ht="16.5" thickBot="1">
+    <row r="22" spans="1:18" ht="16.2" thickBot="1">
       <c r="A22" s="215">
         <v>4</v>
       </c>
@@ -10892,7 +10918,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="16.5" thickBot="1">
+    <row r="23" spans="1:18" ht="16.2" thickBot="1">
       <c r="A23" s="215">
         <v>5</v>
       </c>
@@ -10912,7 +10938,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.75">
+    <row r="24" spans="1:18" ht="15.6">
       <c r="A24" s="215">
         <v>6</v>
       </c>
@@ -10932,7 +10958,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75">
+    <row r="25" spans="1:18" ht="15.6">
       <c r="A25" s="215">
         <v>7</v>
       </c>
@@ -10952,7 +10978,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="16.5" thickBot="1">
+    <row r="26" spans="1:18" ht="16.2" thickBot="1">
       <c r="A26" s="215">
         <v>8</v>
       </c>
@@ -10972,7 +10998,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75">
+    <row r="27" spans="1:18" ht="15.6">
       <c r="A27" s="215">
         <v>9</v>
       </c>
@@ -10986,7 +11012,7 @@
       <c r="E27" s="145"/>
       <c r="F27" s="146"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75">
+    <row r="28" spans="1:18" ht="15.6">
       <c r="A28" s="215">
         <v>10</v>
       </c>
@@ -11000,7 +11026,7 @@
       <c r="E28" s="145"/>
       <c r="F28" s="146"/>
     </row>
-    <row r="29" spans="1:18" ht="15.75">
+    <row r="29" spans="1:18" ht="15.6">
       <c r="A29" s="215">
         <v>11</v>
       </c>
@@ -11014,7 +11040,7 @@
       <c r="E29" s="145"/>
       <c r="F29" s="146"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75">
+    <row r="30" spans="1:18" ht="15.6">
       <c r="A30" s="215">
         <v>12</v>
       </c>
@@ -11028,7 +11054,7 @@
       <c r="E30" s="145"/>
       <c r="F30" s="146"/>
     </row>
-    <row r="31" spans="1:18" ht="15.75">
+    <row r="31" spans="1:18" ht="15.6">
       <c r="A31" s="215">
         <v>13</v>
       </c>
@@ -11056,29 +11082,35 @@
       <c r="E32" s="145"/>
       <c r="F32" s="146"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75">
+    <row r="33" spans="1:6" ht="15.6">
       <c r="A33" s="215">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="216" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
       <c r="C33" s="217" t="s">
-        <v>1059</v>
+        <v>566</v>
       </c>
       <c r="D33" s="145"/>
       <c r="E33" s="145"/>
       <c r="F33" s="146"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
-      <c r="A34" s="215"/>
-      <c r="B34" s="216"/>
-      <c r="C34" s="217"/>
+    <row r="34" spans="1:6" ht="15.6">
+      <c r="A34" s="215">
+        <v>16</v>
+      </c>
+      <c r="B34" s="216" t="s">
+        <v>180</v>
+      </c>
+      <c r="C34" s="217" t="s">
+        <v>1059</v>
+      </c>
       <c r="D34" s="145"/>
       <c r="E34" s="145"/>
       <c r="F34" s="146"/>
     </row>
-    <row r="35" spans="1:6" ht="16.5" thickBot="1">
+    <row r="35" spans="1:6" ht="16.2" thickBot="1">
       <c r="A35" s="219"/>
       <c r="B35" s="220"/>
       <c r="C35" s="221"/>
@@ -11086,14 +11118,14 @@
       <c r="E35" s="145"/>
       <c r="F35" s="146"/>
     </row>
-    <row r="36" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A36" s="294" t="s">
+    <row r="36" spans="1:6" ht="16.2" thickBot="1">
+      <c r="A36" s="283" t="s">
         <v>901</v>
       </c>
-      <c r="B36" s="295"/>
-      <c r="C36" s="295"/>
-      <c r="D36" s="295"/>
-      <c r="E36" s="296"/>
+      <c r="B36" s="284"/>
+      <c r="C36" s="284"/>
+      <c r="D36" s="284"/>
+      <c r="E36" s="285"/>
       <c r="F36" s="147"/>
     </row>
     <row r="37" spans="1:6">
@@ -11114,7 +11146,7 @@
       </c>
       <c r="F37" s="147"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75">
+    <row r="38" spans="1:6" ht="15.6">
       <c r="A38" s="189" t="s">
         <v>779</v>
       </c>
@@ -11132,7 +11164,7 @@
       </c>
       <c r="F38" s="147"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75">
+    <row r="39" spans="1:6" ht="15.6">
       <c r="A39" s="189" t="s">
         <v>778</v>
       </c>
@@ -11150,7 +11182,7 @@
       </c>
       <c r="F39" s="147"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75">
+    <row r="40" spans="1:6" ht="15.6">
       <c r="A40" s="189" t="s">
         <v>892</v>
       </c>
@@ -11168,7 +11200,7 @@
       </c>
       <c r="F40" s="147"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75">
+    <row r="41" spans="1:6" ht="15.6">
       <c r="A41" s="193" t="s">
         <v>909</v>
       </c>
@@ -11186,7 +11218,7 @@
       </c>
       <c r="F41" s="147"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75">
+    <row r="42" spans="1:6" ht="15.6">
       <c r="A42" s="197" t="s">
         <v>894</v>
       </c>
@@ -11204,7 +11236,7 @@
       </c>
       <c r="F42" s="147"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75">
+    <row r="43" spans="1:6" ht="15.6">
       <c r="A43" s="189" t="s">
         <v>725</v>
       </c>
@@ -11222,7 +11254,7 @@
       </c>
       <c r="F43" s="147"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75">
+    <row r="44" spans="1:6" ht="15.6">
       <c r="A44" s="189" t="s">
         <v>726</v>
       </c>
@@ -11240,7 +11272,7 @@
       </c>
       <c r="F44" s="147"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75">
+    <row r="45" spans="1:6" ht="15.6">
       <c r="A45" s="189" t="s">
         <v>727</v>
       </c>
@@ -11258,7 +11290,7 @@
       </c>
       <c r="F45" s="147"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1">
+    <row r="46" spans="1:6" ht="15" thickBot="1">
       <c r="A46" s="202" t="s">
         <v>912</v>
       </c>
@@ -11276,7 +11308,7 @@
       </c>
       <c r="F46" s="147"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1">
+    <row r="47" spans="1:6" ht="15" thickBot="1">
       <c r="A47" s="149"/>
       <c r="B47" s="150"/>
       <c r="C47" s="150"/>
@@ -11284,25 +11316,25 @@
       <c r="E47" s="150"/>
       <c r="F47" s="151"/>
     </row>
-    <row r="48" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A48" s="300" t="s">
+    <row r="48" spans="1:6" ht="16.2" thickBot="1">
+      <c r="A48" s="292" t="s">
         <v>916</v>
       </c>
-      <c r="B48" s="301"/>
-      <c r="C48" s="301"/>
-      <c r="D48" s="302"/>
-      <c r="E48" s="302"/>
-      <c r="F48" s="303"/>
+      <c r="B48" s="293"/>
+      <c r="C48" s="293"/>
+      <c r="D48" s="294"/>
+      <c r="E48" s="294"/>
+      <c r="F48" s="295"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="148"/>
       <c r="B49" s="145"/>
       <c r="C49" s="145"/>
-      <c r="D49" s="304" t="s">
+      <c r="D49" s="296" t="s">
         <v>903</v>
       </c>
-      <c r="E49" s="305"/>
-      <c r="F49" s="306"/>
+      <c r="E49" s="297"/>
+      <c r="F49" s="298"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="148"/>
@@ -11318,7 +11350,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1">
+    <row r="51" spans="1:6" ht="15" thickBot="1">
       <c r="A51" s="148"/>
       <c r="B51" s="145"/>
       <c r="C51" s="145"/>
@@ -11330,15 +11362,15 @@
       </c>
       <c r="F51" s="206"/>
     </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1">
+    <row r="52" spans="1:6" ht="15" thickBot="1">
       <c r="A52" s="148"/>
       <c r="B52" s="145"/>
       <c r="C52" s="145"/>
-      <c r="D52" s="282" t="s">
+      <c r="D52" s="286" t="s">
         <v>858</v>
       </c>
-      <c r="E52" s="283"/>
-      <c r="F52" s="290"/>
+      <c r="E52" s="287"/>
+      <c r="F52" s="288"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="148"/>
@@ -11396,7 +11428,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1">
+    <row r="57" spans="1:6" ht="15" thickBot="1">
       <c r="A57" s="148"/>
       <c r="B57" s="145"/>
       <c r="C57" s="145"/>
@@ -11410,21 +11442,21 @@
         <v>857</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1">
+    <row r="58" spans="1:6" ht="15" thickBot="1">
       <c r="A58" s="148"/>
       <c r="B58" s="145"/>
       <c r="C58" s="145"/>
-      <c r="D58" s="282" t="s">
+      <c r="D58" s="286" t="s">
         <v>907</v>
       </c>
-      <c r="E58" s="283"/>
-      <c r="F58" s="290"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75">
+      <c r="E58" s="287"/>
+      <c r="F58" s="288"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.6">
       <c r="A59" s="148"/>
       <c r="B59" s="145"/>
       <c r="C59" s="145"/>
-      <c r="D59" s="291" t="s">
+      <c r="D59" s="299" t="s">
         <v>691</v>
       </c>
       <c r="E59" s="207" t="s">
@@ -11434,11 +11466,11 @@
         <v>750</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75">
+    <row r="60" spans="1:6" ht="15.6">
       <c r="A60" s="148"/>
       <c r="B60" s="145"/>
       <c r="C60" s="145"/>
-      <c r="D60" s="292"/>
+      <c r="D60" s="300"/>
       <c r="E60" s="190" t="s">
         <v>656</v>
       </c>
@@ -11446,11 +11478,11 @@
         <v>751</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75">
+    <row r="61" spans="1:6" ht="15.6">
       <c r="A61" s="148"/>
       <c r="B61" s="145"/>
       <c r="C61" s="145"/>
-      <c r="D61" s="293"/>
+      <c r="D61" s="301"/>
       <c r="E61" s="210" t="s">
         <v>657</v>
       </c>
@@ -11458,7 +11490,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" thickBot="1">
+    <row r="62" spans="1:6" ht="15" thickBot="1">
       <c r="A62" s="148"/>
       <c r="B62" s="145"/>
       <c r="C62" s="145"/>
@@ -11472,17 +11504,17 @@
         <v>862</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A63" s="294" t="s">
+    <row r="63" spans="1:6" ht="16.2" thickBot="1">
+      <c r="A63" s="283" t="s">
         <v>902</v>
       </c>
-      <c r="B63" s="295"/>
-      <c r="C63" s="295"/>
-      <c r="D63" s="295"/>
-      <c r="E63" s="296"/>
+      <c r="B63" s="284"/>
+      <c r="C63" s="284"/>
+      <c r="D63" s="284"/>
+      <c r="E63" s="285"/>
       <c r="F63" s="146"/>
     </row>
-    <row r="64" spans="1:6" ht="15.75">
+    <row r="64" spans="1:6" ht="15.6">
       <c r="A64" s="189" t="s">
         <v>728</v>
       </c>
@@ -11500,7 +11532,7 @@
       </c>
       <c r="F64" s="146"/>
     </row>
-    <row r="65" spans="1:6" ht="15.75">
+    <row r="65" spans="1:6" ht="15.6">
       <c r="A65" s="189" t="s">
         <v>729</v>
       </c>
@@ -11518,7 +11550,7 @@
       </c>
       <c r="F65" s="146"/>
     </row>
-    <row r="66" spans="1:6" ht="15.75">
+    <row r="66" spans="1:6" ht="15.6">
       <c r="A66" s="189" t="s">
         <v>730</v>
       </c>
@@ -11536,7 +11568,7 @@
       </c>
       <c r="F66" s="146"/>
     </row>
-    <row r="67" spans="1:6" ht="16.5" thickBot="1">
+    <row r="67" spans="1:6" ht="16.2" thickBot="1">
       <c r="A67" s="202" t="s">
         <v>731</v>
       </c>
@@ -11795,6 +11827,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="A3:C3"/>
@@ -11803,11 +11840,6 @@
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="D59:D61"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11822,10 +11854,10 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
+    <row r="2" spans="1:13" ht="15" thickBot="1"/>
+    <row r="3" spans="1:13" ht="15" thickBot="1">
       <c r="A3" s="179" t="s">
         <v>545</v>
       </c>
@@ -11854,7 +11886,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+    <row r="4" spans="1:13" ht="15" thickBot="1">
       <c r="A4" s="179" t="s">
         <v>632</v>
       </c>
@@ -11883,7 +11915,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1">
+    <row r="5" spans="1:13" ht="15" thickBot="1">
       <c r="A5" s="179" t="s">
         <v>633</v>
       </c>
@@ -11912,7 +11944,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1">
+    <row r="6" spans="1:13" ht="15" thickBot="1">
       <c r="A6" s="179" t="s">
         <v>635</v>
       </c>
@@ -11941,7 +11973,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
+    <row r="7" spans="1:13" ht="15" thickBot="1">
       <c r="A7" s="179" t="s">
         <v>637</v>
       </c>
@@ -11970,7 +12002,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1">
+    <row r="8" spans="1:13" ht="15" thickBot="1">
       <c r="A8" s="179" t="s">
         <v>641</v>
       </c>
@@ -11996,7 +12028,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1">
+    <row r="9" spans="1:13" ht="15" thickBot="1">
       <c r="A9" s="179" t="s">
         <v>643</v>
       </c>
@@ -12022,7 +12054,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+    <row r="10" spans="1:13" ht="15" thickBot="1">
       <c r="A10" s="179" t="s">
         <v>646</v>
       </c>
@@ -12048,7 +12080,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1">
+    <row r="11" spans="1:13" ht="15" thickBot="1">
       <c r="A11" s="179" t="s">
         <v>614</v>
       </c>
@@ -12074,7 +12106,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1">
+    <row r="12" spans="1:13" ht="15" thickBot="1">
       <c r="A12" s="179" t="s">
         <v>614</v>
       </c>
@@ -12100,12 +12132,12 @@
         <v>986</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1">
+    <row r="14" spans="1:13" ht="15" thickBot="1">
       <c r="M14" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1">
+    <row r="15" spans="1:13" ht="15" thickBot="1">
       <c r="A15" s="179" t="s">
         <v>987</v>
       </c>
@@ -12131,7 +12163,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1">
+    <row r="16" spans="1:13" ht="15" thickBot="1">
       <c r="A16" s="179" t="s">
         <v>670</v>
       </c>
@@ -12157,8 +12189,8 @@
         <v>963</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1">
+    <row r="19" spans="1:17" ht="15" thickBot="1"/>
+    <row r="20" spans="1:17" ht="15" thickBot="1">
       <c r="A20" s="179" t="s">
         <v>827</v>
       </c>
@@ -12184,7 +12216,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1">
+    <row r="21" spans="1:17" ht="15" thickBot="1">
       <c r="A21" s="179" t="s">
         <v>896</v>
       </c>
@@ -12213,7 +12245,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1">
+    <row r="22" spans="1:17" ht="15" thickBot="1">
       <c r="A22" s="179" t="s">
         <v>895</v>
       </c>
@@ -12252,12 +12284,12 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" thickBot="1">
+    <row r="25" spans="1:17" ht="15" thickBot="1">
       <c r="J25" s="182" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1">
+    <row r="26" spans="1:17" ht="15" thickBot="1">
       <c r="A26" s="179" t="s">
         <v>529</v>
       </c>
@@ -12286,7 +12318,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1">
+    <row r="27" spans="1:17" ht="15" thickBot="1">
       <c r="A27" s="179" t="s">
         <v>367</v>
       </c>
@@ -12325,7 +12357,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1">
+    <row r="28" spans="1:17" ht="15" thickBot="1">
       <c r="A28" s="179" t="s">
         <v>530</v>
       </c>
@@ -12364,7 +12396,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1">
+    <row r="29" spans="1:17" ht="15" thickBot="1">
       <c r="A29" s="179" t="s">
         <v>549</v>
       </c>
@@ -12393,7 +12425,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1">
+    <row r="30" spans="1:17" ht="15" thickBot="1">
       <c r="A30" s="179" t="s">
         <v>556</v>
       </c>
@@ -12494,7 +12526,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1">
+    <row r="34" spans="1:17" ht="15" thickBot="1">
       <c r="M34" t="s">
         <v>725</v>
       </c>
@@ -12511,7 +12543,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1">
+    <row r="35" spans="1:17" ht="15" thickBot="1">
       <c r="A35" s="179" t="s">
         <v>364</v>
       </c>
@@ -12552,7 +12584,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15.75" thickBot="1">
+    <row r="36" spans="1:17" ht="15" thickBot="1">
       <c r="A36" s="179" t="s">
         <v>365</v>
       </c>
@@ -12593,7 +12625,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1">
+    <row r="37" spans="1:17" ht="15" thickBot="1">
       <c r="A37" s="179" t="s">
         <v>366</v>
       </c>
@@ -12634,7 +12666,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15.75" thickBot="1">
+    <row r="38" spans="1:17" ht="15" thickBot="1">
       <c r="A38" s="179" t="s">
         <v>555</v>
       </c>
@@ -12675,7 +12707,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15.75" thickBot="1">
+    <row r="39" spans="1:17" ht="15" thickBot="1">
       <c r="A39" s="179" t="s">
         <v>550</v>
       </c>
@@ -12716,7 +12748,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="15.75" thickBot="1">
+    <row r="40" spans="1:17" ht="15" thickBot="1">
       <c r="A40" s="179" t="s">
         <v>614</v>
       </c>
@@ -12757,7 +12789,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16.5" thickBot="1">
+    <row r="41" spans="1:17" ht="16.2" thickBot="1">
       <c r="A41" s="179" t="s">
         <v>614</v>
       </c>
@@ -12798,7 +12830,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1">
+    <row r="42" spans="1:17" ht="15" thickBot="1">
       <c r="M42" s="126" t="s">
         <v>912</v>
       </c>
@@ -12830,7 +12862,7 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="112" t="s">
@@ -13055,7 +13087,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="4" spans="3:15">
       <c r="C4" s="173"/>
@@ -14216,39 +14248,39 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="262" t="s">
         <v>918</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
-      <c r="H1" s="261"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="258" t="s">
+      <c r="B1" s="262"/>
+      <c r="C1" s="262"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="262"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6">
+      <c r="A2" s="259" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="259"/>
-      <c r="C2" s="259"/>
-      <c r="D2" s="259"/>
-      <c r="E2" s="259"/>
-      <c r="F2" s="259"/>
-      <c r="G2" s="259"/>
-      <c r="H2" s="260"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
+      <c r="F2" s="260"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="261"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6">
       <c r="A3" s="22"/>
       <c r="B3" s="23" t="s">
         <v>319</v>
@@ -14270,7 +14302,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
+    <row r="4" spans="1:8" ht="15.6">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -14294,7 +14326,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
+    <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -14318,7 +14350,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
+    <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -14342,7 +14374,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -14366,7 +14398,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
+    <row r="8" spans="1:8" ht="15.6">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -14390,7 +14422,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
+    <row r="9" spans="1:8" ht="15.6">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -14414,7 +14446,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:8" ht="15.6">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -14438,7 +14470,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
+    <row r="11" spans="1:8" ht="15.6">
       <c r="A11" s="23">
         <v>8</v>
       </c>
@@ -14462,7 +14494,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75">
+    <row r="12" spans="1:8" ht="15.6">
       <c r="A12" s="23">
         <v>9</v>
       </c>
@@ -14482,7 +14514,7 @@
       <c r="G12" s="129"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="23">
         <v>10</v>
       </c>
@@ -14506,7 +14538,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75">
+    <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -14516,19 +14548,19 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="258" t="s">
+    <row r="15" spans="1:8" ht="15.6">
+      <c r="A15" s="259" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="259"/>
-      <c r="C15" s="259"/>
-      <c r="D15" s="259"/>
-      <c r="E15" s="259"/>
-      <c r="F15" s="259"/>
-      <c r="G15" s="259"/>
-      <c r="H15" s="260"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75">
+      <c r="B15" s="260"/>
+      <c r="C15" s="260"/>
+      <c r="D15" s="260"/>
+      <c r="E15" s="260"/>
+      <c r="F15" s="260"/>
+      <c r="G15" s="260"/>
+      <c r="H15" s="261"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.6">
       <c r="A16" s="27"/>
       <c r="B16" s="23" t="s">
         <v>319</v>
@@ -14550,7 +14582,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75">
+    <row r="17" spans="1:8" ht="15.6">
       <c r="A17" s="23">
         <v>1</v>
       </c>
@@ -14576,7 +14608,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75">
+    <row r="18" spans="1:8" ht="15.6">
       <c r="A18" s="23">
         <v>2</v>
       </c>
@@ -14602,7 +14634,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75">
+    <row r="19" spans="1:8" ht="15.6">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -14628,7 +14660,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75">
+    <row r="20" spans="1:8" ht="15.6">
       <c r="A20" s="23">
         <v>4</v>
       </c>
@@ -14654,7 +14686,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75">
+    <row r="21" spans="1:8" ht="15.6">
       <c r="A21" s="23">
         <v>5</v>
       </c>
@@ -14680,7 +14712,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75">
+    <row r="22" spans="1:8" ht="15.6">
       <c r="A22" s="23">
         <v>6</v>
       </c>
@@ -14702,7 +14734,7 @@
       <c r="G22" s="129"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75">
+    <row r="23" spans="1:8" ht="15.6">
       <c r="A23" s="23">
         <v>7</v>
       </c>
@@ -14728,7 +14760,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75">
+    <row r="24" spans="1:8" ht="15.6">
       <c r="A24" s="23">
         <v>8</v>
       </c>
@@ -14754,7 +14786,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75">
+    <row r="25" spans="1:8" ht="15.6">
       <c r="A25" s="23">
         <v>9</v>
       </c>
@@ -14780,7 +14812,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75">
+    <row r="26" spans="1:8" ht="15.6">
       <c r="A26" s="23">
         <v>10</v>
       </c>
@@ -14806,7 +14838,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75">
+    <row r="27" spans="1:8" ht="15.6">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -14816,19 +14848,19 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="258" t="s">
+    <row r="28" spans="1:8" ht="15.6">
+      <c r="A28" s="259" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="259"/>
-      <c r="C28" s="259"/>
-      <c r="D28" s="259"/>
-      <c r="E28" s="259"/>
-      <c r="F28" s="259"/>
-      <c r="G28" s="259"/>
-      <c r="H28" s="260"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75">
+      <c r="B28" s="260"/>
+      <c r="C28" s="260"/>
+      <c r="D28" s="260"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="260"/>
+      <c r="G28" s="260"/>
+      <c r="H28" s="261"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6">
       <c r="A29" s="22"/>
       <c r="B29" s="23" t="s">
         <v>319</v>
@@ -14850,7 +14882,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75">
+    <row r="30" spans="1:8" ht="15.6">
       <c r="A30" s="23">
         <v>1</v>
       </c>
@@ -14876,7 +14908,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75">
+    <row r="31" spans="1:8" ht="15.6">
       <c r="A31" s="23">
         <v>2</v>
       </c>
@@ -14902,7 +14934,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75">
+    <row r="32" spans="1:8" ht="15.6">
       <c r="A32" s="23">
         <v>3</v>
       </c>
@@ -14928,7 +14960,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75">
+    <row r="33" spans="1:8" ht="15.6">
       <c r="A33" s="23">
         <v>4</v>
       </c>
@@ -14950,7 +14982,7 @@
       <c r="G33" s="131"/>
       <c r="H33" s="132"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75">
+    <row r="34" spans="1:8" ht="15.6">
       <c r="A34" s="23">
         <v>5</v>
       </c>
@@ -14972,7 +15004,7 @@
       <c r="G34" s="131"/>
       <c r="H34" s="132"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75">
+    <row r="35" spans="1:8" ht="15.6">
       <c r="A35" s="23">
         <v>6</v>
       </c>
@@ -14994,7 +15026,7 @@
       <c r="G35" s="131"/>
       <c r="H35" s="132"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75">
+    <row r="36" spans="1:8" ht="15.6">
       <c r="A36" s="23">
         <v>7</v>
       </c>
@@ -15012,7 +15044,7 @@
       <c r="G36" s="131"/>
       <c r="H36" s="132"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75">
+    <row r="37" spans="1:8" ht="15.6">
       <c r="A37" s="23">
         <v>8</v>
       </c>
@@ -15030,7 +15062,7 @@
       <c r="G37" s="131"/>
       <c r="H37" s="132"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75">
+    <row r="38" spans="1:8" ht="15.6">
       <c r="A38" s="23">
         <v>9</v>
       </c>
@@ -15048,7 +15080,7 @@
       <c r="G38" s="131"/>
       <c r="H38" s="132"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75">
+    <row r="39" spans="1:8" ht="15.6">
       <c r="A39" s="23">
         <v>10</v>
       </c>
@@ -15090,23 +15122,23 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="262" t="s">
         <v>826</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75">
+      <c r="B1" s="262"/>
+      <c r="C1" s="262"/>
+      <c r="D1" s="262"/>
+    </row>
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="40"/>
       <c r="B2" s="41" t="s">
         <v>319</v>
@@ -15119,7 +15151,7 @@
       </c>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" s="41">
         <v>1</v>
       </c>
@@ -15134,7 +15166,7 @@
       </c>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" spans="1:5" ht="18.75">
+    <row r="4" spans="1:5" ht="18">
       <c r="A4" s="41">
         <v>2</v>
       </c>
@@ -15149,7 +15181,7 @@
       </c>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:5" ht="18.75">
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" s="41">
         <v>3</v>
       </c>
@@ -15164,7 +15196,7 @@
       </c>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75">
+    <row r="6" spans="1:5" ht="18">
       <c r="A6" s="41">
         <v>4</v>
       </c>
@@ -15179,7 +15211,7 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75">
+    <row r="7" spans="1:5" ht="18">
       <c r="A7" s="41">
         <v>5</v>
       </c>
@@ -15194,7 +15226,7 @@
       </c>
       <c r="E7" s="39"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75">
+    <row r="8" spans="1:5" ht="18">
       <c r="A8" s="41">
         <v>6</v>
       </c>
@@ -15209,7 +15241,7 @@
       </c>
       <c r="E8" s="39"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75">
+    <row r="9" spans="1:5" ht="18">
       <c r="A9" s="41">
         <v>7</v>
       </c>
@@ -15224,7 +15256,7 @@
       </c>
       <c r="E9" s="39"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75">
+    <row r="10" spans="1:5" ht="18">
       <c r="A10" s="41">
         <v>8</v>
       </c>
@@ -15239,7 +15271,7 @@
       </c>
       <c r="E10" s="39"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75">
+    <row r="11" spans="1:5" ht="18">
       <c r="A11" s="41">
         <v>9</v>
       </c>
@@ -15254,7 +15286,7 @@
       </c>
       <c r="E11" s="39"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75">
+    <row r="12" spans="1:5" ht="18">
       <c r="A12" s="41">
         <v>10</v>
       </c>
@@ -15269,14 +15301,14 @@
       </c>
       <c r="E12" s="39"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75">
+    <row r="13" spans="1:5" ht="18">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75">
+    <row r="14" spans="1:5" ht="18">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -15300,41 +15332,41 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-      <c r="E1" s="262"/>
-      <c r="F1" s="262"/>
-      <c r="G1" s="262"/>
-      <c r="H1" s="262"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="258" t="s">
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="263"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="263"/>
+      <c r="H1" s="263"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6">
+      <c r="A2" s="259" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="259"/>
-      <c r="C2" s="259"/>
-      <c r="D2" s="259"/>
-      <c r="E2" s="259"/>
-      <c r="F2" s="259"/>
-      <c r="G2" s="259"/>
-      <c r="H2" s="260"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75">
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
+      <c r="F2" s="260"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="261"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6">
       <c r="A3" s="28" t="s">
         <v>324</v>
       </c>
@@ -15360,7 +15392,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
+    <row r="4" spans="1:8" ht="15.6">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -15384,7 +15416,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
+    <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -15408,7 +15440,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
+    <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -15432,7 +15464,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -15458,7 +15490,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
+    <row r="8" spans="1:8" ht="15.6">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -15480,7 +15512,7 @@
       <c r="G8" s="37"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
+    <row r="9" spans="1:8" ht="15.6">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -15506,7 +15538,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:8" ht="15.6">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -15532,7 +15564,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
+    <row r="11" spans="1:8" ht="15.6">
       <c r="A11" s="23">
         <v>8</v>
       </c>
@@ -15558,7 +15590,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75">
+    <row r="12" spans="1:8" ht="15.6">
       <c r="A12" s="23">
         <v>9</v>
       </c>
@@ -15584,7 +15616,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="23">
         <v>10</v>
       </c>
@@ -15608,7 +15640,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75">
+    <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -15618,16 +15650,16 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="258" t="s">
+    <row r="15" spans="1:8" ht="15.6">
+      <c r="A15" s="259" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="259"/>
-      <c r="C15" s="259"/>
-      <c r="D15" s="260"/>
+      <c r="B15" s="260"/>
+      <c r="C15" s="260"/>
+      <c r="D15" s="261"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75">
+    <row r="16" spans="1:8" ht="15.6">
       <c r="A16" s="28" t="s">
         <v>324</v>
       </c>
@@ -15642,7 +15674,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75">
+    <row r="17" spans="1:8" ht="15.6">
       <c r="A17" s="23">
         <v>1</v>
       </c>
@@ -15657,7 +15689,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75">
+    <row r="18" spans="1:8" ht="15.6">
       <c r="A18" s="23">
         <v>2</v>
       </c>
@@ -15672,7 +15704,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75">
+    <row r="19" spans="1:8" ht="15.6">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -15687,7 +15719,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75">
+    <row r="20" spans="1:8" ht="15.6">
       <c r="A20" s="23">
         <v>4</v>
       </c>
@@ -15702,7 +15734,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75">
+    <row r="21" spans="1:8" ht="15.6">
       <c r="A21" s="23">
         <v>5</v>
       </c>
@@ -15717,7 +15749,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75">
+    <row r="22" spans="1:8" ht="15.6">
       <c r="A22" s="23">
         <v>6</v>
       </c>
@@ -15732,7 +15764,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75">
+    <row r="23" spans="1:8" ht="15.6">
       <c r="A23" s="23">
         <v>7</v>
       </c>
@@ -15747,7 +15779,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75">
+    <row r="24" spans="1:8" ht="15.6">
       <c r="A24" s="23">
         <v>8</v>
       </c>
@@ -15762,7 +15794,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75">
+    <row r="25" spans="1:8" ht="15.6">
       <c r="A25" s="23">
         <v>9</v>
       </c>
@@ -15777,7 +15809,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75">
+    <row r="26" spans="1:8" ht="15.6">
       <c r="A26" s="23">
         <v>10</v>
       </c>
@@ -15792,7 +15824,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75">
+    <row r="27" spans="1:8" ht="15.6">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -15802,16 +15834,16 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="258" t="s">
+    <row r="28" spans="1:8" ht="15.6">
+      <c r="A28" s="259" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="259"/>
-      <c r="C28" s="259"/>
-      <c r="D28" s="260"/>
+      <c r="B28" s="260"/>
+      <c r="C28" s="260"/>
+      <c r="D28" s="261"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75">
+    <row r="29" spans="1:8" ht="15.6">
       <c r="A29" s="22" t="s">
         <v>324</v>
       </c>
@@ -15826,7 +15858,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75">
+    <row r="30" spans="1:8" ht="15.6">
       <c r="A30" s="23">
         <v>1</v>
       </c>
@@ -15841,7 +15873,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75">
+    <row r="31" spans="1:8" ht="15.6">
       <c r="A31" s="23">
         <v>2</v>
       </c>
@@ -15856,7 +15888,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75">
+    <row r="32" spans="1:8" ht="15.6">
       <c r="A32" s="23">
         <v>3</v>
       </c>
@@ -15871,7 +15903,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75">
+    <row r="33" spans="1:5" ht="15.6">
       <c r="A33" s="23">
         <v>4</v>
       </c>
@@ -15886,7 +15918,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75">
+    <row r="34" spans="1:5" ht="15.6">
       <c r="A34" s="23">
         <v>5</v>
       </c>
@@ -15901,7 +15933,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75">
+    <row r="35" spans="1:5" ht="15.6">
       <c r="A35" s="23">
         <v>6</v>
       </c>
@@ -15916,7 +15948,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75">
+    <row r="36" spans="1:5" ht="15.6">
       <c r="A36" s="23">
         <v>7</v>
       </c>
@@ -15931,7 +15963,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75">
+    <row r="37" spans="1:5" ht="15.6">
       <c r="A37" s="23">
         <v>8</v>
       </c>
@@ -15946,7 +15978,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75">
+    <row r="38" spans="1:5" ht="15.6">
       <c r="A38" s="23">
         <v>9</v>
       </c>
@@ -15961,7 +15993,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75">
+    <row r="39" spans="1:5" ht="15.6">
       <c r="A39" s="23">
         <v>10</v>
       </c>
@@ -15997,47 +16029,47 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="264" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
       <c r="G1" s="56"/>
       <c r="H1" s="56"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="264"/>
-      <c r="B2" s="264"/>
-      <c r="C2" s="264"/>
-      <c r="D2" s="264"/>
-      <c r="E2" s="264"/>
-      <c r="F2" s="264"/>
+    <row r="2" spans="1:8" ht="15" thickBot="1">
+      <c r="A2" s="265"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
+      <c r="D2" s="265"/>
+      <c r="E2" s="265"/>
+      <c r="F2" s="265"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="266" t="s">
         <v>595</v>
       </c>
-      <c r="B3" s="266"/>
-      <c r="C3" s="267"/>
-      <c r="D3" s="265" t="s">
+      <c r="B3" s="267"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="266" t="s">
         <v>596</v>
       </c>
-      <c r="E3" s="266"/>
-      <c r="F3" s="267"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+      <c r="E3" s="267"/>
+      <c r="F3" s="268"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="51">
         <v>1</v>
       </c>
@@ -16057,7 +16089,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="51">
         <v>2</v>
       </c>
@@ -16077,7 +16109,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+    <row r="6" spans="1:8" ht="15" thickBot="1">
       <c r="A6" s="51">
         <v>3</v>
       </c>
@@ -16097,7 +16129,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+    <row r="7" spans="1:8" ht="15" thickBot="1">
       <c r="A7" s="51">
         <v>4</v>
       </c>
@@ -16117,7 +16149,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" s="51">
         <v>5</v>
       </c>
@@ -16135,7 +16167,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+    <row r="9" spans="1:8" ht="15" thickBot="1">
       <c r="A9" s="51">
         <v>6</v>
       </c>
@@ -16153,7 +16185,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+    <row r="10" spans="1:8" ht="15" thickBot="1">
       <c r="A10" s="51">
         <v>7</v>
       </c>
@@ -16173,7 +16205,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+    <row r="11" spans="1:8" ht="15" thickBot="1">
       <c r="A11" s="51">
         <v>8</v>
       </c>
@@ -16193,7 +16225,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+    <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="51">
         <v>9</v>
       </c>
@@ -16213,7 +16245,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+    <row r="13" spans="1:8" ht="15" thickBot="1">
       <c r="A13" s="51">
         <v>10</v>
       </c>
@@ -16233,7 +16265,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+    <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="51">
         <v>11</v>
       </c>
@@ -16253,7 +16285,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="51">
         <v>12</v>
       </c>
@@ -16273,7 +16305,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+    <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="51">
         <v>13</v>
       </c>
@@ -16293,7 +16325,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+    <row r="17" spans="1:6" ht="15" thickBot="1">
       <c r="A17" s="51">
         <v>14</v>
       </c>
@@ -16313,7 +16345,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+    <row r="18" spans="1:6" ht="15" thickBot="1">
       <c r="A18" s="51">
         <v>15</v>
       </c>
@@ -16333,7 +16365,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+    <row r="19" spans="1:6" ht="15" thickBot="1">
       <c r="A19" s="51">
         <v>16</v>
       </c>
@@ -16353,7 +16385,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15" thickBot="1">
       <c r="A20" s="51">
         <v>17</v>
       </c>
@@ -16373,7 +16405,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+    <row r="21" spans="1:6" ht="15" thickBot="1">
       <c r="A21" s="51">
         <v>18</v>
       </c>
@@ -16393,7 +16425,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+    <row r="22" spans="1:6" ht="15" thickBot="1">
       <c r="A22" s="51">
         <v>19</v>
       </c>
@@ -16413,7 +16445,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6" ht="15" thickBot="1">
       <c r="A23" s="51">
         <v>20</v>
       </c>
@@ -16433,7 +16465,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+    <row r="24" spans="1:6" ht="15" thickBot="1">
       <c r="A24" s="51">
         <v>21</v>
       </c>
@@ -16453,7 +16485,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+    <row r="25" spans="1:6" ht="15" thickBot="1">
       <c r="A25" s="51">
         <v>22</v>
       </c>
@@ -16473,7 +16505,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6" ht="15" thickBot="1">
       <c r="A26" s="51">
         <v>23</v>
       </c>
@@ -16493,7 +16525,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+    <row r="27" spans="1:6" ht="15" thickBot="1">
       <c r="A27" s="51">
         <v>24</v>
       </c>
@@ -16513,7 +16545,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6" ht="15" thickBot="1">
       <c r="A28" s="51">
         <v>25</v>
       </c>
@@ -16531,7 +16563,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+    <row r="29" spans="1:6" ht="15" thickBot="1">
       <c r="A29" s="51">
         <v>26</v>
       </c>
@@ -16571,33 +16603,33 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="270" t="s">
         <v>567</v>
       </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
-      <c r="F1" s="269"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="268" t="s">
+      <c r="B1" s="270"/>
+      <c r="C1" s="270"/>
+      <c r="D1" s="270"/>
+      <c r="E1" s="270"/>
+      <c r="F1" s="270"/>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="B2" s="269" t="s">
         <v>588</v>
       </c>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
+      <c r="C2" s="269"/>
+      <c r="D2" s="269"/>
+      <c r="E2" s="269"/>
+    </row>
+    <row r="3" spans="1:6" ht="18">
       <c r="B3" s="40"/>
       <c r="C3" s="41" t="s">
         <v>319</v>
@@ -16609,7 +16641,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="18">
       <c r="B4" s="41" t="s">
         <v>568</v>
       </c>
@@ -16621,7 +16653,7 @@
       </c>
       <c r="E4" s="40"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="18">
       <c r="B5" s="41" t="s">
         <v>569</v>
       </c>
@@ -16633,7 +16665,7 @@
       </c>
       <c r="E5" s="40"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="18">
       <c r="B6" s="41" t="s">
         <v>570</v>
       </c>
@@ -16645,7 +16677,7 @@
       </c>
       <c r="E6" s="40"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="18">
       <c r="B7" s="41" t="s">
         <v>571</v>
       </c>
@@ -16659,7 +16691,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
+    <row r="8" spans="1:6" ht="18">
       <c r="B8" s="41" t="s">
         <v>572</v>
       </c>
@@ -16673,7 +16705,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="18">
       <c r="B9" s="41" t="s">
         <v>573</v>
       </c>
@@ -16687,7 +16719,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="18">
       <c r="B10" s="41" t="s">
         <v>574</v>
       </c>
@@ -16699,15 +16731,15 @@
       </c>
       <c r="E10" s="40"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="268" t="s">
+    <row r="14" spans="1:6" ht="18">
+      <c r="B14" s="269" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="268"/>
-      <c r="D14" s="268"/>
-      <c r="E14" s="268"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75">
+      <c r="C14" s="269"/>
+      <c r="D14" s="269"/>
+      <c r="E14" s="269"/>
+    </row>
+    <row r="15" spans="1:6" ht="18">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
         <v>319</v>
@@ -16719,7 +16751,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="18">
       <c r="B16" s="41" t="s">
         <v>568</v>
       </c>
@@ -16731,7 +16763,7 @@
       </c>
       <c r="E16" s="40"/>
     </row>
-    <row r="17" spans="2:5" ht="18.75">
+    <row r="17" spans="2:5" ht="18">
       <c r="B17" s="41" t="s">
         <v>569</v>
       </c>
@@ -16743,7 +16775,7 @@
       </c>
       <c r="E17" s="40"/>
     </row>
-    <row r="18" spans="2:5" ht="18.75">
+    <row r="18" spans="2:5" ht="18">
       <c r="B18" s="41" t="s">
         <v>570</v>
       </c>
@@ -16755,7 +16787,7 @@
       </c>
       <c r="E18" s="40"/>
     </row>
-    <row r="19" spans="2:5" ht="18.75">
+    <row r="19" spans="2:5" ht="18">
       <c r="B19" s="41" t="s">
         <v>571</v>
       </c>
@@ -16767,7 +16799,7 @@
       </c>
       <c r="E19" s="40"/>
     </row>
-    <row r="20" spans="2:5" ht="18.75">
+    <row r="20" spans="2:5" ht="18">
       <c r="B20" s="41" t="s">
         <v>572</v>
       </c>
@@ -16779,7 +16811,7 @@
       </c>
       <c r="E20" s="40"/>
     </row>
-    <row r="21" spans="2:5" ht="18.75">
+    <row r="21" spans="2:5" ht="18">
       <c r="B21" s="41" t="s">
         <v>573</v>
       </c>
@@ -16791,7 +16823,7 @@
       </c>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="2:5" ht="18.75">
+    <row r="22" spans="2:5" ht="18">
       <c r="B22" s="41" t="s">
         <v>574</v>
       </c>

</xml_diff>

<commit_message>
chg: Added EX BLUE STORM exercise combatflite file
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="417" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="417"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="F-16 Presets" sheetId="13" r:id="rId12"/>
     <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -4818,9 +4818,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4857,30 +4884,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4953,6 +4956,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4962,15 +5001,6 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4999,36 +5029,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5066,7 +5066,7 @@
         <xdr:cNvPr id="4097" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000001100000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000001100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5124,7 +5124,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5200,7 +5200,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5276,7 +5276,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5352,7 +5352,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5695,17 +5695,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AI78"/>
   <sheetViews>
-    <sheetView topLeftCell="R43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AC68" sqref="AC68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="17" max="17" width="6.44140625" customWidth="1"/>
-    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32">
@@ -5715,7 +5715,7 @@
       <c r="W1" s="137"/>
       <c r="X1" s="138"/>
     </row>
-    <row r="2" spans="2:32" ht="15" thickBot="1">
+    <row r="2" spans="2:32" ht="15.75" thickBot="1">
       <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="18.600000000000001" thickBot="1">
+    <row r="3" spans="2:32" ht="19.5" thickBot="1">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -5762,11 +5762,11 @@
       </c>
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
-      <c r="R3" s="252" t="s">
+      <c r="R3" s="241" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="253"/>
-      <c r="T3" s="254"/>
+      <c r="S3" s="242"/>
+      <c r="T3" s="243"/>
       <c r="V3" s="8" t="s">
         <v>3</v>
       </c>
@@ -5818,11 +5818,11 @@
         <v>22</v>
       </c>
       <c r="O4" s="45"/>
-      <c r="R4" s="239" t="s">
+      <c r="R4" s="248" t="s">
         <v>690</v>
       </c>
-      <c r="S4" s="240"/>
-      <c r="T4" s="241"/>
+      <c r="S4" s="249"/>
+      <c r="T4" s="250"/>
       <c r="V4" s="8" t="s">
         <v>4</v>
       </c>
@@ -5832,18 +5832,18 @@
       <c r="X4" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="Z4" s="238" t="s">
+      <c r="Z4" s="239" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="238"/>
-      <c r="AB4" s="238"/>
-      <c r="AD4" s="238" t="s">
+      <c r="AA4" s="239"/>
+      <c r="AB4" s="239"/>
+      <c r="AD4" s="239" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="238"/>
-      <c r="AF4" s="238"/>
-    </row>
-    <row r="5" spans="2:32" ht="15.6">
+      <c r="AE4" s="239"/>
+      <c r="AF4" s="239"/>
+    </row>
+    <row r="5" spans="2:32" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="15.6">
+    <row r="6" spans="2:32" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>46</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:32" ht="15.6">
+    <row r="7" spans="2:32" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="15.6">
+    <row r="8" spans="2:32" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="15.6">
+    <row r="9" spans="2:32" ht="15.75">
       <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="15.6">
+    <row r="10" spans="2:32" ht="15.75">
       <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="15.6">
+    <row r="11" spans="2:32" ht="15.75">
       <c r="B11" s="1" t="s">
         <v>106</v>
       </c>
@@ -6316,13 +6316,13 @@
       <c r="X11" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="Z11" s="238" t="s">
+      <c r="Z11" s="239" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="238"/>
-      <c r="AB11" s="238"/>
-    </row>
-    <row r="12" spans="2:32" ht="15.6">
+      <c r="AA11" s="239"/>
+      <c r="AB11" s="239"/>
+    </row>
+    <row r="12" spans="2:32" ht="15.75">
       <c r="B12" s="1" t="s">
         <v>118</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="15.6">
+    <row r="13" spans="2:32" ht="15.75">
       <c r="B13" s="1" t="s">
         <v>130</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="15.6">
+    <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="1" t="s">
         <v>141</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="15.6">
+    <row r="15" spans="2:32" ht="15.75">
       <c r="B15" s="1" t="s">
         <v>153</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="16.2" thickBot="1">
+    <row r="16" spans="2:32" ht="16.5" thickBot="1">
       <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>1</v>
@@ -6656,7 +6656,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="15" thickBot="1">
+    <row r="17" spans="2:32" ht="15.75" thickBot="1">
       <c r="B17" s="1" t="s">
         <v>165</v>
       </c>
@@ -6701,11 +6701,11 @@
         <v>382</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="242" t="s">
+      <c r="R17" s="251" t="s">
         <v>700</v>
       </c>
-      <c r="S17" s="243"/>
-      <c r="T17" s="244"/>
+      <c r="S17" s="252"/>
+      <c r="T17" s="253"/>
       <c r="V17" s="53" t="s">
         <v>898</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="18" spans="2:32" ht="15" thickBot="1">
+    <row r="18" spans="2:32" ht="15.75" thickBot="1">
       <c r="B18" s="1" t="s">
         <v>177</v>
       </c>
@@ -6823,27 +6823,27 @@
         <v>314</v>
       </c>
       <c r="Q19" s="4"/>
-      <c r="R19" s="239" t="s">
+      <c r="R19" s="248" t="s">
         <v>691</v>
       </c>
-      <c r="S19" s="240"/>
-      <c r="T19" s="241"/>
-      <c r="V19" s="245" t="s">
+      <c r="S19" s="249"/>
+      <c r="T19" s="250"/>
+      <c r="V19" s="254" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="246"/>
-      <c r="X19" s="246"/>
-      <c r="Y19" s="246"/>
-      <c r="Z19" s="247"/>
-      <c r="AB19" s="238" t="s">
+      <c r="W19" s="255"/>
+      <c r="X19" s="255"/>
+      <c r="Y19" s="255"/>
+      <c r="Z19" s="256"/>
+      <c r="AB19" s="239" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="238"/>
-      <c r="AD19" s="238"/>
-      <c r="AE19" s="238"/>
-      <c r="AF19" s="238"/>
-    </row>
-    <row r="20" spans="2:32" ht="15.6">
+      <c r="AC19" s="239"/>
+      <c r="AD19" s="239"/>
+      <c r="AE19" s="239"/>
+      <c r="AF19" s="239"/>
+    </row>
+    <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
         <v>201</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="22" spans="2:32" ht="15" thickBot="1">
+    <row r="22" spans="2:32" ht="15.75" thickBot="1">
       <c r="B22" s="1" t="s">
         <v>225</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="15" thickBot="1">
+    <row r="23" spans="2:32" ht="15.75" thickBot="1">
       <c r="B23" s="1" t="s">
         <v>237</v>
       </c>
@@ -7559,11 +7559,11 @@
       <c r="Z30" t="s">
         <v>852</v>
       </c>
-      <c r="AC30" s="238" t="s">
+      <c r="AC30" s="239" t="s">
         <v>575</v>
       </c>
-      <c r="AD30" s="238"/>
-      <c r="AE30" s="238"/>
+      <c r="AD30" s="239"/>
+      <c r="AE30" s="239"/>
     </row>
     <row r="31" spans="2:32">
       <c r="B31" s="158" t="s">
@@ -7627,7 +7627,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="2:32" ht="15.6">
+    <row r="32" spans="2:32" ht="15.75">
       <c r="B32" s="158"/>
       <c r="C32" s="163">
         <v>1</v>
@@ -7693,7 +7693,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="33" spans="2:33" ht="15" thickBot="1">
+    <row r="33" spans="2:33" ht="15.75" thickBot="1">
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
@@ -7751,9 +7751,9 @@
       <c r="N34" s="38"/>
       <c r="O34" s="38"/>
       <c r="P34" s="38"/>
-      <c r="R34" s="255"/>
-      <c r="S34" s="255"/>
-      <c r="T34" s="255"/>
+      <c r="R34" s="244"/>
+      <c r="S34" s="244"/>
+      <c r="T34" s="244"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="61" t="s">
         <v>116</v>
@@ -7810,15 +7810,15 @@
       <c r="R36" s="92"/>
       <c r="S36" s="92"/>
       <c r="T36" s="94"/>
-      <c r="U36" s="250" t="s">
+      <c r="U36" s="259" t="s">
         <v>671</v>
       </c>
-      <c r="V36" s="250"/>
-      <c r="W36" s="250"/>
-      <c r="X36" s="250"/>
-      <c r="Y36" s="250"/>
-      <c r="Z36" s="250"/>
-      <c r="AA36" s="250"/>
+      <c r="V36" s="259"/>
+      <c r="W36" s="259"/>
+      <c r="X36" s="259"/>
+      <c r="Y36" s="259"/>
+      <c r="Z36" s="259"/>
+      <c r="AA36" s="259"/>
       <c r="AC36" s="8" t="s">
         <v>587</v>
       </c>
@@ -8028,13 +8028,13 @@
       <c r="AA41" t="s">
         <v>414</v>
       </c>
-      <c r="AC41" s="248" t="s">
+      <c r="AC41" s="257" t="s">
         <v>769</v>
       </c>
-      <c r="AD41" s="249"/>
-      <c r="AE41" s="249"/>
-      <c r="AF41" s="249"/>
-      <c r="AG41" s="249"/>
+      <c r="AD41" s="258"/>
+      <c r="AE41" s="258"/>
+      <c r="AF41" s="258"/>
+      <c r="AG41" s="258"/>
     </row>
     <row r="42" spans="2:33">
       <c r="B42" s="38"/>
@@ -8127,7 +8127,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="2:33" ht="15" thickBot="1">
+    <row r="44" spans="2:33" ht="15.75" thickBot="1">
       <c r="B44" s="38"/>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
@@ -8166,12 +8166,12 @@
         <v>611</v>
       </c>
     </row>
-    <row r="45" spans="2:33" ht="15" thickBot="1">
-      <c r="Q45" s="242" t="s">
+    <row r="45" spans="2:33" ht="15.75" thickBot="1">
+      <c r="Q45" s="251" t="s">
         <v>640</v>
       </c>
-      <c r="R45" s="243"/>
-      <c r="S45" s="244"/>
+      <c r="R45" s="252"/>
+      <c r="S45" s="253"/>
       <c r="T45" s="38"/>
       <c r="W45" t="s">
         <v>719</v>
@@ -8197,7 +8197,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="256" t="s">
+      <c r="Q46" s="245" t="s">
         <v>690</v>
       </c>
       <c r="R46" s="96" t="s">
@@ -8229,7 +8229,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="257"/>
+      <c r="Q47" s="246"/>
       <c r="R47" s="8" t="s">
         <v>654</v>
       </c>
@@ -8237,26 +8237,26 @@
         <v>748</v>
       </c>
     </row>
-    <row r="48" spans="2:33" ht="15" thickBot="1">
-      <c r="B48" s="238" t="s">
+    <row r="48" spans="2:33" ht="15.75" thickBot="1">
+      <c r="B48" s="239" t="s">
         <v>312</v>
       </c>
-      <c r="C48" s="238"/>
-      <c r="D48" s="238"/>
-      <c r="E48" s="238"/>
-      <c r="F48" s="238"/>
-      <c r="G48" s="238"/>
-      <c r="H48" s="238"/>
-      <c r="J48" s="238" t="s">
+      <c r="C48" s="239"/>
+      <c r="D48" s="239"/>
+      <c r="E48" s="239"/>
+      <c r="F48" s="239"/>
+      <c r="G48" s="239"/>
+      <c r="H48" s="239"/>
+      <c r="J48" s="239" t="s">
         <v>313</v>
       </c>
-      <c r="K48" s="238"/>
-      <c r="L48" s="238"/>
-      <c r="M48" s="238"/>
-      <c r="N48" s="238"/>
-      <c r="O48" s="238"/>
-      <c r="P48" s="238"/>
-      <c r="Q48" s="258"/>
+      <c r="K48" s="239"/>
+      <c r="L48" s="239"/>
+      <c r="M48" s="239"/>
+      <c r="N48" s="239"/>
+      <c r="O48" s="239"/>
+      <c r="P48" s="239"/>
+      <c r="Q48" s="247"/>
       <c r="R48" s="82" t="s">
         <v>655</v>
       </c>
@@ -8308,7 +8308,7 @@
       <c r="P49" s="157" t="s">
         <v>304</v>
       </c>
-      <c r="Q49" s="256" t="s">
+      <c r="Q49" s="245" t="s">
         <v>691</v>
       </c>
       <c r="R49" s="96" t="s">
@@ -8359,7 +8359,7 @@
       <c r="P50" t="s">
         <v>403</v>
       </c>
-      <c r="Q50" s="257"/>
+      <c r="Q50" s="246"/>
       <c r="R50" s="8" t="s">
         <v>656</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="51" spans="2:35" ht="15" thickBot="1">
+    <row r="51" spans="2:35" ht="15.75" thickBot="1">
       <c r="B51" t="s">
         <v>365</v>
       </c>
@@ -8416,7 +8416,7 @@
       <c r="P51" t="s">
         <v>404</v>
       </c>
-      <c r="Q51" s="258"/>
+      <c r="Q51" s="247"/>
       <c r="R51" s="82" t="s">
         <v>657</v>
       </c>
@@ -8438,15 +8438,15 @@
       <c r="Y51" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="AC51" s="238" t="s">
+      <c r="AC51" s="239" t="s">
         <v>616</v>
       </c>
-      <c r="AD51" s="238"/>
-      <c r="AE51" s="238"/>
-      <c r="AF51" s="238"/>
-      <c r="AG51" s="238"/>
-      <c r="AH51" s="238"/>
-      <c r="AI51" s="238"/>
+      <c r="AD51" s="239"/>
+      <c r="AE51" s="239"/>
+      <c r="AF51" s="239"/>
+      <c r="AG51" s="239"/>
+      <c r="AH51" s="239"/>
+      <c r="AI51" s="239"/>
     </row>
     <row r="52" spans="2:35">
       <c r="B52" t="s">
@@ -8747,15 +8747,15 @@
       <c r="H56" t="s">
         <v>390</v>
       </c>
-      <c r="J56" s="251" t="s">
+      <c r="J56" s="240" t="s">
         <v>401</v>
       </c>
-      <c r="K56" s="251"/>
-      <c r="L56" s="251"/>
-      <c r="M56" s="251"/>
-      <c r="N56" s="251"/>
-      <c r="O56" s="251"/>
-      <c r="P56" s="251"/>
+      <c r="K56" s="240"/>
+      <c r="L56" s="240"/>
+      <c r="M56" s="240"/>
+      <c r="N56" s="240"/>
+      <c r="O56" s="240"/>
+      <c r="P56" s="240"/>
       <c r="R56" s="101"/>
       <c r="S56" s="101"/>
       <c r="T56" s="101"/>
@@ -9027,18 +9027,18 @@
       <c r="Y64" s="8" t="s">
         <v>856</v>
       </c>
-      <c r="AC64" s="238" t="s">
+      <c r="AC64" s="239" t="s">
         <v>669</v>
       </c>
-      <c r="AD64" s="238"/>
-      <c r="AE64" s="238"/>
-      <c r="AF64" s="238"/>
-      <c r="AG64" s="238"/>
-      <c r="AH64" s="238"/>
-      <c r="AI64" s="238"/>
+      <c r="AD64" s="239"/>
+      <c r="AE64" s="239"/>
+      <c r="AF64" s="239"/>
+      <c r="AG64" s="239"/>
+      <c r="AH64" s="239"/>
+      <c r="AI64" s="239"/>
     </row>
     <row r="65" spans="21:35">
-      <c r="U65" s="308">
+      <c r="U65" s="238">
         <v>15</v>
       </c>
       <c r="V65" s="169" t="s">
@@ -9277,13 +9277,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="J48:P48"/>
-    <mergeCell ref="J56:P56"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="Q46:Q48"/>
-    <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="AB19:AF19"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="R19:T19"/>
@@ -9298,6 +9291,13 @@
     <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="U36:AA36"/>
     <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="J48:P48"/>
+    <mergeCell ref="J56:P56"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="Q46:Q48"/>
+    <mergeCell ref="Q49:Q51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9312,53 +9312,53 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="272" t="s">
         <v>854</v>
       </c>
-      <c r="B1" s="272"/>
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="273"/>
+      <c r="B1" s="273"/>
+      <c r="C1" s="273"/>
+      <c r="D1" s="273"/>
+      <c r="E1" s="273"/>
+      <c r="F1" s="273"/>
+      <c r="G1" s="273"/>
+      <c r="H1" s="274"/>
       <c r="I1" s="56"/>
       <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="274"/>
-      <c r="B2" s="275"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="276"/>
-    </row>
-    <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="277" t="s">
+      <c r="A2" s="275"/>
+      <c r="B2" s="276"/>
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
+      <c r="F2" s="276"/>
+      <c r="G2" s="276"/>
+      <c r="H2" s="277"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75">
+      <c r="A3" s="278" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="279"/>
-      <c r="D3" s="280"/>
-      <c r="E3" s="277" t="s">
+      <c r="B3" s="279"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="281"/>
+      <c r="E3" s="278" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="278"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="280"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
+      <c r="F3" s="279"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="281"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="115">
         <v>1</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="115">
         <v>2</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="115">
         <v>3</v>
       </c>
@@ -9436,7 +9436,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="115">
         <v>4</v>
       </c>
@@ -9462,7 +9462,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="115">
         <v>5</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1">
       <c r="A9" s="115">
         <v>6</v>
       </c>
@@ -9510,7 +9510,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="115">
         <v>7</v>
       </c>
@@ -9534,7 +9534,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="115">
         <v>8</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="115">
         <v>9</v>
       </c>
@@ -9586,7 +9586,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="115">
         <v>10</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1">
       <c r="A14" s="115">
         <v>11</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
       <c r="A15" s="115">
         <v>12</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="115">
         <v>13</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="115">
         <v>14</v>
       </c>
@@ -9716,7 +9716,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="115">
         <v>15</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="115">
         <v>16</v>
       </c>
@@ -9768,7 +9768,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" s="115">
         <v>17</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" s="115">
         <v>18</v>
       </c>
@@ -9820,7 +9820,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" s="115">
         <v>19</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1">
       <c r="A23" s="115">
         <v>20</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18">
+    <row r="24" spans="1:8" ht="18.75">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -9882,7 +9882,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
     </row>
-    <row r="25" spans="1:8" ht="18">
+    <row r="25" spans="1:8" ht="18.75">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -9911,7 +9911,7 @@
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -9932,55 +9932,55 @@
       <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="282" t="s">
         <v>771</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1">
-      <c r="A2" s="282"/>
-      <c r="B2" s="282"/>
-      <c r="C2" s="282"/>
-      <c r="D2" s="282"/>
-      <c r="E2" s="282"/>
-      <c r="F2" s="282"/>
-      <c r="G2" s="282"/>
-      <c r="H2" s="282"/>
-    </row>
-    <row r="3" spans="1:8" ht="18">
-      <c r="A3" s="277" t="s">
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="282"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A2" s="283"/>
+      <c r="B2" s="283"/>
+      <c r="C2" s="283"/>
+      <c r="D2" s="283"/>
+      <c r="E2" s="283"/>
+      <c r="F2" s="283"/>
+      <c r="G2" s="283"/>
+      <c r="H2" s="283"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75">
+      <c r="A3" s="278" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="279"/>
-      <c r="D3" s="280"/>
-      <c r="E3" s="277" t="s">
+      <c r="B3" s="279"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="281"/>
+      <c r="E3" s="278" t="s">
         <v>627</v>
       </c>
-      <c r="F3" s="278"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="280"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1">
+      <c r="F3" s="279"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="281"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="111">
         <v>1</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="111">
         <v>2</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
       <c r="A6" s="111">
         <v>3</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="111">
         <v>4</v>
       </c>
@@ -10070,7 +10070,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1">
       <c r="A8" s="111">
         <v>5</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="111">
         <v>6</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="111">
         <v>7</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1">
       <c r="A11" s="111">
         <v>8</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="A12" s="111">
         <v>9</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
       <c r="A13" s="111">
         <v>10</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1">
       <c r="A14" s="111">
         <v>11</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1">
       <c r="A15" s="111">
         <v>12</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
       <c r="A16" s="111">
         <v>13</v>
       </c>
@@ -10302,7 +10302,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="111">
         <v>14</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="111">
         <v>15</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="111">
         <v>16</v>
       </c>
@@ -10380,7 +10380,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" s="111">
         <v>17</v>
       </c>
@@ -10406,7 +10406,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" s="111">
         <v>18</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" s="111">
         <v>19</v>
       </c>
@@ -10458,7 +10458,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1">
       <c r="A23" s="111">
         <v>20</v>
       </c>
@@ -10499,47 +10499,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1">
-      <c r="A1" s="305" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A1" s="289" t="s">
         <v>1062</v>
       </c>
-      <c r="B1" s="306"/>
-      <c r="C1" s="306"/>
-      <c r="D1" s="306"/>
-      <c r="E1" s="306"/>
-      <c r="F1" s="307"/>
+      <c r="B1" s="290"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="291"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="286" t="s">
+      <c r="A2" s="284" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="302" t="s">
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="286" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="303"/>
-      <c r="F2" s="304"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="288"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="299" t="s">
         <v>908</v>
       </c>
-      <c r="B3" s="290"/>
-      <c r="C3" s="291"/>
+      <c r="B3" s="300"/>
+      <c r="C3" s="301"/>
       <c r="D3" s="230" t="s">
         <v>2</v>
       </c>
@@ -10550,7 +10550,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="232" t="s">
         <v>672</v>
       </c>
@@ -10570,7 +10570,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="189" t="s">
         <v>672</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="189" t="s">
         <v>672</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="189" t="s">
         <v>672</v>
       </c>
@@ -10630,7 +10630,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="232" t="s">
         <v>681</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="189" t="s">
         <v>681</v>
       </c>
@@ -10670,7 +10670,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="189" t="s">
         <v>681</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="189" t="s">
         <v>681</v>
       </c>
@@ -10710,7 +10710,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="189" t="s">
         <v>686</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="193" t="s">
         <v>686</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="189" t="s">
         <v>688</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.2" thickBot="1">
+    <row r="15" spans="1:6" ht="16.5" thickBot="1">
       <c r="A15" s="202" t="s">
         <v>688</v>
       </c>
@@ -10788,7 +10788,7 @@
       </c>
       <c r="F15" s="192"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
       <c r="A16" s="139" t="s">
         <v>700</v>
       </c>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="F16" s="192"/>
     </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="222" t="s">
         <v>770</v>
       </c>
@@ -10820,7 +10820,7 @@
       </c>
       <c r="F17" s="205"/>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1">
       <c r="A18" s="116" t="s">
         <v>330</v>
       </c>
@@ -10830,13 +10830,13 @@
       <c r="C18" s="121" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="286" t="s">
+      <c r="D18" s="284" t="s">
         <v>900</v>
       </c>
-      <c r="E18" s="287"/>
-      <c r="F18" s="288"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.6">
+      <c r="E18" s="285"/>
+      <c r="F18" s="292"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75">
       <c r="A19" s="215">
         <v>1</v>
       </c>
@@ -10846,7 +10846,7 @@
       <c r="C19" s="217" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="299" t="s">
+      <c r="D19" s="293" t="s">
         <v>690</v>
       </c>
       <c r="E19" s="207" t="s">
@@ -10856,7 +10856,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.6">
+    <row r="20" spans="1:18" ht="15.75">
       <c r="A20" s="215">
         <v>2</v>
       </c>
@@ -10866,7 +10866,7 @@
       <c r="C20" s="217" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="300"/>
+      <c r="D20" s="294"/>
       <c r="E20" s="190" t="s">
         <v>654</v>
       </c>
@@ -10877,7 +10877,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="50"/>
     </row>
-    <row r="21" spans="1:18" ht="15.6">
+    <row r="21" spans="1:18" ht="15.75">
       <c r="A21" s="215">
         <v>3</v>
       </c>
@@ -10887,7 +10887,7 @@
       <c r="C21" s="217" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="301"/>
+      <c r="D21" s="295"/>
       <c r="E21" s="210" t="s">
         <v>655</v>
       </c>
@@ -10898,7 +10898,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="50"/>
     </row>
-    <row r="22" spans="1:18" ht="16.2" thickBot="1">
+    <row r="22" spans="1:18" ht="16.5" thickBot="1">
       <c r="A22" s="215">
         <v>4</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="16.2" thickBot="1">
+    <row r="23" spans="1:18" ht="16.5" thickBot="1">
       <c r="A23" s="215">
         <v>5</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.6">
+    <row r="24" spans="1:18" ht="15.75">
       <c r="A24" s="215">
         <v>6</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.6">
+    <row r="25" spans="1:18" ht="15.75">
       <c r="A25" s="215">
         <v>7</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="16.2" thickBot="1">
+    <row r="26" spans="1:18" ht="16.5" thickBot="1">
       <c r="A26" s="215">
         <v>8</v>
       </c>
@@ -10998,7 +10998,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.6">
+    <row r="27" spans="1:18" ht="15.75">
       <c r="A27" s="215">
         <v>9</v>
       </c>
@@ -11012,7 +11012,7 @@
       <c r="E27" s="145"/>
       <c r="F27" s="146"/>
     </row>
-    <row r="28" spans="1:18" ht="15.6">
+    <row r="28" spans="1:18" ht="15.75">
       <c r="A28" s="215">
         <v>10</v>
       </c>
@@ -11026,7 +11026,7 @@
       <c r="E28" s="145"/>
       <c r="F28" s="146"/>
     </row>
-    <row r="29" spans="1:18" ht="15.6">
+    <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="215">
         <v>11</v>
       </c>
@@ -11040,7 +11040,7 @@
       <c r="E29" s="145"/>
       <c r="F29" s="146"/>
     </row>
-    <row r="30" spans="1:18" ht="15.6">
+    <row r="30" spans="1:18" ht="15.75">
       <c r="A30" s="215">
         <v>12</v>
       </c>
@@ -11054,7 +11054,7 @@
       <c r="E30" s="145"/>
       <c r="F30" s="146"/>
     </row>
-    <row r="31" spans="1:18" ht="15.6">
+    <row r="31" spans="1:18" ht="15.75">
       <c r="A31" s="215">
         <v>13</v>
       </c>
@@ -11082,7 +11082,7 @@
       <c r="E32" s="145"/>
       <c r="F32" s="146"/>
     </row>
-    <row r="33" spans="1:6" ht="15.6">
+    <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="215">
         <v>15</v>
       </c>
@@ -11096,7 +11096,7 @@
       <c r="E33" s="145"/>
       <c r="F33" s="146"/>
     </row>
-    <row r="34" spans="1:6" ht="15.6">
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="215">
         <v>16</v>
       </c>
@@ -11110,7 +11110,7 @@
       <c r="E34" s="145"/>
       <c r="F34" s="146"/>
     </row>
-    <row r="35" spans="1:6" ht="16.2" thickBot="1">
+    <row r="35" spans="1:6" ht="16.5" thickBot="1">
       <c r="A35" s="219"/>
       <c r="B35" s="220"/>
       <c r="C35" s="221"/>
@@ -11118,14 +11118,14 @@
       <c r="E35" s="145"/>
       <c r="F35" s="146"/>
     </row>
-    <row r="36" spans="1:6" ht="16.2" thickBot="1">
-      <c r="A36" s="283" t="s">
+    <row r="36" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A36" s="296" t="s">
         <v>901</v>
       </c>
-      <c r="B36" s="284"/>
-      <c r="C36" s="284"/>
-      <c r="D36" s="284"/>
-      <c r="E36" s="285"/>
+      <c r="B36" s="297"/>
+      <c r="C36" s="297"/>
+      <c r="D36" s="297"/>
+      <c r="E36" s="298"/>
       <c r="F36" s="147"/>
     </row>
     <row r="37" spans="1:6">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="F37" s="147"/>
     </row>
-    <row r="38" spans="1:6" ht="15.6">
+    <row r="38" spans="1:6" ht="15.75">
       <c r="A38" s="189" t="s">
         <v>779</v>
       </c>
@@ -11164,7 +11164,7 @@
       </c>
       <c r="F38" s="147"/>
     </row>
-    <row r="39" spans="1:6" ht="15.6">
+    <row r="39" spans="1:6" ht="15.75">
       <c r="A39" s="189" t="s">
         <v>778</v>
       </c>
@@ -11182,7 +11182,7 @@
       </c>
       <c r="F39" s="147"/>
     </row>
-    <row r="40" spans="1:6" ht="15.6">
+    <row r="40" spans="1:6" ht="15.75">
       <c r="A40" s="189" t="s">
         <v>892</v>
       </c>
@@ -11200,7 +11200,7 @@
       </c>
       <c r="F40" s="147"/>
     </row>
-    <row r="41" spans="1:6" ht="15.6">
+    <row r="41" spans="1:6" ht="15.75">
       <c r="A41" s="193" t="s">
         <v>909</v>
       </c>
@@ -11218,7 +11218,7 @@
       </c>
       <c r="F41" s="147"/>
     </row>
-    <row r="42" spans="1:6" ht="15.6">
+    <row r="42" spans="1:6" ht="15.75">
       <c r="A42" s="197" t="s">
         <v>894</v>
       </c>
@@ -11236,7 +11236,7 @@
       </c>
       <c r="F42" s="147"/>
     </row>
-    <row r="43" spans="1:6" ht="15.6">
+    <row r="43" spans="1:6" ht="15.75">
       <c r="A43" s="189" t="s">
         <v>725</v>
       </c>
@@ -11254,7 +11254,7 @@
       </c>
       <c r="F43" s="147"/>
     </row>
-    <row r="44" spans="1:6" ht="15.6">
+    <row r="44" spans="1:6" ht="15.75">
       <c r="A44" s="189" t="s">
         <v>726</v>
       </c>
@@ -11272,7 +11272,7 @@
       </c>
       <c r="F44" s="147"/>
     </row>
-    <row r="45" spans="1:6" ht="15.6">
+    <row r="45" spans="1:6" ht="15.75">
       <c r="A45" s="189" t="s">
         <v>727</v>
       </c>
@@ -11290,7 +11290,7 @@
       </c>
       <c r="F45" s="147"/>
     </row>
-    <row r="46" spans="1:6" ht="15" thickBot="1">
+    <row r="46" spans="1:6" ht="15.75" thickBot="1">
       <c r="A46" s="202" t="s">
         <v>912</v>
       </c>
@@ -11308,7 +11308,7 @@
       </c>
       <c r="F46" s="147"/>
     </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1">
       <c r="A47" s="149"/>
       <c r="B47" s="150"/>
       <c r="C47" s="150"/>
@@ -11316,25 +11316,25 @@
       <c r="E47" s="150"/>
       <c r="F47" s="151"/>
     </row>
-    <row r="48" spans="1:6" ht="16.2" thickBot="1">
-      <c r="A48" s="292" t="s">
+    <row r="48" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A48" s="302" t="s">
         <v>916</v>
       </c>
-      <c r="B48" s="293"/>
-      <c r="C48" s="293"/>
-      <c r="D48" s="294"/>
-      <c r="E48" s="294"/>
-      <c r="F48" s="295"/>
+      <c r="B48" s="303"/>
+      <c r="C48" s="303"/>
+      <c r="D48" s="304"/>
+      <c r="E48" s="304"/>
+      <c r="F48" s="305"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="148"/>
       <c r="B49" s="145"/>
       <c r="C49" s="145"/>
-      <c r="D49" s="296" t="s">
+      <c r="D49" s="306" t="s">
         <v>903</v>
       </c>
-      <c r="E49" s="297"/>
-      <c r="F49" s="298"/>
+      <c r="E49" s="307"/>
+      <c r="F49" s="308"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="148"/>
@@ -11350,7 +11350,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" thickBot="1">
+    <row r="51" spans="1:6" ht="15.75" thickBot="1">
       <c r="A51" s="148"/>
       <c r="B51" s="145"/>
       <c r="C51" s="145"/>
@@ -11362,15 +11362,15 @@
       </c>
       <c r="F51" s="206"/>
     </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1">
+    <row r="52" spans="1:6" ht="15.75" thickBot="1">
       <c r="A52" s="148"/>
       <c r="B52" s="145"/>
       <c r="C52" s="145"/>
-      <c r="D52" s="286" t="s">
+      <c r="D52" s="284" t="s">
         <v>858</v>
       </c>
-      <c r="E52" s="287"/>
-      <c r="F52" s="288"/>
+      <c r="E52" s="285"/>
+      <c r="F52" s="292"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="148"/>
@@ -11428,7 +11428,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" thickBot="1">
+    <row r="57" spans="1:6" ht="15.75" thickBot="1">
       <c r="A57" s="148"/>
       <c r="B57" s="145"/>
       <c r="C57" s="145"/>
@@ -11442,21 +11442,21 @@
         <v>857</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1">
+    <row r="58" spans="1:6" ht="15.75" thickBot="1">
       <c r="A58" s="148"/>
       <c r="B58" s="145"/>
       <c r="C58" s="145"/>
-      <c r="D58" s="286" t="s">
+      <c r="D58" s="284" t="s">
         <v>907</v>
       </c>
-      <c r="E58" s="287"/>
-      <c r="F58" s="288"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.6">
+      <c r="E58" s="285"/>
+      <c r="F58" s="292"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="148"/>
       <c r="B59" s="145"/>
       <c r="C59" s="145"/>
-      <c r="D59" s="299" t="s">
+      <c r="D59" s="293" t="s">
         <v>691</v>
       </c>
       <c r="E59" s="207" t="s">
@@ -11466,11 +11466,11 @@
         <v>750</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.6">
+    <row r="60" spans="1:6" ht="15.75">
       <c r="A60" s="148"/>
       <c r="B60" s="145"/>
       <c r="C60" s="145"/>
-      <c r="D60" s="300"/>
+      <c r="D60" s="294"/>
       <c r="E60" s="190" t="s">
         <v>656</v>
       </c>
@@ -11478,11 +11478,11 @@
         <v>751</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.6">
+    <row r="61" spans="1:6" ht="15.75">
       <c r="A61" s="148"/>
       <c r="B61" s="145"/>
       <c r="C61" s="145"/>
-      <c r="D61" s="301"/>
+      <c r="D61" s="295"/>
       <c r="E61" s="210" t="s">
         <v>657</v>
       </c>
@@ -11490,7 +11490,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1">
+    <row r="62" spans="1:6" ht="15.75" thickBot="1">
       <c r="A62" s="148"/>
       <c r="B62" s="145"/>
       <c r="C62" s="145"/>
@@ -11504,17 +11504,17 @@
         <v>862</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16.2" thickBot="1">
-      <c r="A63" s="283" t="s">
+    <row r="63" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A63" s="296" t="s">
         <v>902</v>
       </c>
-      <c r="B63" s="284"/>
-      <c r="C63" s="284"/>
-      <c r="D63" s="284"/>
-      <c r="E63" s="285"/>
+      <c r="B63" s="297"/>
+      <c r="C63" s="297"/>
+      <c r="D63" s="297"/>
+      <c r="E63" s="298"/>
       <c r="F63" s="146"/>
     </row>
-    <row r="64" spans="1:6" ht="15.6">
+    <row r="64" spans="1:6" ht="15.75">
       <c r="A64" s="189" t="s">
         <v>728</v>
       </c>
@@ -11532,7 +11532,7 @@
       </c>
       <c r="F64" s="146"/>
     </row>
-    <row r="65" spans="1:6" ht="15.6">
+    <row r="65" spans="1:6" ht="15.75">
       <c r="A65" s="189" t="s">
         <v>729</v>
       </c>
@@ -11550,7 +11550,7 @@
       </c>
       <c r="F65" s="146"/>
     </row>
-    <row r="66" spans="1:6" ht="15.6">
+    <row r="66" spans="1:6" ht="15.75">
       <c r="A66" s="189" t="s">
         <v>730</v>
       </c>
@@ -11568,7 +11568,7 @@
       </c>
       <c r="F66" s="146"/>
     </row>
-    <row r="67" spans="1:6" ht="16.2" thickBot="1">
+    <row r="67" spans="1:6" ht="16.5" thickBot="1">
       <c r="A67" s="202" t="s">
         <v>731</v>
       </c>
@@ -11827,11 +11827,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:D21"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="A3:C3"/>
@@ -11840,6 +11835,11 @@
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="D59:D61"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11854,10 +11854,10 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:13" ht="15" thickBot="1"/>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1">
       <c r="A3" s="179" t="s">
         <v>545</v>
       </c>
@@ -11886,7 +11886,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1">
       <c r="A4" s="179" t="s">
         <v>632</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="179" t="s">
         <v>633</v>
       </c>
@@ -11944,7 +11944,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="A6" s="179" t="s">
         <v>635</v>
       </c>
@@ -11973,7 +11973,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1">
       <c r="A7" s="179" t="s">
         <v>637</v>
       </c>
@@ -12002,7 +12002,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1">
       <c r="A8" s="179" t="s">
         <v>641</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1">
       <c r="A9" s="179" t="s">
         <v>643</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1">
       <c r="A10" s="179" t="s">
         <v>646</v>
       </c>
@@ -12080,7 +12080,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1">
       <c r="A11" s="179" t="s">
         <v>614</v>
       </c>
@@ -12106,7 +12106,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="A12" s="179" t="s">
         <v>614</v>
       </c>
@@ -12132,12 +12132,12 @@
         <v>986</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1">
       <c r="M14" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1">
       <c r="A15" s="179" t="s">
         <v>987</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1">
       <c r="A16" s="179" t="s">
         <v>670</v>
       </c>
@@ -12189,8 +12189,8 @@
         <v>963</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15" thickBot="1"/>
-    <row r="20" spans="1:17" ht="15" thickBot="1">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1"/>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1">
       <c r="A20" s="179" t="s">
         <v>827</v>
       </c>
@@ -12216,7 +12216,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" thickBot="1">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1">
       <c r="A21" s="179" t="s">
         <v>896</v>
       </c>
@@ -12245,7 +12245,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" thickBot="1">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1">
       <c r="A22" s="179" t="s">
         <v>895</v>
       </c>
@@ -12284,12 +12284,12 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" thickBot="1">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1">
       <c r="J25" s="182" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15" thickBot="1">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1">
       <c r="A26" s="179" t="s">
         <v>529</v>
       </c>
@@ -12318,7 +12318,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15" thickBot="1">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1">
       <c r="A27" s="179" t="s">
         <v>367</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15" thickBot="1">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1">
       <c r="A28" s="179" t="s">
         <v>530</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" thickBot="1">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1">
       <c r="A29" s="179" t="s">
         <v>549</v>
       </c>
@@ -12425,7 +12425,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15" thickBot="1">
+    <row r="30" spans="1:17" ht="15.75" thickBot="1">
       <c r="A30" s="179" t="s">
         <v>556</v>
       </c>
@@ -12526,7 +12526,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" thickBot="1">
+    <row r="34" spans="1:17" ht="15.75" thickBot="1">
       <c r="M34" t="s">
         <v>725</v>
       </c>
@@ -12543,7 +12543,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" thickBot="1">
+    <row r="35" spans="1:17" ht="15.75" thickBot="1">
       <c r="A35" s="179" t="s">
         <v>364</v>
       </c>
@@ -12584,7 +12584,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" thickBot="1">
+    <row r="36" spans="1:17" ht="15.75" thickBot="1">
       <c r="A36" s="179" t="s">
         <v>365</v>
       </c>
@@ -12625,7 +12625,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" thickBot="1">
+    <row r="37" spans="1:17" ht="15.75" thickBot="1">
       <c r="A37" s="179" t="s">
         <v>366</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15" thickBot="1">
+    <row r="38" spans="1:17" ht="15.75" thickBot="1">
       <c r="A38" s="179" t="s">
         <v>555</v>
       </c>
@@ -12707,7 +12707,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15" thickBot="1">
+    <row r="39" spans="1:17" ht="15.75" thickBot="1">
       <c r="A39" s="179" t="s">
         <v>550</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="15" thickBot="1">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1">
       <c r="A40" s="179" t="s">
         <v>614</v>
       </c>
@@ -12789,7 +12789,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16.2" thickBot="1">
+    <row r="41" spans="1:17" ht="16.5" thickBot="1">
       <c r="A41" s="179" t="s">
         <v>614</v>
       </c>
@@ -12830,7 +12830,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15" thickBot="1">
+    <row r="42" spans="1:17" ht="15.75" thickBot="1">
       <c r="M42" s="126" t="s">
         <v>912</v>
       </c>
@@ -12862,7 +12862,7 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="112" t="s">
@@ -13087,7 +13087,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="3:15">
       <c r="C4" s="173"/>
@@ -14248,39 +14248,39 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>918</v>
       </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-      <c r="E1" s="262"/>
-      <c r="F1" s="262"/>
-      <c r="G1" s="262"/>
-      <c r="H1" s="262"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.6">
-      <c r="A2" s="259" t="s">
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="263"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="263"/>
+      <c r="H1" s="263"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75">
+      <c r="A2" s="260" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="261"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.6">
+      <c r="B2" s="261"/>
+      <c r="C2" s="261"/>
+      <c r="D2" s="261"/>
+      <c r="E2" s="261"/>
+      <c r="F2" s="261"/>
+      <c r="G2" s="261"/>
+      <c r="H2" s="262"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="22"/>
       <c r="B3" s="23" t="s">
         <v>319</v>
@@ -14302,7 +14302,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -14326,7 +14326,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -14350,7 +14350,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6">
+    <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -14374,7 +14374,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -14398,7 +14398,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.6">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -14446,7 +14446,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -14470,7 +14470,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="23">
         <v>8</v>
       </c>
@@ -14494,7 +14494,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="23">
         <v>9</v>
       </c>
@@ -14514,7 +14514,7 @@
       <c r="G12" s="129"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="23">
         <v>10</v>
       </c>
@@ -14538,7 +14538,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -14548,19 +14548,19 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6">
-      <c r="A15" s="259" t="s">
+    <row r="15" spans="1:8" ht="15.75">
+      <c r="A15" s="260" t="s">
         <v>321</v>
       </c>
-      <c r="B15" s="260"/>
-      <c r="C15" s="260"/>
-      <c r="D15" s="260"/>
-      <c r="E15" s="260"/>
-      <c r="F15" s="260"/>
-      <c r="G15" s="260"/>
-      <c r="H15" s="261"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6">
+      <c r="B15" s="261"/>
+      <c r="C15" s="261"/>
+      <c r="D15" s="261"/>
+      <c r="E15" s="261"/>
+      <c r="F15" s="261"/>
+      <c r="G15" s="261"/>
+      <c r="H15" s="262"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="27"/>
       <c r="B16" s="23" t="s">
         <v>319</v>
@@ -14582,7 +14582,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.6">
+    <row r="17" spans="1:8" ht="15.75">
       <c r="A17" s="23">
         <v>1</v>
       </c>
@@ -14608,7 +14608,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.6">
+    <row r="18" spans="1:8" ht="15.75">
       <c r="A18" s="23">
         <v>2</v>
       </c>
@@ -14634,7 +14634,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.6">
+    <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -14660,7 +14660,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.6">
+    <row r="20" spans="1:8" ht="15.75">
       <c r="A20" s="23">
         <v>4</v>
       </c>
@@ -14686,7 +14686,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.6">
+    <row r="21" spans="1:8" ht="15.75">
       <c r="A21" s="23">
         <v>5</v>
       </c>
@@ -14712,7 +14712,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.6">
+    <row r="22" spans="1:8" ht="15.75">
       <c r="A22" s="23">
         <v>6</v>
       </c>
@@ -14734,7 +14734,7 @@
       <c r="G22" s="129"/>
       <c r="H22" s="25"/>
     </row>
-    <row r="23" spans="1:8" ht="15.6">
+    <row r="23" spans="1:8" ht="15.75">
       <c r="A23" s="23">
         <v>7</v>
       </c>
@@ -14760,7 +14760,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.6">
+    <row r="24" spans="1:8" ht="15.75">
       <c r="A24" s="23">
         <v>8</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.6">
+    <row r="25" spans="1:8" ht="15.75">
       <c r="A25" s="23">
         <v>9</v>
       </c>
@@ -14812,7 +14812,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.6">
+    <row r="26" spans="1:8" ht="15.75">
       <c r="A26" s="23">
         <v>10</v>
       </c>
@@ -14838,7 +14838,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.6">
+    <row r="27" spans="1:8" ht="15.75">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -14848,19 +14848,19 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="15.6">
-      <c r="A28" s="259" t="s">
+    <row r="28" spans="1:8" ht="15.75">
+      <c r="A28" s="260" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="260"/>
-      <c r="C28" s="260"/>
-      <c r="D28" s="260"/>
-      <c r="E28" s="260"/>
-      <c r="F28" s="260"/>
-      <c r="G28" s="260"/>
-      <c r="H28" s="261"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.6">
+      <c r="B28" s="261"/>
+      <c r="C28" s="261"/>
+      <c r="D28" s="261"/>
+      <c r="E28" s="261"/>
+      <c r="F28" s="261"/>
+      <c r="G28" s="261"/>
+      <c r="H28" s="262"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="22"/>
       <c r="B29" s="23" t="s">
         <v>319</v>
@@ -14882,7 +14882,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.6">
+    <row r="30" spans="1:8" ht="15.75">
       <c r="A30" s="23">
         <v>1</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.6">
+    <row r="31" spans="1:8" ht="15.75">
       <c r="A31" s="23">
         <v>2</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.6">
+    <row r="32" spans="1:8" ht="15.75">
       <c r="A32" s="23">
         <v>3</v>
       </c>
@@ -14960,7 +14960,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.6">
+    <row r="33" spans="1:8" ht="15.75">
       <c r="A33" s="23">
         <v>4</v>
       </c>
@@ -14982,7 +14982,7 @@
       <c r="G33" s="131"/>
       <c r="H33" s="132"/>
     </row>
-    <row r="34" spans="1:8" ht="15.6">
+    <row r="34" spans="1:8" ht="15.75">
       <c r="A34" s="23">
         <v>5</v>
       </c>
@@ -15004,7 +15004,7 @@
       <c r="G34" s="131"/>
       <c r="H34" s="132"/>
     </row>
-    <row r="35" spans="1:8" ht="15.6">
+    <row r="35" spans="1:8" ht="15.75">
       <c r="A35" s="23">
         <v>6</v>
       </c>
@@ -15026,7 +15026,7 @@
       <c r="G35" s="131"/>
       <c r="H35" s="132"/>
     </row>
-    <row r="36" spans="1:8" ht="15.6">
+    <row r="36" spans="1:8" ht="15.75">
       <c r="A36" s="23">
         <v>7</v>
       </c>
@@ -15044,7 +15044,7 @@
       <c r="G36" s="131"/>
       <c r="H36" s="132"/>
     </row>
-    <row r="37" spans="1:8" ht="15.6">
+    <row r="37" spans="1:8" ht="15.75">
       <c r="A37" s="23">
         <v>8</v>
       </c>
@@ -15062,7 +15062,7 @@
       <c r="G37" s="131"/>
       <c r="H37" s="132"/>
     </row>
-    <row r="38" spans="1:8" ht="15.6">
+    <row r="38" spans="1:8" ht="15.75">
       <c r="A38" s="23">
         <v>9</v>
       </c>
@@ -15080,7 +15080,7 @@
       <c r="G38" s="131"/>
       <c r="H38" s="132"/>
     </row>
-    <row r="39" spans="1:8" ht="15.6">
+    <row r="39" spans="1:8" ht="15.75">
       <c r="A39" s="23">
         <v>10</v>
       </c>
@@ -15122,23 +15122,23 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>826</v>
       </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-    </row>
-    <row r="2" spans="1:5" ht="18">
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="40"/>
       <c r="B2" s="41" t="s">
         <v>319</v>
@@ -15151,7 +15151,7 @@
       </c>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="41">
         <v>1</v>
       </c>
@@ -15166,7 +15166,7 @@
       </c>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" spans="1:5" ht="18">
+    <row r="4" spans="1:5" ht="18.75">
       <c r="A4" s="41">
         <v>2</v>
       </c>
@@ -15181,7 +15181,7 @@
       </c>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18.75">
       <c r="A5" s="41">
         <v>3</v>
       </c>
@@ -15196,7 +15196,7 @@
       </c>
       <c r="E5" s="39"/>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18.75">
       <c r="A6" s="41">
         <v>4</v>
       </c>
@@ -15211,7 +15211,7 @@
       </c>
       <c r="E6" s="39"/>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18.75">
       <c r="A7" s="41">
         <v>5</v>
       </c>
@@ -15226,7 +15226,7 @@
       </c>
       <c r="E7" s="39"/>
     </row>
-    <row r="8" spans="1:5" ht="18">
+    <row r="8" spans="1:5" ht="18.75">
       <c r="A8" s="41">
         <v>6</v>
       </c>
@@ -15241,7 +15241,7 @@
       </c>
       <c r="E8" s="39"/>
     </row>
-    <row r="9" spans="1:5" ht="18">
+    <row r="9" spans="1:5" ht="18.75">
       <c r="A9" s="41">
         <v>7</v>
       </c>
@@ -15256,7 +15256,7 @@
       </c>
       <c r="E9" s="39"/>
     </row>
-    <row r="10" spans="1:5" ht="18">
+    <row r="10" spans="1:5" ht="18.75">
       <c r="A10" s="41">
         <v>8</v>
       </c>
@@ -15271,7 +15271,7 @@
       </c>
       <c r="E10" s="39"/>
     </row>
-    <row r="11" spans="1:5" ht="18">
+    <row r="11" spans="1:5" ht="18.75">
       <c r="A11" s="41">
         <v>9</v>
       </c>
@@ -15286,7 +15286,7 @@
       </c>
       <c r="E11" s="39"/>
     </row>
-    <row r="12" spans="1:5" ht="18">
+    <row r="12" spans="1:5" ht="18.75">
       <c r="A12" s="41">
         <v>10</v>
       </c>
@@ -15301,14 +15301,14 @@
       </c>
       <c r="E12" s="39"/>
     </row>
-    <row r="13" spans="1:5" ht="18">
+    <row r="13" spans="1:5" ht="18.75">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
     </row>
-    <row r="14" spans="1:5" ht="18">
+    <row r="14" spans="1:5" ht="18.75">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -15332,41 +15332,41 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" style="33" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="264" t="s">
         <v>524</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.6">
-      <c r="A2" s="259" t="s">
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75">
+      <c r="A2" s="260" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="261"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.6">
+      <c r="B2" s="261"/>
+      <c r="C2" s="261"/>
+      <c r="D2" s="261"/>
+      <c r="E2" s="261"/>
+      <c r="F2" s="261"/>
+      <c r="G2" s="261"/>
+      <c r="H2" s="262"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="28" t="s">
         <v>324</v>
       </c>
@@ -15392,7 +15392,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6">
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -15416,7 +15416,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="23">
         <v>2</v>
       </c>
@@ -15440,7 +15440,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6">
+    <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="23">
         <v>3</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6">
+    <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="23">
         <v>4</v>
       </c>
@@ -15490,7 +15490,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.6">
+    <row r="8" spans="1:8" ht="15.75">
       <c r="A8" s="23">
         <v>5</v>
       </c>
@@ -15512,7 +15512,7 @@
       <c r="G8" s="37"/>
       <c r="H8" s="36"/>
     </row>
-    <row r="9" spans="1:8" ht="15.6">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="23">
         <v>6</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6">
+    <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="23">
         <v>7</v>
       </c>
@@ -15564,7 +15564,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6">
+    <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="23">
         <v>8</v>
       </c>
@@ -15590,7 +15590,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.6">
+    <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="23">
         <v>9</v>
       </c>
@@ -15616,7 +15616,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6">
+    <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="23">
         <v>10</v>
       </c>
@@ -15640,7 +15640,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6">
+    <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -15650,16 +15650,16 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6">
-      <c r="A15" s="259" t="s">
+    <row r="15" spans="1:8" ht="15.75">
+      <c r="A15" s="260" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="260"/>
-      <c r="C15" s="260"/>
-      <c r="D15" s="261"/>
+      <c r="B15" s="261"/>
+      <c r="C15" s="261"/>
+      <c r="D15" s="262"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:8" ht="15.6">
+    <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="28" t="s">
         <v>324</v>
       </c>
@@ -15674,7 +15674,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:8" ht="15.6">
+    <row r="17" spans="1:8" ht="15.75">
       <c r="A17" s="23">
         <v>1</v>
       </c>
@@ -15689,7 +15689,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:8" ht="15.6">
+    <row r="18" spans="1:8" ht="15.75">
       <c r="A18" s="23">
         <v>2</v>
       </c>
@@ -15704,7 +15704,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6">
+    <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -15719,7 +15719,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:8" ht="15.6">
+    <row r="20" spans="1:8" ht="15.75">
       <c r="A20" s="23">
         <v>4</v>
       </c>
@@ -15734,7 +15734,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:8" ht="15.6">
+    <row r="21" spans="1:8" ht="15.75">
       <c r="A21" s="23">
         <v>5</v>
       </c>
@@ -15749,7 +15749,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:8" ht="15.6">
+    <row r="22" spans="1:8" ht="15.75">
       <c r="A22" s="23">
         <v>6</v>
       </c>
@@ -15764,7 +15764,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:8" ht="15.6">
+    <row r="23" spans="1:8" ht="15.75">
       <c r="A23" s="23">
         <v>7</v>
       </c>
@@ -15779,7 +15779,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:8" ht="15.6">
+    <row r="24" spans="1:8" ht="15.75">
       <c r="A24" s="23">
         <v>8</v>
       </c>
@@ -15794,7 +15794,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.6">
+    <row r="25" spans="1:8" ht="15.75">
       <c r="A25" s="23">
         <v>9</v>
       </c>
@@ -15809,7 +15809,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:8" ht="15.6">
+    <row r="26" spans="1:8" ht="15.75">
       <c r="A26" s="23">
         <v>10</v>
       </c>
@@ -15824,7 +15824,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:8" ht="15.6">
+    <row r="27" spans="1:8" ht="15.75">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -15834,16 +15834,16 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="15.6">
-      <c r="A28" s="259" t="s">
+    <row r="28" spans="1:8" ht="15.75">
+      <c r="A28" s="260" t="s">
         <v>326</v>
       </c>
-      <c r="B28" s="260"/>
-      <c r="C28" s="260"/>
-      <c r="D28" s="261"/>
+      <c r="B28" s="261"/>
+      <c r="C28" s="261"/>
+      <c r="D28" s="262"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:8" ht="15.6">
+    <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="22" t="s">
         <v>324</v>
       </c>
@@ -15858,7 +15858,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:8" ht="15.6">
+    <row r="30" spans="1:8" ht="15.75">
       <c r="A30" s="23">
         <v>1</v>
       </c>
@@ -15873,7 +15873,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:8" ht="15.6">
+    <row r="31" spans="1:8" ht="15.75">
       <c r="A31" s="23">
         <v>2</v>
       </c>
@@ -15888,7 +15888,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:8" ht="15.6">
+    <row r="32" spans="1:8" ht="15.75">
       <c r="A32" s="23">
         <v>3</v>
       </c>
@@ -15903,7 +15903,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="15.6">
+    <row r="33" spans="1:5" ht="15.75">
       <c r="A33" s="23">
         <v>4</v>
       </c>
@@ -15918,7 +15918,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="15.6">
+    <row r="34" spans="1:5" ht="15.75">
       <c r="A34" s="23">
         <v>5</v>
       </c>
@@ -15933,7 +15933,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="15.6">
+    <row r="35" spans="1:5" ht="15.75">
       <c r="A35" s="23">
         <v>6</v>
       </c>
@@ -15948,7 +15948,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="15.6">
+    <row r="36" spans="1:5" ht="15.75">
       <c r="A36" s="23">
         <v>7</v>
       </c>
@@ -15963,7 +15963,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" ht="15.6">
+    <row r="37" spans="1:5" ht="15.75">
       <c r="A37" s="23">
         <v>8</v>
       </c>
@@ -15978,7 +15978,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="15.6">
+    <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="23">
         <v>9</v>
       </c>
@@ -15993,7 +15993,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="15.6">
+    <row r="39" spans="1:5" ht="15.75">
       <c r="A39" s="23">
         <v>10</v>
       </c>
@@ -16029,47 +16029,47 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="264" t="s">
+      <c r="A1" s="265" t="s">
         <v>564</v>
       </c>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
       <c r="G1" s="56"/>
       <c r="H1" s="56"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1">
-      <c r="A2" s="265"/>
-      <c r="B2" s="265"/>
-      <c r="C2" s="265"/>
-      <c r="D2" s="265"/>
-      <c r="E2" s="265"/>
-      <c r="F2" s="265"/>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A2" s="266"/>
+      <c r="B2" s="266"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="266" t="s">
+      <c r="A3" s="267" t="s">
         <v>595</v>
       </c>
-      <c r="B3" s="267"/>
-      <c r="C3" s="268"/>
-      <c r="D3" s="266" t="s">
+      <c r="B3" s="268"/>
+      <c r="C3" s="269"/>
+      <c r="D3" s="267" t="s">
         <v>596</v>
       </c>
-      <c r="E3" s="267"/>
-      <c r="F3" s="268"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1">
+      <c r="E3" s="268"/>
+      <c r="F3" s="269"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="51">
         <v>1</v>
       </c>
@@ -16089,7 +16089,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="51">
         <v>2</v>
       </c>
@@ -16109,7 +16109,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
       <c r="A6" s="51">
         <v>3</v>
       </c>
@@ -16129,7 +16129,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="51">
         <v>4</v>
       </c>
@@ -16149,7 +16149,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1">
       <c r="A8" s="51">
         <v>5</v>
       </c>
@@ -16167,7 +16167,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="51">
         <v>6</v>
       </c>
@@ -16185,7 +16185,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="51">
         <v>7</v>
       </c>
@@ -16205,7 +16205,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1">
       <c r="A11" s="51">
         <v>8</v>
       </c>
@@ -16225,7 +16225,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
       <c r="A12" s="51">
         <v>9</v>
       </c>
@@ -16245,7 +16245,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
       <c r="A13" s="51">
         <v>10</v>
       </c>
@@ -16265,7 +16265,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1">
       <c r="A14" s="51">
         <v>11</v>
       </c>
@@ -16285,7 +16285,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1">
       <c r="A15" s="51">
         <v>12</v>
       </c>
@@ -16305,7 +16305,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
       <c r="A16" s="51">
         <v>13</v>
       </c>
@@ -16325,7 +16325,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
       <c r="A17" s="51">
         <v>14</v>
       </c>
@@ -16345,7 +16345,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
       <c r="A18" s="51">
         <v>15</v>
       </c>
@@ -16365,7 +16365,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
       <c r="A19" s="51">
         <v>16</v>
       </c>
@@ -16385,7 +16385,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
       <c r="A20" s="51">
         <v>17</v>
       </c>
@@ -16405,7 +16405,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
       <c r="A21" s="51">
         <v>18</v>
       </c>
@@ -16425,7 +16425,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
       <c r="A22" s="51">
         <v>19</v>
       </c>
@@ -16445,7 +16445,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
       <c r="A23" s="51">
         <v>20</v>
       </c>
@@ -16465,7 +16465,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1">
       <c r="A24" s="51">
         <v>21</v>
       </c>
@@ -16485,7 +16485,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1">
       <c r="A25" s="51">
         <v>22</v>
       </c>
@@ -16505,7 +16505,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
       <c r="A26" s="51">
         <v>23</v>
       </c>
@@ -16525,7 +16525,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1">
       <c r="A27" s="51">
         <v>24</v>
       </c>
@@ -16545,7 +16545,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
       <c r="A28" s="51">
         <v>25</v>
       </c>
@@ -16563,7 +16563,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1">
       <c r="A29" s="51">
         <v>26</v>
       </c>
@@ -16603,33 +16603,33 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="270" t="s">
+      <c r="A1" s="271" t="s">
         <v>567</v>
       </c>
-      <c r="B1" s="270"/>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="270"/>
-    </row>
-    <row r="2" spans="1:6" ht="18">
-      <c r="B2" s="269" t="s">
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="B2" s="270" t="s">
         <v>588</v>
       </c>
-      <c r="C2" s="269"/>
-      <c r="D2" s="269"/>
-      <c r="E2" s="269"/>
-    </row>
-    <row r="3" spans="1:6" ht="18">
+      <c r="C2" s="270"/>
+      <c r="D2" s="270"/>
+      <c r="E2" s="270"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="40"/>
       <c r="C3" s="41" t="s">
         <v>319</v>
@@ -16641,7 +16641,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18">
+    <row r="4" spans="1:6" ht="18.75">
       <c r="B4" s="41" t="s">
         <v>568</v>
       </c>
@@ -16653,7 +16653,7 @@
       </c>
       <c r="E4" s="40"/>
     </row>
-    <row r="5" spans="1:6" ht="18">
+    <row r="5" spans="1:6" ht="18.75">
       <c r="B5" s="41" t="s">
         <v>569</v>
       </c>
@@ -16665,7 +16665,7 @@
       </c>
       <c r="E5" s="40"/>
     </row>
-    <row r="6" spans="1:6" ht="18">
+    <row r="6" spans="1:6" ht="18.75">
       <c r="B6" s="41" t="s">
         <v>570</v>
       </c>
@@ -16677,7 +16677,7 @@
       </c>
       <c r="E6" s="40"/>
     </row>
-    <row r="7" spans="1:6" ht="18">
+    <row r="7" spans="1:6" ht="18.75">
       <c r="B7" s="41" t="s">
         <v>571</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18">
+    <row r="8" spans="1:6" ht="18.75">
       <c r="B8" s="41" t="s">
         <v>572</v>
       </c>
@@ -16705,7 +16705,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18">
+    <row r="9" spans="1:6" ht="18.75">
       <c r="B9" s="41" t="s">
         <v>573</v>
       </c>
@@ -16719,7 +16719,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18">
+    <row r="10" spans="1:6" ht="18.75">
       <c r="B10" s="41" t="s">
         <v>574</v>
       </c>
@@ -16731,15 +16731,15 @@
       </c>
       <c r="E10" s="40"/>
     </row>
-    <row r="14" spans="1:6" ht="18">
-      <c r="B14" s="269" t="s">
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="B14" s="270" t="s">
         <v>583</v>
       </c>
-      <c r="C14" s="269"/>
-      <c r="D14" s="269"/>
-      <c r="E14" s="269"/>
-    </row>
-    <row r="15" spans="1:6" ht="18">
+      <c r="C14" s="270"/>
+      <c r="D14" s="270"/>
+      <c r="E14" s="270"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
         <v>319</v>
@@ -16751,7 +16751,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18">
+    <row r="16" spans="1:6" ht="18.75">
       <c r="B16" s="41" t="s">
         <v>568</v>
       </c>
@@ -16763,7 +16763,7 @@
       </c>
       <c r="E16" s="40"/>
     </row>
-    <row r="17" spans="2:5" ht="18">
+    <row r="17" spans="2:5" ht="18.75">
       <c r="B17" s="41" t="s">
         <v>569</v>
       </c>
@@ -16775,7 +16775,7 @@
       </c>
       <c r="E17" s="40"/>
     </row>
-    <row r="18" spans="2:5" ht="18">
+    <row r="18" spans="2:5" ht="18.75">
       <c r="B18" s="41" t="s">
         <v>570</v>
       </c>
@@ -16787,7 +16787,7 @@
       </c>
       <c r="E18" s="40"/>
     </row>
-    <row r="19" spans="2:5" ht="18">
+    <row r="19" spans="2:5" ht="18.75">
       <c r="B19" s="41" t="s">
         <v>571</v>
       </c>
@@ -16799,7 +16799,7 @@
       </c>
       <c r="E19" s="40"/>
     </row>
-    <row r="20" spans="2:5" ht="18">
+    <row r="20" spans="2:5" ht="18.75">
       <c r="B20" s="41" t="s">
         <v>572</v>
       </c>
@@ -16811,7 +16811,7 @@
       </c>
       <c r="E20" s="40"/>
     </row>
-    <row r="21" spans="2:5" ht="18">
+    <row r="21" spans="2:5" ht="18.75">
       <c r="B21" s="41" t="s">
         <v>573</v>
       </c>
@@ -16823,7 +16823,7 @@
       </c>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="2:5" ht="18">
+    <row r="22" spans="2:5" ht="18.75">
       <c r="B22" s="41" t="s">
         <v>574</v>
       </c>

</xml_diff>

<commit_message>
chg: Added RED FARP Warzaw (243.5) at Al Dahfra at freq overview fix: Corrected IFF code for AR402 and AR403
</commit_message>
<xml_diff>
--- a/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
+++ b/Files/ATRM (Persian Gulf) Frequency and Callsign master list.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E0C5BC-6A9D-44D8-B7A3-1BA9F55E95A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="540" windowWidth="24570" windowHeight="18345" tabRatio="735" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="540" windowWidth="24570" windowHeight="16440" tabRatio="735"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="F-16 Presets" sheetId="13" r:id="rId12"/>
     <sheet name="FREQ ONEPAGER" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="1116">
   <si>
     <t>AWACS</t>
   </si>
@@ -3377,12 +3376,21 @@
   </si>
   <si>
     <t>ARC-210 - VHF/UHF</t>
+  </si>
+  <si>
+    <t>RED 10</t>
+  </si>
+  <si>
+    <t>FARP WARSAW</t>
+  </si>
+  <si>
+    <t>Red FARP at Al Dahfra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="31">
     <font>
       <sz val="11"/>
@@ -4953,213 +4961,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5171,6 +4972,213 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5214,7 +5222,7 @@
         <xdr:cNvPr id="4097" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000001100000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000001100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5272,7 +5280,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5348,7 +5356,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5424,7 +5432,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5481,7 +5489,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5523,7 +5531,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5555,27 +5563,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5607,24 +5597,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5800,14 +5772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AI78"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="17" max="17" width="6.42578125" customWidth="1"/>
@@ -5816,14 +5788,14 @@
     <col min="22" max="22" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32">
+    <row r="1" spans="2:33">
       <c r="V1" s="113" t="s">
         <v>0</v>
       </c>
       <c r="W1" s="114"/>
       <c r="X1" s="115"/>
     </row>
-    <row r="2" spans="2:32" ht="15.75" thickBot="1">
+    <row r="2" spans="2:33" ht="15.75" thickBot="1">
       <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
@@ -5834,7 +5806,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="19.5" thickBot="1">
+    <row r="3" spans="2:33" ht="19.5" thickBot="1">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -5868,11 +5840,11 @@
       <c r="M3" s="1">
         <v>11</v>
       </c>
-      <c r="R3" s="219" t="s">
+      <c r="R3" s="235" t="s">
         <v>298</v>
       </c>
-      <c r="S3" s="220"/>
-      <c r="T3" s="221"/>
+      <c r="S3" s="236"/>
+      <c r="T3" s="237"/>
       <c r="V3" s="8" t="s">
         <v>3</v>
       </c>
@@ -5883,7 +5855,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="2:32">
+    <row r="4" spans="2:33">
       <c r="B4" s="1" t="s">
         <v>686</v>
       </c>
@@ -5924,11 +5896,11 @@
         <v>686</v>
       </c>
       <c r="O4" s="4"/>
-      <c r="R4" s="226" t="s">
+      <c r="R4" s="223" t="s">
         <v>686</v>
       </c>
-      <c r="S4" s="227"/>
-      <c r="T4" s="228"/>
+      <c r="S4" s="224"/>
+      <c r="T4" s="225"/>
       <c r="V4" s="8" t="s">
         <v>4</v>
       </c>
@@ -5938,18 +5910,18 @@
       <c r="X4" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="Z4" s="217" t="s">
+      <c r="Z4" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="217"/>
-      <c r="AB4" s="217"/>
-      <c r="AD4" s="217" t="s">
+      <c r="AA4" s="222"/>
+      <c r="AB4" s="222"/>
+      <c r="AD4" s="222" t="s">
         <v>297</v>
       </c>
-      <c r="AE4" s="217"/>
-      <c r="AF4" s="217"/>
-    </row>
-    <row r="5" spans="2:32" ht="15.75">
+      <c r="AE4" s="222"/>
+      <c r="AF4" s="222"/>
+    </row>
+    <row r="5" spans="2:33" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>1050</v>
       </c>
@@ -6030,7 +6002,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="15.75">
+    <row r="6" spans="2:33" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>687</v>
       </c>
@@ -6061,7 +6033,7 @@
       <c r="K6" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="12" t="s">
         <v>56</v>
       </c>
       <c r="M6" s="14" t="s">
@@ -6096,8 +6068,20 @@
       <c r="Z6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:32" ht="15.75">
+      <c r="AD6" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AE6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>1051</v>
       </c>
@@ -6164,7 +6148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:32" ht="15.75">
+    <row r="8" spans="2:33" ht="15.75">
       <c r="B8" s="1" t="s">
         <v>1052</v>
       </c>
@@ -6231,7 +6215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:32" ht="15.75">
+    <row r="9" spans="2:33" ht="15.75">
       <c r="B9" s="1" t="s">
         <v>1053</v>
       </c>
@@ -6295,7 +6279,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="2:32" ht="15.75">
+    <row r="10" spans="2:33" ht="15.75">
       <c r="B10" s="1" t="s">
         <v>1054</v>
       </c>
@@ -6359,7 +6343,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="2:32" ht="15.75">
+    <row r="11" spans="2:33" ht="15.75">
       <c r="B11" s="1" t="s">
         <v>1055</v>
       </c>
@@ -6422,13 +6406,13 @@
       <c r="X11" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="Z11" s="217" t="s">
+      <c r="Z11" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="AA11" s="217"/>
-      <c r="AB11" s="217"/>
-    </row>
-    <row r="12" spans="2:32" ht="15.75">
+      <c r="AA11" s="222"/>
+      <c r="AB11" s="222"/>
+    </row>
+    <row r="12" spans="2:33" ht="15.75">
       <c r="B12" s="1" t="s">
         <v>1056</v>
       </c>
@@ -6501,7 +6485,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="2:32" ht="15.75">
+    <row r="13" spans="2:33" ht="15.75">
       <c r="B13" s="1" t="s">
         <v>1057</v>
       </c>
@@ -6568,7 +6552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:32" ht="15.75">
+    <row r="14" spans="2:33" ht="15.75">
       <c r="B14" s="1" t="s">
         <v>1058</v>
       </c>
@@ -6635,7 +6619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:32" ht="15.75">
+    <row r="15" spans="2:33" ht="15.75">
       <c r="B15" s="1" t="s">
         <v>1059</v>
       </c>
@@ -6702,7 +6686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:32" ht="16.5" thickBot="1">
+    <row r="16" spans="2:33" ht="16.5" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>1044</v>
       </c>
@@ -6811,11 +6795,11 @@
         <v>381</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="229" t="s">
+      <c r="R17" s="226" t="s">
         <v>696</v>
       </c>
-      <c r="S17" s="230"/>
-      <c r="T17" s="231"/>
+      <c r="S17" s="227"/>
+      <c r="T17" s="228"/>
       <c r="V17" s="46" t="s">
         <v>881</v>
       </c>
@@ -6933,25 +6917,25 @@
         <v>314</v>
       </c>
       <c r="Q19" s="4"/>
-      <c r="R19" s="226" t="s">
+      <c r="R19" s="223" t="s">
         <v>687</v>
       </c>
-      <c r="S19" s="227"/>
-      <c r="T19" s="228"/>
-      <c r="V19" s="232" t="s">
+      <c r="S19" s="224"/>
+      <c r="T19" s="225"/>
+      <c r="V19" s="229" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="233"/>
-      <c r="X19" s="233"/>
-      <c r="Y19" s="233"/>
-      <c r="Z19" s="234"/>
-      <c r="AB19" s="217" t="s">
+      <c r="W19" s="230"/>
+      <c r="X19" s="230"/>
+      <c r="Y19" s="230"/>
+      <c r="Z19" s="231"/>
+      <c r="AB19" s="222" t="s">
         <v>13</v>
       </c>
-      <c r="AC19" s="217"/>
-      <c r="AD19" s="217"/>
-      <c r="AE19" s="217"/>
-      <c r="AF19" s="217"/>
+      <c r="AC19" s="222"/>
+      <c r="AD19" s="222"/>
+      <c r="AE19" s="222"/>
+      <c r="AF19" s="222"/>
     </row>
     <row r="20" spans="2:32" ht="15.75">
       <c r="B20" s="1" t="s">
@@ -7669,11 +7653,11 @@
       <c r="Z30" t="s">
         <v>843</v>
       </c>
-      <c r="AC30" s="217" t="s">
+      <c r="AC30" s="222" t="s">
         <v>574</v>
       </c>
-      <c r="AD30" s="217"/>
-      <c r="AE30" s="217"/>
+      <c r="AD30" s="222"/>
+      <c r="AE30" s="222"/>
     </row>
     <row r="31" spans="2:32">
       <c r="B31" s="133" t="s">
@@ -7831,9 +7815,9 @@
       </c>
     </row>
     <row r="34" spans="2:33">
-      <c r="R34" s="222"/>
-      <c r="S34" s="222"/>
-      <c r="T34" s="222"/>
+      <c r="R34" s="238"/>
+      <c r="S34" s="238"/>
+      <c r="T34" s="238"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="53" t="s">
         <v>116</v>
@@ -7860,15 +7844,15 @@
       <c r="R36" s="78"/>
       <c r="S36" s="78"/>
       <c r="T36" s="80"/>
-      <c r="U36" s="236" t="s">
+      <c r="U36" s="233" t="s">
         <v>667</v>
       </c>
-      <c r="V36" s="236"/>
-      <c r="W36" s="236"/>
-      <c r="X36" s="236"/>
-      <c r="Y36" s="236"/>
-      <c r="Z36" s="236"/>
-      <c r="AA36" s="236"/>
+      <c r="V36" s="233"/>
+      <c r="W36" s="233"/>
+      <c r="X36" s="233"/>
+      <c r="Y36" s="233"/>
+      <c r="Z36" s="233"/>
+      <c r="AA36" s="233"/>
       <c r="AC36" s="8" t="s">
         <v>586</v>
       </c>
@@ -8003,13 +7987,13 @@
       <c r="AA41" t="s">
         <v>413</v>
       </c>
-      <c r="AC41" s="235" t="s">
+      <c r="AC41" s="232" t="s">
         <v>763</v>
       </c>
-      <c r="AD41" s="235"/>
-      <c r="AE41" s="235"/>
-      <c r="AF41" s="235"/>
-      <c r="AG41" s="235"/>
+      <c r="AD41" s="232"/>
+      <c r="AE41" s="232"/>
+      <c r="AF41" s="232"/>
+      <c r="AG41" s="232"/>
     </row>
     <row r="42" spans="2:33">
       <c r="W42" t="s">
@@ -8097,11 +8081,11 @@
       </c>
     </row>
     <row r="45" spans="2:33" ht="15.75" thickBot="1">
-      <c r="Q45" s="229" t="s">
+      <c r="Q45" s="226" t="s">
         <v>639</v>
       </c>
-      <c r="R45" s="230"/>
-      <c r="S45" s="231"/>
+      <c r="R45" s="227"/>
+      <c r="S45" s="228"/>
       <c r="W45" t="s">
         <v>715</v>
       </c>
@@ -8126,7 +8110,7 @@
       </c>
     </row>
     <row r="46" spans="2:33">
-      <c r="Q46" s="223" t="s">
+      <c r="Q46" s="239" t="s">
         <v>686</v>
       </c>
       <c r="R46" s="82" t="s">
@@ -8158,7 +8142,7 @@
       </c>
     </row>
     <row r="47" spans="2:33">
-      <c r="Q47" s="224"/>
+      <c r="Q47" s="240"/>
       <c r="R47" s="8" t="s">
         <v>1073</v>
       </c>
@@ -8167,25 +8151,25 @@
       </c>
     </row>
     <row r="48" spans="2:33" ht="15.75" thickBot="1">
-      <c r="B48" s="217" t="s">
+      <c r="B48" s="222" t="s">
         <v>312</v>
       </c>
-      <c r="C48" s="217"/>
-      <c r="D48" s="217"/>
-      <c r="E48" s="217"/>
-      <c r="F48" s="217"/>
-      <c r="G48" s="217"/>
-      <c r="H48" s="217"/>
-      <c r="J48" s="217" t="s">
+      <c r="C48" s="222"/>
+      <c r="D48" s="222"/>
+      <c r="E48" s="222"/>
+      <c r="F48" s="222"/>
+      <c r="G48" s="222"/>
+      <c r="H48" s="222"/>
+      <c r="J48" s="222" t="s">
         <v>313</v>
       </c>
-      <c r="K48" s="217"/>
-      <c r="L48" s="217"/>
-      <c r="M48" s="217"/>
-      <c r="N48" s="217"/>
-      <c r="O48" s="217"/>
-      <c r="P48" s="217"/>
-      <c r="Q48" s="225"/>
+      <c r="K48" s="222"/>
+      <c r="L48" s="222"/>
+      <c r="M48" s="222"/>
+      <c r="N48" s="222"/>
+      <c r="O48" s="222"/>
+      <c r="P48" s="222"/>
+      <c r="Q48" s="241"/>
       <c r="R48" s="72" t="s">
         <v>1074</v>
       </c>
@@ -8236,7 +8220,7 @@
       <c r="P49" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="Q49" s="223" t="s">
+      <c r="Q49" s="239" t="s">
         <v>687</v>
       </c>
       <c r="R49" s="82" t="s">
@@ -8287,7 +8271,7 @@
       <c r="P50" t="s">
         <v>402</v>
       </c>
-      <c r="Q50" s="224"/>
+      <c r="Q50" s="240"/>
       <c r="R50" s="8" t="s">
         <v>652</v>
       </c>
@@ -8344,7 +8328,7 @@
       <c r="P51" t="s">
         <v>403</v>
       </c>
-      <c r="Q51" s="225"/>
+      <c r="Q51" s="241"/>
       <c r="R51" s="72" t="s">
         <v>653</v>
       </c>
@@ -8366,15 +8350,15 @@
       <c r="Y51" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="AC51" s="217" t="s">
+      <c r="AC51" s="222" t="s">
         <v>615</v>
       </c>
-      <c r="AD51" s="217"/>
-      <c r="AE51" s="217"/>
-      <c r="AF51" s="217"/>
-      <c r="AG51" s="217"/>
-      <c r="AH51" s="217"/>
-      <c r="AI51" s="217"/>
+      <c r="AD51" s="222"/>
+      <c r="AE51" s="222"/>
+      <c r="AF51" s="222"/>
+      <c r="AG51" s="222"/>
+      <c r="AH51" s="222"/>
+      <c r="AI51" s="222"/>
     </row>
     <row r="52" spans="2:35">
       <c r="B52" t="s">
@@ -8674,15 +8658,15 @@
       <c r="H56" t="s">
         <v>389</v>
       </c>
-      <c r="J56" s="218" t="s">
+      <c r="J56" s="234" t="s">
         <v>400</v>
       </c>
-      <c r="K56" s="218"/>
-      <c r="L56" s="218"/>
-      <c r="M56" s="218"/>
-      <c r="N56" s="218"/>
-      <c r="O56" s="218"/>
-      <c r="P56" s="218"/>
+      <c r="K56" s="234"/>
+      <c r="L56" s="234"/>
+      <c r="M56" s="234"/>
+      <c r="N56" s="234"/>
+      <c r="O56" s="234"/>
+      <c r="P56" s="234"/>
       <c r="R56" s="87"/>
       <c r="S56" s="87"/>
       <c r="T56" s="87"/>
@@ -8953,15 +8937,15 @@
       <c r="Y64" s="8" t="s">
         <v>846</v>
       </c>
-      <c r="AC64" s="217" t="s">
+      <c r="AC64" s="222" t="s">
         <v>665</v>
       </c>
-      <c r="AD64" s="217"/>
-      <c r="AE64" s="217"/>
-      <c r="AF64" s="217"/>
-      <c r="AG64" s="217"/>
-      <c r="AH64" s="217"/>
-      <c r="AI64" s="217"/>
+      <c r="AD64" s="222"/>
+      <c r="AE64" s="222"/>
+      <c r="AF64" s="222"/>
+      <c r="AG64" s="222"/>
+      <c r="AH64" s="222"/>
+      <c r="AI64" s="222"/>
     </row>
     <row r="65" spans="21:35">
       <c r="U65" s="209">
@@ -9203,6 +9187,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="J48:P48"/>
+    <mergeCell ref="J56:P56"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="Q46:Q48"/>
+    <mergeCell ref="Q49:Q51"/>
     <mergeCell ref="AB19:AF19"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="R19:T19"/>
@@ -9217,13 +9208,6 @@
     <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="U36:AA36"/>
     <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="J48:P48"/>
-    <mergeCell ref="J56:P56"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="Q46:Q48"/>
-    <mergeCell ref="Q49:Q51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9231,14 +9215,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
@@ -9249,42 +9233,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="254" t="s">
         <v>1078</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="256"/>
       <c r="I1" s="48"/>
       <c r="R1" s="48"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="252"/>
-      <c r="B2" s="253"/>
-      <c r="C2" s="253"/>
-      <c r="D2" s="253"/>
-      <c r="E2" s="253"/>
-      <c r="F2" s="253"/>
-      <c r="G2" s="253"/>
-      <c r="H2" s="254"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="258"/>
+      <c r="C2" s="258"/>
+      <c r="D2" s="258"/>
+      <c r="E2" s="258"/>
+      <c r="F2" s="258"/>
+      <c r="G2" s="258"/>
+      <c r="H2" s="259"/>
     </row>
     <row r="3" spans="1:18" ht="18.75">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="260" t="s">
         <v>625</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="257"/>
-      <c r="D3" s="258"/>
-      <c r="E3" s="255" t="s">
+      <c r="B3" s="261"/>
+      <c r="C3" s="262"/>
+      <c r="D3" s="263"/>
+      <c r="E3" s="260" t="s">
         <v>626</v>
       </c>
-      <c r="F3" s="256"/>
-      <c r="G3" s="257"/>
-      <c r="H3" s="258"/>
+      <c r="F3" s="261"/>
+      <c r="G3" s="262"/>
+      <c r="H3" s="263"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="95">
@@ -9854,14 +9838,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" customWidth="1"/>
@@ -9872,40 +9856,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="254" t="s">
         <v>1081</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="256"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="252"/>
-      <c r="B2" s="253"/>
-      <c r="C2" s="253"/>
-      <c r="D2" s="253"/>
-      <c r="E2" s="253"/>
-      <c r="F2" s="253"/>
-      <c r="G2" s="253"/>
-      <c r="H2" s="254"/>
+      <c r="A2" s="257"/>
+      <c r="B2" s="258"/>
+      <c r="C2" s="258"/>
+      <c r="D2" s="258"/>
+      <c r="E2" s="258"/>
+      <c r="F2" s="258"/>
+      <c r="G2" s="258"/>
+      <c r="H2" s="259"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="260" t="s">
         <v>1093</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="257"/>
-      <c r="D3" s="258"/>
-      <c r="E3" s="255" t="s">
+      <c r="B3" s="261"/>
+      <c r="C3" s="262"/>
+      <c r="D3" s="263"/>
+      <c r="E3" s="260" t="s">
         <v>1094</v>
       </c>
-      <c r="F3" s="256"/>
-      <c r="G3" s="257"/>
-      <c r="H3" s="258"/>
+      <c r="F3" s="261"/>
+      <c r="G3" s="262"/>
+      <c r="H3" s="263"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="95">
@@ -10569,14 +10553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -10589,40 +10573,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="259" t="s">
+      <c r="A1" s="264" t="s">
         <v>765</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="260"/>
-      <c r="B2" s="260"/>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
+      <c r="A2" s="265"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
+      <c r="D2" s="265"/>
+      <c r="E2" s="265"/>
+      <c r="F2" s="265"/>
+      <c r="G2" s="265"/>
+      <c r="H2" s="265"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="255" t="s">
+      <c r="A3" s="260" t="s">
         <v>625</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="257"/>
-      <c r="D3" s="258"/>
-      <c r="E3" s="255" t="s">
+      <c r="B3" s="261"/>
+      <c r="C3" s="262"/>
+      <c r="D3" s="263"/>
+      <c r="E3" s="260" t="s">
         <v>626</v>
       </c>
-      <c r="F3" s="256"/>
-      <c r="G3" s="257"/>
-      <c r="H3" s="258"/>
+      <c r="F3" s="261"/>
+      <c r="G3" s="262"/>
+      <c r="H3" s="263"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="93">
@@ -11140,14 +11124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
@@ -11157,33 +11141,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="288" t="s">
         <v>1099</v>
       </c>
-      <c r="B1" s="267"/>
-      <c r="C1" s="267"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="267"/>
-      <c r="F1" s="268"/>
+      <c r="B1" s="289"/>
+      <c r="C1" s="289"/>
+      <c r="D1" s="289"/>
+      <c r="E1" s="289"/>
+      <c r="F1" s="290"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="261" t="s">
+      <c r="A2" s="269" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="262"/>
-      <c r="C2" s="262"/>
-      <c r="D2" s="263" t="s">
+      <c r="B2" s="270"/>
+      <c r="C2" s="270"/>
+      <c r="D2" s="285" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="264"/>
-      <c r="F2" s="265"/>
+      <c r="E2" s="286"/>
+      <c r="F2" s="287"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="276" t="s">
+      <c r="A3" s="272" t="s">
         <v>890</v>
       </c>
-      <c r="B3" s="277"/>
-      <c r="C3" s="278"/>
+      <c r="B3" s="273"/>
+      <c r="C3" s="274"/>
       <c r="D3" s="202" t="s">
         <v>2</v>
       </c>
@@ -11474,11 +11458,11 @@
       <c r="C18" s="101" t="s">
         <v>303</v>
       </c>
-      <c r="D18" s="261" t="s">
+      <c r="D18" s="269" t="s">
         <v>1095</v>
       </c>
-      <c r="E18" s="262"/>
-      <c r="F18" s="269"/>
+      <c r="E18" s="270"/>
+      <c r="F18" s="271"/>
     </row>
     <row r="19" spans="1:17" ht="15.75">
       <c r="A19" s="187">
@@ -11490,7 +11474,7 @@
       <c r="C19" s="189" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="270" t="s">
+      <c r="D19" s="282" t="s">
         <v>686</v>
       </c>
       <c r="E19" s="179" t="s">
@@ -11510,7 +11494,7 @@
       <c r="C20" s="189" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="271"/>
+      <c r="D20" s="283"/>
       <c r="E20" s="162" t="s">
         <v>1097</v>
       </c>
@@ -11530,7 +11514,7 @@
       <c r="C21" s="189" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="272"/>
+      <c r="D21" s="284"/>
       <c r="E21" s="182" t="s">
         <v>1098</v>
       </c>
@@ -11760,13 +11744,13 @@
       <c r="F35" s="123"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A36" s="273" t="s">
+      <c r="A36" s="266" t="s">
         <v>883</v>
       </c>
-      <c r="B36" s="274"/>
-      <c r="C36" s="274"/>
-      <c r="D36" s="274"/>
-      <c r="E36" s="275"/>
+      <c r="B36" s="267"/>
+      <c r="C36" s="267"/>
+      <c r="D36" s="267"/>
+      <c r="E36" s="268"/>
       <c r="F36" s="124"/>
     </row>
     <row r="37" spans="1:6">
@@ -11958,24 +11942,24 @@
       <c r="F47" s="128"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A48" s="279" t="s">
+      <c r="A48" s="275" t="s">
         <v>898</v>
       </c>
-      <c r="B48" s="280"/>
-      <c r="C48" s="280"/>
-      <c r="D48" s="281"/>
-      <c r="E48" s="281"/>
-      <c r="F48" s="282"/>
+      <c r="B48" s="276"/>
+      <c r="C48" s="276"/>
+      <c r="D48" s="277"/>
+      <c r="E48" s="277"/>
+      <c r="F48" s="278"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="125"/>
       <c r="B49" s="122"/>
       <c r="C49" s="122"/>
-      <c r="D49" s="283" t="s">
+      <c r="D49" s="279" t="s">
         <v>885</v>
       </c>
-      <c r="E49" s="284"/>
-      <c r="F49" s="285"/>
+      <c r="E49" s="280"/>
+      <c r="F49" s="281"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="125"/>
@@ -12007,11 +11991,11 @@
       <c r="A52" s="125"/>
       <c r="B52" s="122"/>
       <c r="C52" s="122"/>
-      <c r="D52" s="261" t="s">
+      <c r="D52" s="269" t="s">
         <v>848</v>
       </c>
-      <c r="E52" s="262"/>
-      <c r="F52" s="269"/>
+      <c r="E52" s="270"/>
+      <c r="F52" s="271"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="125"/>
@@ -12087,17 +12071,17 @@
       <c r="A58" s="125"/>
       <c r="B58" s="122"/>
       <c r="C58" s="122"/>
-      <c r="D58" s="261" t="s">
+      <c r="D58" s="269" t="s">
         <v>889</v>
       </c>
-      <c r="E58" s="262"/>
-      <c r="F58" s="269"/>
+      <c r="E58" s="270"/>
+      <c r="F58" s="271"/>
     </row>
     <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="125"/>
       <c r="B59" s="122"/>
       <c r="C59" s="122"/>
-      <c r="D59" s="270" t="s">
+      <c r="D59" s="282" t="s">
         <v>687</v>
       </c>
       <c r="E59" s="179" t="s">
@@ -12111,7 +12095,7 @@
       <c r="A60" s="125"/>
       <c r="B60" s="122"/>
       <c r="C60" s="122"/>
-      <c r="D60" s="271"/>
+      <c r="D60" s="283"/>
       <c r="E60" s="162" t="s">
         <v>652</v>
       </c>
@@ -12123,7 +12107,7 @@
       <c r="A61" s="125"/>
       <c r="B61" s="122"/>
       <c r="C61" s="122"/>
-      <c r="D61" s="272"/>
+      <c r="D61" s="284"/>
       <c r="E61" s="182" t="s">
         <v>653</v>
       </c>
@@ -12146,13 +12130,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A63" s="273" t="s">
+      <c r="A63" s="266" t="s">
         <v>884</v>
       </c>
-      <c r="B63" s="274"/>
-      <c r="C63" s="274"/>
-      <c r="D63" s="274"/>
-      <c r="E63" s="275"/>
+      <c r="B63" s="267"/>
+      <c r="C63" s="267"/>
+      <c r="D63" s="267"/>
+      <c r="E63" s="268"/>
       <c r="F63" s="123"/>
     </row>
     <row r="64" spans="1:6" ht="15.75">
@@ -12456,6 +12440,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="A3:C3"/>
@@ -12464,11 +12453,6 @@
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="D59:D61"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12476,14 +12460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="15" max="15" width="16" customWidth="1"/>
   </cols>
@@ -13486,14 +13470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:11">
       <c r="B2" s="48" t="s">
@@ -13711,14 +13695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="3:15">
       <c r="C4" s="145"/>
@@ -14872,14 +14856,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -14890,28 +14874,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="245" t="s">
         <v>900</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
     </row>
     <row r="2" spans="1:19" ht="15.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="242" t="s">
         <v>1112</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="239"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
+      <c r="E2" s="243"/>
+      <c r="F2" s="243"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="244"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="21"/>
@@ -14958,14 +14942,14 @@
       <c r="H4" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="L4" s="286"/>
-      <c r="M4" s="286"/>
-      <c r="N4" s="286"/>
-      <c r="O4" s="286"/>
-      <c r="P4" s="286"/>
-      <c r="Q4" s="286"/>
-      <c r="R4" s="286"/>
-      <c r="S4" s="286"/>
+      <c r="L4" s="217"/>
+      <c r="M4" s="217"/>
+      <c r="N4" s="217"/>
+      <c r="O4" s="217"/>
+      <c r="P4" s="217"/>
+      <c r="Q4" s="217"/>
+      <c r="R4" s="217"/>
+      <c r="S4" s="217"/>
     </row>
     <row r="5" spans="1:19" ht="15.75">
       <c r="A5" s="22">
@@ -14990,14 +14974,14 @@
       <c r="H5" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="L5" s="287"/>
-      <c r="M5" s="288"/>
-      <c r="N5" s="289"/>
-      <c r="O5" s="290"/>
-      <c r="P5" s="287"/>
-      <c r="Q5" s="288"/>
-      <c r="R5" s="289"/>
-      <c r="S5" s="290"/>
+      <c r="L5" s="218"/>
+      <c r="M5" s="219"/>
+      <c r="N5" s="220"/>
+      <c r="O5" s="221"/>
+      <c r="P5" s="218"/>
+      <c r="Q5" s="219"/>
+      <c r="R5" s="220"/>
+      <c r="S5" s="221"/>
     </row>
     <row r="6" spans="1:19" ht="15.75">
       <c r="A6" s="22">
@@ -15022,14 +15006,14 @@
       <c r="H6" s="24" t="s">
         <v>649</v>
       </c>
-      <c r="L6" s="287"/>
-      <c r="M6" s="288"/>
-      <c r="N6" s="289"/>
-      <c r="O6" s="290"/>
-      <c r="P6" s="287"/>
-      <c r="Q6" s="288"/>
-      <c r="R6" s="289"/>
-      <c r="S6" s="290"/>
+      <c r="L6" s="218"/>
+      <c r="M6" s="219"/>
+      <c r="N6" s="220"/>
+      <c r="O6" s="221"/>
+      <c r="P6" s="218"/>
+      <c r="Q6" s="219"/>
+      <c r="R6" s="220"/>
+      <c r="S6" s="221"/>
     </row>
     <row r="7" spans="1:19" ht="15.75">
       <c r="A7" s="22">
@@ -15054,14 +15038,14 @@
       <c r="H7" s="24" t="s">
         <v>927</v>
       </c>
-      <c r="L7" s="287"/>
-      <c r="M7" s="288"/>
-      <c r="N7" s="289"/>
-      <c r="O7" s="290"/>
-      <c r="P7" s="287"/>
-      <c r="Q7" s="288"/>
-      <c r="R7" s="289"/>
-      <c r="S7" s="290"/>
+      <c r="L7" s="218"/>
+      <c r="M7" s="219"/>
+      <c r="N7" s="220"/>
+      <c r="O7" s="221"/>
+      <c r="P7" s="218"/>
+      <c r="Q7" s="219"/>
+      <c r="R7" s="220"/>
+      <c r="S7" s="221"/>
     </row>
     <row r="8" spans="1:19" ht="15.75">
       <c r="A8" s="22">
@@ -15088,14 +15072,14 @@
       <c r="H8" s="24" t="s">
         <v>901</v>
       </c>
-      <c r="L8" s="287"/>
-      <c r="M8" s="288"/>
-      <c r="N8" s="289"/>
-      <c r="O8" s="290"/>
-      <c r="P8" s="287"/>
-      <c r="Q8" s="288"/>
-      <c r="R8" s="289"/>
-      <c r="S8" s="290"/>
+      <c r="L8" s="218"/>
+      <c r="M8" s="219"/>
+      <c r="N8" s="220"/>
+      <c r="O8" s="221"/>
+      <c r="P8" s="218"/>
+      <c r="Q8" s="219"/>
+      <c r="R8" s="220"/>
+      <c r="S8" s="221"/>
     </row>
     <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="22">
@@ -15120,14 +15104,14 @@
       <c r="H9" s="24" t="s">
         <v>928</v>
       </c>
-      <c r="L9" s="287"/>
-      <c r="M9" s="288"/>
-      <c r="N9" s="289"/>
-      <c r="O9" s="290"/>
-      <c r="P9" s="287"/>
-      <c r="Q9" s="288"/>
-      <c r="R9" s="289"/>
-      <c r="S9" s="290"/>
+      <c r="L9" s="218"/>
+      <c r="M9" s="219"/>
+      <c r="N9" s="220"/>
+      <c r="O9" s="221"/>
+      <c r="P9" s="218"/>
+      <c r="Q9" s="219"/>
+      <c r="R9" s="220"/>
+      <c r="S9" s="221"/>
     </row>
     <row r="10" spans="1:19" ht="15.75">
       <c r="A10" s="22">
@@ -15152,14 +15136,14 @@
       <c r="H10" s="24" t="s">
         <v>903</v>
       </c>
-      <c r="L10" s="287"/>
-      <c r="M10" s="288"/>
-      <c r="N10" s="289"/>
-      <c r="O10" s="290"/>
-      <c r="P10" s="287"/>
-      <c r="Q10" s="288"/>
-      <c r="R10" s="289"/>
-      <c r="S10" s="290"/>
+      <c r="L10" s="218"/>
+      <c r="M10" s="219"/>
+      <c r="N10" s="220"/>
+      <c r="O10" s="221"/>
+      <c r="P10" s="218"/>
+      <c r="Q10" s="219"/>
+      <c r="R10" s="220"/>
+      <c r="S10" s="221"/>
     </row>
     <row r="11" spans="1:19" ht="15.75">
       <c r="A11" s="22">
@@ -15184,14 +15168,14 @@
       <c r="H11" s="24" t="s">
         <v>476</v>
       </c>
-      <c r="L11" s="287"/>
-      <c r="M11" s="288"/>
-      <c r="N11" s="289"/>
-      <c r="O11" s="290"/>
-      <c r="P11" s="287"/>
-      <c r="Q11" s="288"/>
-      <c r="R11" s="289"/>
-      <c r="S11" s="290"/>
+      <c r="L11" s="218"/>
+      <c r="M11" s="219"/>
+      <c r="N11" s="220"/>
+      <c r="O11" s="221"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="219"/>
+      <c r="R11" s="220"/>
+      <c r="S11" s="221"/>
     </row>
     <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="22">
@@ -15216,14 +15200,14 @@
       <c r="H12" s="24" t="s">
         <v>846</v>
       </c>
-      <c r="L12" s="287"/>
-      <c r="M12" s="288"/>
-      <c r="N12" s="289"/>
-      <c r="O12" s="290"/>
-      <c r="P12" s="287"/>
-      <c r="Q12" s="288"/>
-      <c r="R12" s="289"/>
-      <c r="S12" s="290"/>
+      <c r="L12" s="218"/>
+      <c r="M12" s="219"/>
+      <c r="N12" s="220"/>
+      <c r="O12" s="221"/>
+      <c r="P12" s="218"/>
+      <c r="Q12" s="219"/>
+      <c r="R12" s="220"/>
+      <c r="S12" s="221"/>
     </row>
     <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="22">
@@ -15250,14 +15234,14 @@
       <c r="H13" s="24" t="s">
         <v>1042</v>
       </c>
-      <c r="L13" s="287"/>
-      <c r="M13" s="288"/>
-      <c r="N13" s="289"/>
-      <c r="O13" s="290"/>
-      <c r="P13" s="287"/>
-      <c r="Q13" s="288"/>
-      <c r="R13" s="289"/>
-      <c r="S13" s="290"/>
+      <c r="L13" s="218"/>
+      <c r="M13" s="219"/>
+      <c r="N13" s="220"/>
+      <c r="O13" s="221"/>
+      <c r="P13" s="218"/>
+      <c r="Q13" s="219"/>
+      <c r="R13" s="220"/>
+      <c r="S13" s="221"/>
     </row>
     <row r="14" spans="1:19" ht="15.75">
       <c r="A14" s="22">
@@ -15284,14 +15268,14 @@
       <c r="H14" s="24" t="s">
         <v>903</v>
       </c>
-      <c r="L14" s="287"/>
-      <c r="M14" s="288"/>
-      <c r="N14" s="289"/>
-      <c r="O14" s="290"/>
-      <c r="P14" s="287"/>
-      <c r="Q14" s="288"/>
-      <c r="R14" s="289"/>
-      <c r="S14" s="290"/>
+      <c r="L14" s="218"/>
+      <c r="M14" s="219"/>
+      <c r="N14" s="220"/>
+      <c r="O14" s="221"/>
+      <c r="P14" s="218"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="220"/>
+      <c r="S14" s="221"/>
     </row>
     <row r="15" spans="1:19" ht="15.75">
       <c r="A15" s="22">
@@ -15334,16 +15318,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75">
-      <c r="A18" s="237" t="s">
+      <c r="A18" s="242" t="s">
         <v>320</v>
       </c>
-      <c r="B18" s="238"/>
-      <c r="C18" s="238"/>
-      <c r="D18" s="238"/>
-      <c r="E18" s="238"/>
-      <c r="F18" s="238"/>
-      <c r="G18" s="238"/>
-      <c r="H18" s="239"/>
+      <c r="B18" s="243"/>
+      <c r="C18" s="243"/>
+      <c r="D18" s="243"/>
+      <c r="E18" s="243"/>
+      <c r="F18" s="243"/>
+      <c r="G18" s="243"/>
+      <c r="H18" s="244"/>
     </row>
     <row r="19" spans="1:8" ht="15.75">
       <c r="A19" s="26"/>
@@ -15634,16 +15618,16 @@
       <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" ht="15.75">
-      <c r="A31" s="237" t="s">
+      <c r="A31" s="242" t="s">
         <v>321</v>
       </c>
-      <c r="B31" s="238"/>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="239"/>
+      <c r="B31" s="243"/>
+      <c r="C31" s="243"/>
+      <c r="D31" s="243"/>
+      <c r="E31" s="243"/>
+      <c r="F31" s="243"/>
+      <c r="G31" s="243"/>
+      <c r="H31" s="244"/>
     </row>
     <row r="32" spans="1:8" ht="15.75">
       <c r="A32" s="21"/>
@@ -15901,14 +15885,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -15917,12 +15901,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="245" t="s">
         <v>820</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="36"/>
@@ -16111,14 +16095,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
@@ -16129,28 +16113,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="246" t="s">
         <v>523</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
-      <c r="G1" s="241"/>
-      <c r="H1" s="241"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="242" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="239"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
+      <c r="E2" s="243"/>
+      <c r="F2" s="243"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="244"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="27" t="s">
@@ -16437,12 +16421,12 @@
       <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="242" t="s">
         <v>324</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="239"/>
+      <c r="B15" s="243"/>
+      <c r="C15" s="243"/>
+      <c r="D15" s="244"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -16621,12 +16605,12 @@
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="237" t="s">
+      <c r="A28" s="242" t="s">
         <v>325</v>
       </c>
-      <c r="B28" s="238"/>
-      <c r="C28" s="238"/>
-      <c r="D28" s="239"/>
+      <c r="B28" s="243"/>
+      <c r="C28" s="243"/>
+      <c r="D28" s="244"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -16808,14 +16792,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
@@ -16824,36 +16808,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="242" t="s">
+      <c r="A1" s="247" t="s">
         <v>563</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="243"/>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
+      <c r="A2" s="248"/>
+      <c r="B2" s="248"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="249" t="s">
         <v>594</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="244" t="s">
+      <c r="B3" s="250"/>
+      <c r="C3" s="251"/>
+      <c r="D3" s="249" t="s">
         <v>595</v>
       </c>
-      <c r="E3" s="245"/>
-      <c r="F3" s="246"/>
+      <c r="E3" s="250"/>
+      <c r="F3" s="251"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1">
       <c r="A4" s="44">
@@ -17382,14 +17366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -17398,22 +17382,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="248" t="s">
+      <c r="A1" s="253" t="s">
         <v>566</v>
       </c>
-      <c r="B1" s="248"/>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="248"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="253"/>
+      <c r="D1" s="253"/>
+      <c r="E1" s="253"/>
+      <c r="F1" s="253"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="247" t="s">
+      <c r="B2" s="252" t="s">
         <v>587</v>
       </c>
-      <c r="C2" s="247"/>
-      <c r="D2" s="247"/>
-      <c r="E2" s="247"/>
+      <c r="C2" s="252"/>
+      <c r="D2" s="252"/>
+      <c r="E2" s="252"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="36"/>
@@ -17518,12 +17502,12 @@
       <c r="E10" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="247" t="s">
+      <c r="B14" s="252" t="s">
         <v>582</v>
       </c>
-      <c r="C14" s="247"/>
-      <c r="D14" s="247"/>
-      <c r="E14" s="247"/>
+      <c r="C14" s="252"/>
+      <c r="D14" s="252"/>
+      <c r="E14" s="252"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="36"/>

</xml_diff>